<commit_message>
Refactor Dropbox integration and update KPI alert calculations
- Removed DROPBOX_ACCESS_TOKEN from the GitHub Actions workflow for security reasons.
- Updated 'calculated_KPIs_alerts.csv' to reflect new total TBS, vertical TBS, and pod TBS values with adjusted timestamps.
- Enhanced 'calculated_kpis.py' to properly handle Dropbox API authentication and access token retrieval.
- Updated binary files 'calculated_KPIs_alerts.xlsx' and 'calculated_KPIs_critical_alerts.xlsx' to reflect recent changes in calculations.
</commit_message>
<xml_diff>
--- a/scripts/calculated_KPIs_alerts.xlsx
+++ b/scripts/calculated_KPIs_alerts.xlsx
@@ -507,29 +507,29 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45656.95833333334</v>
+        <v>45657.875</v>
       </c>
       <c r="E2" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
-        <v>36.35456963855825</v>
+        <v>40.84987772406356</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45656.95833333334</v>
+        <v>45657.875</v>
       </c>
       <c r="H2" t="n">
-        <v>21.19708117770453</v>
+        <v>23.44153440709918</v>
       </c>
       <c r="I2" t="n">
-        <v>4.224039173475912</v>
+        <v>6.582104548438676</v>
       </c>
       <c r="J2" t="n">
-        <v>36.35456963855825</v>
+        <v>40.84987772406356</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACPJklEQVR4nOzdd3hUdfr38c+UNAhJICQSIEgJTRBQKYJURURUXKnqKkVc64ptVxdWl0UXsCDWx8LqD1BxFXDdFStlibICIhqawoJSJIQWAhMS0iZznj9CJhlmJpmQMmfg/bouLs09Z8657zl17nzPicUwDEMAAAAAAACASVmDnQAAAAAAAABQERpYAAAAAAAAMDUaWAAAAAAAADA1GlgAAAAAAAAwNRpYAAAAAAAAMDUaWAAAAAAAADA1GlgAAAAAAAAwNRpYAAAAAAAAMDUaWAAAAAAAADA1GlgAAAAAAAAwNRpYAAAAAAAAMDUaWAAAAAAAADA1GlgAAAAAAAAwNRpYAAAAAAAAMDUaWAAA1CGLxVLlfwMHDgx22m4tW7aUxWLRnj17gp1KtZR+tqhde/bskcViUcuWLYOdCgAACHH2YCcAAMC5ZPz48V6xgwcP6ssvv/T7eocOHaq0jNTUVA0aNEgDBgxQamrqGeUZygYOHKivvvpKq1atMlXzz5fSJpphGLW+rL/+9a+aPn26pk2bpr/+9a+1vjwAAICaRAMLAIA6NH/+fK9Yamqqu4Hl63XUvG3btgU7BQAAAFQBDSwAAHDOqeqoNgAAAAQXz8ACAMDk0tPTdd9996lt27aKjIxUbGysLrvsMr3xxhsqLi72mHbgwIEaNGiQJOmrr77yeJZW+ecQHTlyRC+99JKGDRumVq1aKSoqSjExMerevbuefvpp5efn11j+EyZMkMVi0fz587Vp0yaNGDFCCQkJioqKUpcuXfTiiy961SFJJ06c0N///neNGDFCbdu2Vf369VW/fn1deOGF+vOf/6zjx497TJ+amiqLxaKvvvpKkjRo0CCP+suPbqvoGVhOp1NvvvmmBg4cqEaNGikiIkKtWrXS3XffrX379nlNX7rcgQMHqqioSE8//bQ6deqkqKgoxcfHa8SIEV4jvv761796LP/0556Vf8bY4sWLNXjwYMXHxyssLEzx8fG64IIL9Lvf/U6bN2+u7ON3z3/69OmSpOnTp3ssa8KECR7TZmVlaerUqerUqZPq1aunBg0a6JJLLtEzzzyjvLy8gJbni9Pp1DPPPOP+bBo3bqwxY8Zo+/btft+Tl5en5557Tpdeeqni4uIUGRmp9u3b65FHHtHRo0ernMOKFSt03XXX6bzzzlNYWJgaNmyotm3b6pZbbtHXX3/t8z0rV67UiBEjlJSUpPDwcCUmJuqGG27Q2rVrayzv+fPnu9dFbm6upkyZopSUFEVERKhJkyYaP3689u/fX+V6AQA4mzACCwAAE/vuu+80dOhQZWVlqUWLFvrNb34jh8Oh1NRUrVmzRh999JE+/vhjhYeHS5KGDh2qyMhIffnllzrvvPM0dOhQ97waN27s/v8vv/xS999/v5o1a6aUlBRdeumlOnLkiL799lv96U9/0r///W+tWrVKERERNVbL+vXrdffdd6tJkya64oordOzYMaWmpuqBBx7Qf//7Xy1atMijqbNp0ybdcccdSkhIUPv27XXJJZfo2LFj+v777zVz5kwtWrRI69atU3x8vCS5v+h/8cUXOnTokK666io1adLEPb+UlJRKczxx4oSGDx+u1NRURUdH65JLLlFCQoK2bNmi119/XYsXL9by5ct10UUXeb23qKhIw4YN05o1a9S/f3917NhR69ev10cffaRVq1YpLS3N3UTs1q2bxo8frwULFkjyfvZZdHS0JOmJJ57QtGnTZLfb1adPHzVr1kwOh0O//vqr3nrrLXXq1EldunSptK7x48dr48aN2rRpk7p27apu3bq5X+vbt6/7/3ft2qXLL79ce/fuVUJCgoYNG6aioiKtWrVKjz76qD744AOtWLFCDRs2rHSZpxs7dqyWLl2qAQMGqEuXLlq/fr0WL16szz//XMuWLVPv3r09ps/IyNDQoUO1ZcsWNWrUSD169FCDBg30ww8/6Nlnn9XixYuVmpqq888/P6DlL1iwQBMnTpQk9ezZU4MGDVJeXp7S09P1/vvvq3Hjxurfv7/He/7whz/oueeek9VqVffu3dWvXz/9+uuv+ve//62lS5fq73//u3ueNZG3w+FQnz599Ouvv6pfv37q3Lmz1q5dq7fffltfffWVNm3apNjY2Kp87AAAnD0MAAAQVKtWrTIkGaeflvPz843zzz/fkGTcddddRmFhofu1X375xWjZsqUhyZg6darP+Q0YMMDvMn/66Sdj7dq1XvGsrCxjyJAhhiTjmWee8Xq9NJ/du3cHXN/48ePd9d1zzz1GUVGR+7WtW7caCQkJhiTj9ddf93jfvn37jBUrVhjFxcUe8dzcXGPcuHHu+Z1uwIABhiRj1apVfnPy9XkbhmHcfPPNhiTj2muvNQ4dOuTx2vPPP29IMtq2bWs4nU53vPz6u+iii4wDBw64X8vLyzOuuuoqQ5Jxxx13BJyHYZSs/6ioKCM6OtrYvn271+t79uwxtm3b5rfG002bNs2QZEybNs3vNL169TIkGcOHDzdycnLc8cOHDxsXX3yxIcm4+eabA17m7t273TU2btzY2LRpk/s1p9Np3HfffYYk4/zzzzfy8/Pdr7lcLuOyyy4zJBmTJk0ysrOz3a8VFRUZDz/8sCHJGDRoUMC5tGrVypBkrF692uu1Q4cOGT/88INHbO7cuYYkIyUlxSNvwzCMr776ymjQoIERHh5u7Nixo9p5z5s3z/05XXXVVYbD4XC/lpWVZXTr1s2QZMycOTPgegEAONvQwAIAIMj8NbDeeecdQ5LRtGlTjy/3pZYsWWJIMho0aGDk5eV5za+iBlZF/ve//xmSjB49eni9Vp0GVlJSkkeepV5++WV3YyhQubm5ht1uNxISErxeO9MG1k8//WRYLBajadOmHo2H8oYNG2ZIMpYuXeqOlX7eFovF2Lhxo9d71q1bZ0gyWrduHVAepQ4fPmxIMrp06eK3jqqorIG1evVqQ5JRr1494+DBg16vb9iwwZBkWK1WY9++fQEts3wD64UXXvB6PT8/32jWrJkhyVi4cKE7/vnnnxuSjG7dunk0PEsVFxcbnTt3NiQZW7ZsCSiXevXqGbGxsQFNW1xcbDRt2tSQZGzYsMHnNM8884whyXj44YernXdpA6t+/fpGRkaG1/vef/99Q5Jx+eWXB5Q/AABnI56BBQCASaWmpkqSbrzxRp+38o0YMUINGzbUiRMn9P3331d5/sXFxVq5cqWefPJJ3XPPPZo4caImTJigGTNmSJL+97//VSv/040ZM0aRkZFe8dLb53bu3KmMjAyv19esWaOnn35a9957rzvHe+65R+Hh4Tpy5IiOHTtWI/l99tlnMgxDV199tRo0aOBzmoEDB7pzOl2LFi3UtWtXr3jHjh0lqcrPMEpISFDLli21efNmPfzww/rpp5+q9P6qKt3ehg4dqvPOO8/r9UsuuURdu3aVy+VyP2esKk6/TVKSIiIiNHbsWI/lS9Knn34qSRo5cqTsdu8nXlitVvftfr7WhS89e/aUw+HQuHHj9P3338vlcvmdNi0tTRkZGWrTpo0uueQSn9P42haqm3f37t2VlJTkFT/TbQgAgLMJz8ACAMCkSr+stmrVyufrFotFrVq10rFjx6r8xXbnzp264YYb9OOPP/qdJjs7u0rzrIy/Oho0aKD4+HgdPXpU6enpatq0qSTp8OHDGjlypP773/9WON/s7OwzeibT6Xbt2iVJeuutt/TWW29VOO2RI0e8Yi1atPA5bUxMjCSpoKCgyjm9/fbbGjVqlObMmaM5c+aoUaNG6tWrl6688krdeuutHs81q67KtjdJatOmjTZt2lTl7S0uLk5xcXE+XytdXnp6ujtWui4ef/xxPf744xXO29e68OXVV1/Vtddeq3feeUfvvPOOGjRooB49eujyyy/Xrbfe6rH+Spf/yy+/+H3Yv6/lVzfvyrahmvzjCgAAhBoaWAAAnINGjRqlH3/8Uddee60eeeQRXXDBBYqJiVFYWJgKCwtr9OHtVWEYhvv/b7/9dv33v/9V7969NX36dHXt2lUNGzZUWFiYJKlp06Y6cOCAx3uqo3RETrdu3XyOpCqvV69eXjGrteYHtvfr10979uzRp59+qq+++kpr1qzRl19+qc8//1zTpk3TRx99pCuuuKLGlxsM5ddj6bro27ev2rRpU+H7OnXqFND8O3bsqP/9739atmyZ/vOf/2jNmjVavXq1/vOf/+iJJ57QW2+9pVtuucVj+U2aNNFVV11V4XzLNxGrm3dtbEMAAJwtaGABAGBSzZo1k1Q2qsOX3bt3e0wbiO3bt2vz5s1KTEzURx995HWr086dO88g28qV5nq6EydO6OjRo5Kk5s2bS5Jyc3P12WefyWq16rPPPvMavZObm6uDBw/WaH7JycmSpMsuu0yvvPJKjc67OqKiojRq1CiNGjVKUsnInccee0xz587Vbbfdpr1799bIcgLZ3kpfq8r2JknHjx/X8ePHfY7C2rNnj6SydS+VrYvrr79ef/jDH6q0rIrY7XYNGzZMw4YNk1Qyem/OnDmaPn267rzzTt1www2qX7++e/nx8fGaP39+wPOvrbwBAIDEr3kAADCp0mfsfPDBBz5vHfroo4907NgxNWjQwOM5PeHh4ZIkp9Ppc75ZWVmSSkYw+XpOz7vvvlvd1H1avHixz9vo3nnnHUlSSkqKuzHicDhUXFysmJgYn02Pd9991+/Iq8rq9+fqq6+WJH388cd1dqtW6WiyquSakJCgZ555RpL066+/BvwMsMo+l9Lt7YsvvtChQ4e8Xk9LS9PGjRs9nuNUFaXrubzCwkJ98MEHHsuXytbF4sWLa2yEnS8xMTH661//qri4OJ08eVI7duyQJPXo0UONGzfWTz/9VOFttqerq7wBADgX0cACAMCkRo8erRYtWigjI0MPPfSQR+Nh9+7devjhhyVJ9913n8fD0UtHsuzcuVNFRUVe823Xrp1sNpu2bNni8eBsSVq6dKmef/75WqhGysjI0B/+8AcVFxe7Y9u2bdMTTzwhSXrwwQfd8fPOO08NGzbU8ePHvRof69at05QpU/wup7T+qjQeJOmiiy7SyJEjtW/fPo0YMcI9Mqi83NxcLVy40GeD50xUlOvevXv15ptv+nwW2dKlSyVJDRs2dD8fqTrLkkpue+vVq5fy8vJ055136uTJk+7XMjMzdeedd0oq+aMCpSONquLJJ5/U1q1b3T+7XC49+uijSk9PV3JyskaOHOl+7frrr1ePHj20fv16TZw40efzoo4dO6bXX389oObfyZMnNWfOHJ/zWb16tY4fPy6bzeb+jMLCwjRt2jQZhqEbbrjB53PYiouL9Z///Efr1q2rtbwBAEA5wfsDiAAAwDAMY9WqVYYkw9dpef369UajRo0MScb5559vjB071hg2bJgRGRlpSDKuuuoqo6CgwOt93bt3NyQZ7du3N377298akyZNMh599FH36/fff78hybBarcaAAQOMm266ybj44osNScZjjz3mN5/zzz/fkGTs3r074PrGjx9vSDLuuusuIzIy0mjVqpVx4403GldddZURHh5uSDJuuOEGw+Vyebzv+eefd+fRq1cv46abbjIuu+wyw2KxGLfeeqvfXD755BNDkhEeHm5ce+21xm233WZMmjTJ+Oabb9zT+KsvOzvbuOKKK9zv79GjhzFmzBhj9OjRRo8ePdz5btu2zf2e0vU3YMAAv5+Bv+X94Q9/MCQZjRs3NsaMGWNMmjTJmDRpkpGZmWmkpaUZkoywsDB3HmPGjDEuuugiQ5JhsViMN998M8C1YBgHDx406tevb0gyLrvsMmPChAnGpEmTjP/7v/9zT/PLL7+4P9fExERj1KhRxvXXX2/ExMQYkoyLL77YyMrKCniZu3fvNiQZLVq0MG644QYjLCzMuPLKK40bb7zRaNOmjSHJqF+/vrF69Wqv9+7fv9/o1q2be5o+ffoYN954ozFixAijW7duhs1mMyQZeXl5leZx7Ngx9/betWtXY9SoUcZNN91k9O7d27BYLIYk4y9/+YvX+/74xz+6112nTp2M66+/3rjxxhuNgQMHGnFxcYYk47XXXqt23vPmzTMkGePHj6/wczz//PMrrRUAgLMVDSwAAIKsogaWYRjGr7/+atx7771G69atjfDwcKNBgwZG7969jddee80oKiry+Z69e/caN998s5GUlGTY7XavL78ul8t46623jEsuucSIjo42YmNjjb59+xrvv/++YRj+Gy7VaWDNmzfP+OGHH4zrrrvOiI+PNyIiIoxOnToZc+bM8VvHv/71L6NPnz5GXFycER0dbXTv3t149dVXDZfLVWEuf//7342LL77YqFevnruWefPmuV+v6PMuLi423nvvPWPYsGHGeeedZ4SFhRnx8fFG586djYkTJxofffSRUVhY6J6+Og2svLw845FHHjFSUlLczbHSmrKzs40XXnjBuOGGG4y2bdsa0dHRRv369Y127doZ48aNMzZs2OB3ef58/fXXxuDBg42GDRsaVqvVZ9Pk6NGjxpQpU4yOHTsakZGRRr169YyLLrrIeOqpp4yTJ09WaXnlGy9FRUXGjBkzjA4dOhgRERFGo0aNjJEjRxo//vij3/fn5+cbr7/+ujFo0CAjPj7esNvtRmJiotGtWzfj3nvvNb788suA8igqKjJef/1146abbjI6dOhgxMbGGlFRUUabNm2MkSNHGitXrvT73m+++cb47W9/a5x//vlGRESE0aBBA6Ndu3bGb37zG+PNN9/02dCrat40sAAAqJzFMLhBHwAA1J4JEyZowYIFmjdvniZMmBDsdAAAABCCeAYWAAAAAAAATI0GFgAAAAAAAEyNBhYAAAAAAABMjWdgAQAAAAAAwNQYgQUAAAAAAABTo4EFAAAAAAAAU7MHO4Ez4XK5lJGRoQYNGshisQQ7HQAAAAAAAFTAMAydOHFCTZs2ldVa9fFUIdnAysjIUHJycrDTAAAAAAAAQBXs27dPzZs3r/L7QrKB1aBBA0klRcfExAQ5GwAAAAAAAFQkOztbycnJ7p5OVYVkA6v0tsGYmBgaWAAAAAAAACHiTB8FxUPcAQAAAAAAYGo0sAAAAAAAAGBqNLAAAAAAAABgajSwAAAAAAAAYGo0sAAAAAAAAGBqIflXCAEAAAAAQN0zDEPFxcVyOp3BTgUmYbfbZbPZzvivCwa8nFqdOwAAAAAACHmGYej48eM6cuSIiouLg50OTMZmsykxMVGxsbG11siigQUAAAAAACp08OBBHT9+XDExMYqJiZHdbq/1ETcwP8Mw5HQ6lZ2drQMHDigvL09JSUm1siwaWAAAAAAAwK/i4mI5HA4lJCSocePGwU4HJtSgQQNFREQoMzNTiYmJstlsNb4MHuIOAAAAAAD8KioqkmEYql+/frBTgYnVr19fhmGoqKioVuZPAwsAAAAAAFSKWwZRkdrePmhgAQAAAAAAwNRoYAEAAAAAAMCnCRMmqGXLlsFOgwYWAAAAAAA4d82fP18Wi8Xvv3Xr1gU7xUr99NNP+utf/6o9e/YEO5Vaw18hBAAAAAAA57wnnnhCrVq18oqnpKQEIZuq+emnnzR9+nQNHDjQFKOlagMNLAAAAAAAcMaWbQ12BtKQztWfx9VXX63u3btXf0aoFdxCCAAAAAAAUIFp06bJarVq5cqVHvE77rhD4eHh2rRpkyQpNTVVFotFH3zwgaZOnaomTZqofv36Gj58uPbt2+c132+//VZDhw5VbGys6tWrpwEDBuibb77xmm7//v2aNGmSmjZtqoiICLVq1Up33323CgsLNX/+fI0ePVqSNGjQIPetj6mpqe73f/755+rXr5/q16+vBg0a6JprrtGPP/7otZx//etf6ty5syIjI9W5c2d99NFH1fnYahQjsAAAAAAAwDnP4XAoMzPTI2axWBQfH6/HHntMS5cu1aRJk7RlyxY1aNBAX375pf7+97/rySefVNeuXT3eN2PGDFksFj366KM6fPiwXnjhBQ0ePFgbN25UVFSUJOk///mPrr76al1yySXuBtm8efN0+eWXa/Xq1erZs6ckKSMjQz179tTx48d1xx13qEOHDtq/f7+WLFmikydPqn///po8ebJeeuklTZ06VR07dpQk93/feecdjR8/XldddZWefvppnTx5Uq+99pr69u2rtLQ09y2Hy5Yt08iRI3XBBRdo1qxZOnr0qCZOnKjmzZvX5sceMIthGEawk6iq7OxsxcbGyuFwKCYmJtjpAAAAAABw1srPz9fu3bvVqlUrRUZGer0e6rcQzp8/XxMnTvT5WkREhPLz8yVJW7du1SWXXKJx48bp2WefVefOnZWUlKS1a9fKbi8ZH5SamqpBgwapWbNm2rZtmxo0aCBJWrx4scaMGaMXX3xRkydPlmEYat++vVq3bq3PP/9cFotFkpSXl6dOnTopJSVFy5YtkySNHz9e7777rr799luvWxwNw5DFYtGSJUs0evRorVq1SgMHDnS/npOTo+TkZI0ePVpz5851xw8dOqT27dtrzJgx7vhFF12kQ4cOadu2bYqNjZUkLV++XEOGDNH5559f6QPiK9tOqtvLYQQWAAAAAAA45/2///f/1K5dO4+YzWZz/3/nzp01ffp0TZkyRZs3b1ZmZqaWLVvmbl6VN27cOHfzSpJGjRqlpKQkffbZZ5o8ebI2btyonTt36rHHHtPRo0c93nvFFVfonXfekcvlklRyW991113n8/lcpY0vf5YvX67jx4/rpptu8hhdZrPZ1KtXL61atUqSdODAAW3cuFF/+tOf3M0rSbryyit1wQUXKDc3t8Ll1AUaWAAAAAAA4JzXs2fPSh/i/sc//lHvv/++1q9fr5kzZ+qCCy7wOV3btm09frZYLEpJSXGPYtq5c6ekktFV/jgcDhUWFio7O1udO5/ZELPS5Vx++eU+Xy8dCbV3716feUtS+/bt9cMPP5zR8msSDSwAAAAA57affw52BmVSUoKdAYAK7Nq1y90U2rJlyxnPp3R01bPPPqtu3br5nCY6OlpZWVlnvIzyy3nnnXfUpEkTr9d9jR4zq9DJFAAAAAAAIEhcLpcmTJigmJgYPfDAA5o5c6ZGjRqlESNGeE1b2uQqZRiGfv75Z3Xp0kWS1KZNG0klI6AGDx7sd5kJCQmKiYnR1q0VP2jM362EpctJTEyscDnnn3++z7wl6X//+1+Fy64r1mAnAAAAAAAAYHZz5szRmjVrNHfuXD355JPq06eP7r77bq+/XChJb7/9tk6cOOH+ecmSJTpw4ICuvvpqSdIll1yiNm3aaPbs2crJyfF6/5EjRyRJVqtVv/nNb7R06VJt2LDBa7rSv8tXv359SdLx48c9Xr/qqqsUExOjmTNnqqioyO9ykpKS1K1bNy1YsEAOh8P9+vLly/XTTz9V+LnUFUZgAQAAAACAc97nn3+u7du3e8X79OmjgoICPf7445owYYKuu+46SSV/vbBbt2665557tGjRIo/3NGrUSH379tXEiRN16NAhvfDCC0pJSdHvfvc7SSWNqTfffFNXX321OnXqpIkTJ6pZs2bav3+/Vq1apZiYGC1dulSSNHPmTC1btkwDBgzQHXfcoY4dO+rAgQNavHix/vvf/youLk7dunWTzWbT008/LYfDoYiICF1++eVKTEzUa6+9pltvvVUXX3yxbrzxRiUkJOjXX3/Vp59+qssuu0yvvPKKJGnWrFm65ppr1LdvX912223KysrSyy+/rE6dOvlsstU1GlgAAAAAAOCc95e//MVn/M0339Qbb7yhxo0b64UXXnDH27Ztq1mzZun+++/XokWLNGbMGPdrU6dO1ebNmzVr1iydOHFCV1xxhV599VXVq1fPPc3AgQO1du1aPfnkk3rllVeUk5OjJk2aqFevXrrzzjvd0zVr1kzffvutHn/8cS1cuFDZ2dlq1qyZrr76avf8mjRpotdff12zZs3SpEmTVFxcrFWrVikxMVE333yzmjZtqqeeekrPPvusCgoK1KxZM/Xr108TJ050L2fo0KFavHixHnvsMU2ZMkVt2rTRvHnz9O9//1upqak19CmfOYtROt4shGRnZys2NlYOh8P9xHwAAAAAOCM8xB2oUH5+vnbv3q1WrVopMjIy2OmYWmpqqgYNGqTFixdr1KhRwU6nTlW2nVS3l8MzsAAAAAAAAGBqNLAAAAAAAABgajSwAAAAAAAAYGo8xB0AAAAAAKAGDBw4UCH4qPGQwAgsAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAABwzpo/f74sFosiIyO1f/9+r9cHDhyozp07ByEzlGcPdgIAAAAAACCEffFFsDOQhg6t9iwKCgr01FNP6eWXX66BhFDTGIEFAAAAAADOed26ddPf//53ZWRkBDsV+EADCwAAAEDN+/ln8/wDgABMnTpVxcXFeuqppyqczul06sknn1SbNm0UERGhli1baurUqSooKHBP89BDDyk+Pl6GYbhj9913nywWi1566SV37NChQ7JYLHrttddqvqCzTI01sH744QcNHz5cjRo1Ur169dS5c2ePlSJJa9asUd++fVWvXj01adJEkydPVk5OTk2lAAAAAAAAcEZatWqlcePGVToK6/bbb9df/vIXXXzxxXr++ec1YMAAzZo1SzfeeKN7mn79+ikrK0s//vijO7Z69WpZrVatXr3aIyZJ/fv3r4WKzi410sBatmyZevfurcOHD+vxxx/Xiy++qGuvvVbp6enuaTZu3KgrrrhCJ0+e1Jw5c3T77bdr7ty5Gj16dE2kAAAAAAAAUC1//vOf5XQ69fTTT/t8fdOmTVqwYIFuv/12LV68WPfcc48WLFigP/zhD/rXv/6lVatWSZL69u0rqaxB5XA4tGXLFo0cOdKrgdWoUSNdcMEFtVxZ6Kv2Q9yzs7M1btw4XXPNNVqyZImsVt89salTp6phw4ZKTU1VTEyMJKlly5b63e9+p2XLlmnIkCHVTQUAAAAAAOCMtW7dWrfeeqvmzp2rP/3pT0pKSvJ4/bPPPpNUcotgeQ8//LBmz56tTz/9VIMGDVJCQoI6dOigr7/+Wnfffbe++eYb2Ww2/fGPf9TixYu1c+dOtW3bVqtXr1bfvn1lsVjqrMZQVe0RWO+9954OHTqkGTNmyGq1Kjc3Vy6Xy2Oa7OxsLV++XLfccou7eSVJ48aNU3R0tBYtWlTdNAAAAAAAAKrtsccek9Pp9PksrL1798pqtSolJcUj3qRJE8XFxWnv3r3uWL9+/dyjrVavXq3u3bure/fuatSokVavXq3s7Gxt2rRJ/fr1q92CzhLVbmCtWLFCMTEx2r9/v9q3b6/o6GjFxMTo7rvvVn5+viRpy5Ytcjqd6t69u8d7w8PD1a1bN6WlpVU3DQAAAAAAgGpr3bq1brnlFs2dO1cHDhzwOU0gI6b69u2r/fv3a9euXVq9erX69esni8Wivn37avXq1VqzZo1cLhcNrABV+xbCnTt3yul06vrrr9ekSZM0a9Yspaam6uWXX9bx48f1j3/8w73CTx96Vxorf/+nLwUFBR5P88/OzpZU8uR/p9MpSbJarbJarXK5XB4jwErjxcXFHk//9xe32WyyWCzu+ZaPS1JxcXFAcbvdLsMwPOIWi0U2m80rR39xaqImaqImaqImaqImaqKmkK6p3LytFousFouKXS4ZAcRtFktJTafd3WE79aWx2DACitut1sprOrUMiySb1SqXYchV/nM/VVed1FRuHbLtUZNZanI6ne75GaftY1LJvuMdreO4j7wCYbFYPGor/f/HHntM7777rscoLMMwdP7558vlcmnHjh3q2LGj+7XDhw/r+PHjatGihXsepc/BWrZsmb777js9+uijMgxD/fr10+uvv66kpCTVr19fF198sfs95fM5U/7mUdtxqeQzKt+rKb/tnb79VVW1G1g5OTk6efKk7rrrLvdfHRwxYoQKCwv1xhtv6IknnlBeXp4kKSIiwuv9kZGR7tf9mTVrlqZPn+4VT0tLU/369SVJCQkJatOmjXbv3q0jR464p2nevLmaN2+uHTt2yOFwuOOtW7dWYmKitm7d6rH8Dh06KC4uTmlpaR47cZcuXRQeHq4NGzZ45NC9e3cVFhZq8+bN7pjNZlOPHj3kcDi0fft2dzwqKkpdu3ZVZmamdu3a5Y7HxsaqY8eOysjI8HjwPTVREzVREzVREzVREzVRU8jWdOyYjpT7i+PNY2PVPC5OOzIz5SiXe+v4eCVGR2vrwYPKKyoqqykxUXFRUUrbv1/F5b64d0lKUrjdrg379nnWlJysQqdTm8uNlrBZreqRnFx5Tbm5JTVFRaljYqIyHA6ll/vcE6Kj1SY+vm5qysqq2/V0Nm571FQrNUVGRkoqaWqV3m0llTTN6p2Kl29QWK1WhYeFecVtNpvC7HY5nU6PXOx2u+w2m4qKijyadaXxwsJCj6ZJWFiYbFarO+48tR9HRUW5H29UXv369eVyuTw+F4vF4o5LUl5ennJzc2W1WtWmTRvdfPPNmjt3rpKTk2W325Wfn69hw4Zp6tSpmj17trsHYrfbNWfOHEnSFVdc4V528+bN1axZMz3//PMqKipSt27dlJubqz59+uiPf/yjlixZoh49ergH7URGRsput+vkyZMetZ5JTT7XU716cjqdHgOEbDaboqKiVFRUpMLCQo/PPTIyUgUFBR7rLzw8XOHh4crPz/dYf6X9nqKiIm3dutUdL7/tlQ5GOlMWo5qtvc6dO+vHH3/UV1995fFnH7/++msNGDBACxYsUL169TR69Gh9/fXXXkPjxowZo9WrV/sdlif5HoGVnJyso0ePup+pZZbOdKmzqdtOTdRETdRETdRETdRETdRU5Zp27DDPCKw2bSqu6VQjwRQjsFq3Louz7VGTSWrKz8/Xr7/+qtatW/scmGL58svgj8C66iofU1TOYrFo3rx5uu2227R+/Xr3o48sFot27typjh07qri4WJ06ddKWLVtksVg0YcIELViwQGPGjFH//v313XffacGCBfrNb36jf/7znx7zv/nmm/X+++/rwgsv1KZNmySVjGhr2LChcnNzNW3aNE2bNs0jn1AdgVVQUKBdu3apRYsW7oZn+W0vOztb8fHxcjgcHs9HD1S1R2A1bdpUP/74o8477zyPeGJioiTp2LFjatOmjST5bFIdOHBATZs2rXAZERERPncSu90uu92zhNId9nSlO2Cg8dPneyZxi8XiM+4vx6rGqYma/MWpiZokavKXY1Xj1ERNEjX5y7GqcWo6B2vysUybj2kritv9xS2+nz/jK15pTacto7QB5XN6H8us0Zp85Mm2R03Brslut8tyap+w+Nn3/D0Rqs7ifvIKRPnaytfXtm1b3XLLLVqwYIHHdG+++aZat26t+fPn66OPPlKTJk00ZcoUTZs2zevz6devn95//32PvzQYFham3r17a8WKFerfv7/Xe/x9xmdSUzDivno1vmJVVe0RWFOmTNFTTz2llStX6vLLL3fH//Of/+iKK67QwoULdc0116hx48Z68MEH9cwzz7inKSwsVHx8vMaMGaO33nor4GVmZ2crNjb2jLt2AAAAAGrZzz8HO4Myp/21MC+hlCsQBPn5+dq9e7datWrlHlkDnK6y7aS6vZxq/xXCMWPGSJJXA+rNN9+U3W7XwIEDFRsbq8GDB+vdd9/ViRMn3NO88847ysnJ0ejRo6ubBgAAAAAAAM5S1b6F8KKLLtJtt92m//u//5PT6dSAAQOUmpqqxYsXa8qUKe7bA2fMmKE+ffpowIABuuOOO5Senq7nnntOQ4YM0dChQ6tdCAAAAAAAAM5O1W5gSdLrr7+uFi1aaN68efroo490/vnn6/nnn9cDDzzgnubiiy/WihUr9Oijj+rBBx9UgwYNNGnSJM2aNasmUgAAAAAAAMBZqtrPwAoGnoEFAAAAmFwoPVcqlHIFgoBnYCEQpn8GFgAAAAAAAFCbaGABAAAAAADA1GhgAQAAAAAAwNRoYAEAAAAAAMDUaGABAAAAAADA1GhgAQAAAAAAwNRoYAEAAAAAAMDU7MFOAAAAAEAAfv452BmUSUkJdgYAEDIsFoumTZumv/71r8FOJaQxAgsAAAAAAJyTLBZLQP9SU1ODneo5jxFYAAAAAADgzJlhhOgZjgx95513PH5+++23tXz5cq94x44dzzg11AwaWAAAAAAA4Jx0yy23ePy8bt06LV++3CuO4OMWQgAAAAAAAD9yc3P18MMPKzk5WREREWrfvr1mz54twzA8pisoKNCDDz6ohIQENWjQQMOHD1d6errX/Pbu3at77rlH7du3V1RUlOLj4zV69Gjt2bPHPc2uXbtksVj0/PPPe71/zZo1slgs+sc//lHjtZoZDSwAAAAAAAAfDMPQ8OHD9fzzz2vo0KGaM2eO2rdvrz/+8Y966KGHPKa9/fbb9cILL2jIkCF66qmnFBYWpmuuucZrnt99953WrFmjG2+8US+99JLuuusurVy5UgMHDtTJkyclSa1bt9Zll12mhQsXer1/4cKFatCgga6//vraKdqkuIUQAAAAAADAh48//lj/+c9/9Le//U1//vOfJUn33nuvRo8erRdffFG///3v1aZNG23atEnvvvuu7rnnHv2///f/3NP99re/1ebNmz3mec0112jUqFEeseuuu069e/fWhx9+qFtvvVWSNG7cON15553avn27OnToIEkqKirSokWLNGLECNWrV6+2yzcVRmABAAAAAAD48Nlnn8lms2ny5Mke8YcffliGYejzzz93TyfJa7oHHnjAa55RUVHu/y8qKtLRo0eVkpKiuLg4/fDDD+7XxowZo8jISI9RWF9++aUyMzPPyWd00cACAAAAAADwYe/evWratKkaNGjgES/9q4R79+51/9dqtapNmzYe07Vv395rnnl5efrLX/7ifqZW48aNlZCQoOPHj8vhcLini4uL03XXXaf33nvPHVu4cKGaNWumyy+/vMZqDBU0sAAAAAAAAOrIfffdpxkzZmjMmDFatGiRli1bpuXLlys+Pl4ul8tj2nHjxmnXrl1as2aNTpw4oY8//lg33XSTrNZzr53DM7AAAAAAAAB8OP/887VixQqdOHHCYxTW9u3b3a+X/tflcumXX37xGHX1v//9z2ueS5Ys0fjx4/Xcc8+5Y/n5+Tp+/LjXtEOHDlVCQoIWLlyoXr166eTJk+5nZJ1rzr2WHQAAAAAAQACGDRum4uJivfLKKx7x559/XhaLRVdffbUkuf/70ksveUz3wgsveM3TZrPJMAyP2Msvv6zi4mKvae12u2666SYtWrRI8+fP14UXXqguXbpUp6SQxQgsAAAAAAAAH6677joNGjRIf/7zn7Vnzx517dpVy5Yt07///W898MAD7mdedevWTTfddJNeffVVORwO9enTRytXrtTPP//sNc9rr71W77zzjmJjY3XBBRdo7dq1WrFiheLj433mMG7cOL300ktatWqVnn766Vqt18xoYAEAAAAAAPhgtVr18ccf6y9/+Ys++OADzZs3Ty1bttSzzz6rhx9+2GPa//u//3Pf7vevf/1Ll19+uT799FMlJyd7TPfiiy/KZrNp4cKFys/P12WXXaYVK1boqquu8pnDJZdcok6dOmnbtm367W9/W2u1mp3FOH3cWgjIzs5WbGysHA6HYmJigp0OAAAAUPt8/BY/aFJSKp8mlPINpVyBIMjPz9fu3bvVqlUrRUZGBjudc9JFF12kRo0aaeXKlcFOxa/KtpPq9nJ4BhYAAAAAAIBJbdiwQRs3btS4ceOCnUpQcQshAAAAAACAyWzdulXff/+9nnvuOSUlJWns2LHBTimoGIEFAAAAAABgMkuWLNHEiRNVVFSkf/zjH+f87Zs0sAAAAAAAAEzmr3/9q1wul7Zt26YBAwYEO52go4EFAAAAAAAAU6OBBQAAAAAAAFOjgQUAAAAAACplGEawU4CJ1fb2QQMLAAAAAAD4ZbPZJElFRUVBzgRmVrp9lG4vNY0GFgAAAAAA8CssLEwRERFyOByMwoJPhmHI4XAoIiJCYWFhtbIMe63MFQAAAAAAnDUaN26s/fv3Kz09XbGxsQoLC5PFYgl2WggywzBUVFQkh8OhnJwcNWvWrNaWRQMLAAAAAABUKCYmRpKUmZmp/fv3BzkbmE1ERISaNWvm3k5qAw0sAAAAAABQqZiYGMXExKioqEjFxcXBTgcmYbPZau22wfJoYAEAAAAAgICFhYXVScMCKI+HuAMAAAAAAMDUGIEFAAAAAKHk55+DnUGZlJRgZwDgHMEILAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYWrUbWKmpqbJYLD7/rVu3zmPaNWvWqG/fvqpXr56aNGmiyZMnKycnp7opAAAAAAAA4Cxmr6kZTZ48WT169PCIpaSkuP9/48aNuuKKK9SxY0fNmTNH6enpmj17tnbu3KnPP/+8ptIAAAAAAADAWabGGlj9+vXTqFGj/L4+depUNWzYUKmpqYqJiZEktWzZUr/73e+0bNkyDRkypKZSAQAAAAAAwFmkRp+BdeLECTmdTq94dna2li9frltuucXdvJKkcePGKTo6WosWLarJNAAAAAAAAHAWqbEG1sSJExUTE6PIyEgNGjRIGzZscL+2ZcsWOZ1Ode/e3eM94eHh6tatm9LS0moqDQAAAAAAAJxlqn0LYXh4uEaOHKlhw4apcePG+umnnzR79mz169dPa9as0UUXXaQDBw5IkpKSkrzen5SUpNWrV1e4jIKCAhUUFLh/zs7OliQ5nU73iC+r1Sqr1SqXyyWXy+WetjReXFwswzAqjdtsNlksFq+RZDabTZJUXFwcUNxut8swDI+4xWKRzWbzytFfnJqoiZqoiZqoiZqoiZqoyZ27yyWrxSKrxaJil0tlFUm2U39EyVluHqVxSSo2jIDidqu1pKZycYskm9Uql2HIVRp3OgOrqdy8/eVeZzVVtJ5OLcNnrSr5rX+d1VRuu/S77UmBrae6qMkwQnN/qiAesscIaqImk9fk6469qqh2A6tPnz7q06eP++fhw4dr1KhR6tKli6ZMmaIvvvhCeXl5kqSIiAiv90dGRrpf92fWrFmaPn26VzwtLU3169eXJCUkJKhNmzbavXu3jhw54p6mefPmat68uXbs2CGHw+GOt27dWomJidq6davH8jt06KC4uDilpaV5rOwuXbooPDzcY2SZJHXv3l2FhYXavHmzO2az2dSjRw85HA5t377dHY+KilLXrl2VmZmpXbt2ueOxsbHq2LGjMjIylJ6e7o5TEzVREzVREzVREzVREzW5a8rNVev4eCVGR2vrwYPKKyoqqykxUXFRUUrbv1/F5b5odElKUrjdrg379nnWlJysQqdTm0/9olkqaXL0SE6WIz9f2w8fLqspLExdmzZVZm6udh09WhLMyqq8pmPHdKTcXxxvHhur5nFx2pGZKUe59VEnNVW2nnJzS9ZTVJQ6JiYqw+FQerltKSE6Wm3i4+umpqysspr8bXsNGwa2nuqqplDcn3QWHiOoiZpMXlPpYKQzZTGM035FUUNuuukm/fOf/9TJkyf10UcfafTo0fr666/Vr18/j+nGjBmj1atXu0dp+eJrBFZycrKOHj3qfqYWHU9qoiZqoiZqoiZqoiZqOqtr2rXLPCOwWreuvKYdO8wzAqtNm4rX06kvc6YYgdW6dVnc37a3Z495RmC1bRua+1MF8ZA9RlATNZm8puzsbMXHx8vhcHg8Hz1QNfZXCE+XnJyswsJC5ebmum8d9NWkOnDggJo2bVrhvCIiInyO3rLb7bLbPUso/dBOV7piA42fPt8ziVssFp9xfzlWNU5N1OQvTk3UJFGTvxyrGqcmapKoyV+OVY1TUzVrKve6zce0Ukmzxmf8VIMkkLjFYvEZL21glLyxrOYKa/KxTH+513pNFa2n05bhUevp0/tYZo3W5CNPv9teZespkHh1azo1z5DbnwKIUxM1UVPN1uQv/0DV6F8hLG/Xrl2KjIxUdHS0OnfuLLvd7jXcrbCwUBs3blS3bt1qKw0AAAAAAACEuGo3sMrfC1lq06ZN+vjjjzVkyBBZrVbFxsZq8ODBevfdd3XixAn3dO+8845ycnI0evTo6qYBAAAAAACAs1S1byEcO3asoqKi1KdPHyUmJuqnn37S3LlzVa9ePT311FPu6WbMmKE+ffpowIABuuOOO5Senq7nnntOQ4YM0dChQ6ubBgAAAAAAAM5S1R6B9Zvf/EaZmZmaM2eO7rnnHn3wwQcaMWKENmzYoI4dO7qnu/jii7VixQpFRUXpwQcf1Ny5czVp0iQtWbKkuikAAAAAAADgLFZrf4WwNmVnZys2NvaMn1wPAACAWvLzz8HOoExKSuXThFK+oZSrFFr5hlKuUujlCwCqfi+n1h7iDgAAAAAAANQEGlgAAAAAAAAwNRpYAAAAAAAAMDUaWAAAAAAAADA1GlgAAAAAAAAwNRpYAAAAAAAAMDUaWAAAAAAAADA1GlgAAAAAAAAwNRpYAAAAAAAAMDUaWAAAAAAAADA1GlgAAAAAAAAwNRpYAAAAAAAAMDUaWAAAAAAAADA1GlgAAAAAAAAwNRpYAAAAAAAAMDUaWAAAAAAAADA1GlgAAAAAAAAwNRpYAAAAAAAAMDUaWAAAAAAAADA1GlgAAAAAAAAwNRpYAAAAAAAAMDV7sBMAAAAAAJylfv452BmUSUkJdgYAqoERWAAAAAAAADA1GlgAAAAAAAAwNRpYAAAAAAAAMDUaWAAAAAAAADA1GlgAAAAAAAAwNRpYAAAAAAAAMDV7sBMAAAAAAMAUfv452BmUSUkJdgaAqTACCwAAAAAAAKZGAwsAAAAAAACmRgMLAAAAAAAApkYDCwAAAAAAAKZGAwsAAAAAAACmRgMLAAAAAAAApkYDCwAAAAAAAKZmD3YCAAAAAACgin7+OdgZlElJCXYGOAcwAgsAAAAAAACmRgMLAAAAAAAApkYDCwAAAAAAAKZGAwsAAAAAAACmRgMLAAAAAAAApkYDCwAAAAAAAKZGAwsAAAAAAACmRgMLAAAAAAAApkYDCwAAAAAAAKZGAwsAAAAAAACmRgMLAAAAAAAApkYDCwAAAAAAAKZGAwsAAAAAAACmZg92AgAAAKjEzz8HO4MyKSnBzgAAAJyDGIEFAAAAAAAAU6OBBQAAAAAAAFOjgQUAAAAAAABTo4EFAAAAAAAAU6OBBQAAAAAAAFOjgQUAAAAAAABTo4EFAAAAAAAAU6OBBQAAAAAAAFOrlQbWjBkzZLFY1LlzZ6/X1qxZo759+6pevXpq0qSJJk+erJycnNpIAwAAAAAAAGcBe03PMD09XTNnzlT9+vW9Xtu4caOuuOIKdezYUXPmzFF6erpmz56tnTt36vPPP6/pVAAAAAAAAHAWqPEG1h/+8AddeumlKi4uVmZmpsdrU6dOVcOGDZWamqqYmBhJUsuWLfW73/1Oy5Yt05AhQ2o6HQAAAAAAAIS4Gr2F8Ouvv9aSJUv0wgsveL2WnZ2t5cuX65ZbbnE3ryRp3Lhxio6O1qJFi2oyFQAAAAAAAJwlaqyBVVxcrPvuu0+33367LrzwQq/Xt2zZIqfTqe7du3vEw8PD1a1bN6WlpdVUKgAAAAAAADiL1NgthK+//rr27t2rFStW+Hz9wIEDkqSkpCSv15KSkrR69Wq/8y4oKFBBQYH75+zsbEmS0+mU0+mUJFmtVlmtVrlcLrlcLve0pfHi4mIZhlFp3GazyWKxuOdbPi6VNOoCidvtdhmG4RG3WCyy2WxeOfqLUxM1URM1URM1URM1SZJcLlkk2axWuQxDrnLL9Be3nsrT5XLJVW7eVotFVotFxS6XjADiNoulpKbSz+VUbX5rOpVDsWF4xO1Wa0lNAeReYzW5XJWvp3Lr22ax+MzdX7zGayq33fjcxlyuwNdTbdfkdAa2P5Wbd7W3verWVNEx4tQy6nx/8pV7ue3A7zFCqvv9yV9NhlHxcS/A9Vcnx4hAjuUuV93vT/7iTmfF5ycpePvT6blLZ885t4Lcqal6NZ1eV1XVSAPr6NGj+stf/qLHH39cCQkJPqfJy8uTJEVERHi9FhkZ6X7dl1mzZmn69Ole8bS0NPfD4hMSEtSmTRvt3r1bR44ccU/TvHlzNW/eXDt27JDD4XDHW7durcTERG3dutVj2R06dFBcXJzS0tI8VnaXLl0UHh6uDRs2eOTQvXt3FRYWavPmze6YzWZTjx495HA4tH37dnc8KipKXbt2VWZmpnbt2uWOx8bGqmPHjsrIyFB6ero7Tk3URE3URE3URE3UJEnKzVVUWJi6Nm2qzNxc7Tp6tKymqCh1TExUhsOh9HI5JkRHq018vHYfO6Yj5f7ic/PYWDWPi9OOzEw5yuXeOj5eidHR2nrwoPKKispqSkxUXFSU0vbvL/kimpVVcU2NGqnQ6dTmU7+8lEq+lPVITpYjP1/bDx8uW0+1XVNcXOXr6dQvRiWpS1KSwu12bdi3z7Om5OS6qancZ+lz28vNDXw91XZNWVmV7081ve1Vp6bKjhG5uYGvp9qu6dQ+JlVwjGjYsO73p4pqqui4F6z9yVdNgRzLc3Prfn/yV1NWVsXnJyk4+5Ovmtq1q/yce2o/c6+no0d9r6fDh33XlJHhu6Z9+6pe06k+wjlzHWGSmrLLnXPPhMUwTmupnoG7775bK1as0I8//qjw8HBJ0sCBA5WZmamtW7dKkpYsWaLRo0fr66+/Vr9+/TzeP2bMGK1evdo9Sut0vkZgJScn6+jRo+7nadHxpCZqoiZqoiZqoqaztqZdu8wzAqt164pr2r27JG6GEVgpKZWvp3IX8UEfgXXqs5X8bGO7dplnBFbr1pXvTzt2mGcEVps2FR8jTm0HphiBVW478HuM2LPHPCOw2rat+Li3c6f/WsvXVBfHiFatKj+W79plnhFYrVtXfH7atcs8I7Datav8nHtqP6vT/clfvNx+dk5cR5ikpuzsbMXHx8vhcHg8Gz1Q1R6BtXPnTs2dO1cvvPCCMjIy3PH8/HwVFRVpz549iomJcd866KtJdeDAATVt2tTvMiIiInyO3LLb7bLbPUso/dBOV7piA42fPt8ziVssFp9xfzlWNU5N1OQvTk3UJFGTvxyrGqcmapJMUFO5nEov5E/nN261+nzoqc1HnRXF7aXx03L1yv1UDnYfuVgsFp/xWqvp1M8Vricf9frK0V+8RmvysR145F4u10rXUwC5+4sHVFO5XCvcn3ws84y3vdPjVa2pomPEacuos/3p9LjF4rWPSRUcI+pyf/IXL93n/R3fqrD+ar2mQI7l5fKts/3JXzyA/Sxo+5O/z72ic+vp+1kwjxGnba9n/XVEADnWRU3+8g9UtR/ivn//frlcLk2ePFmtWrVy//v222+1Y8cOtWrVSk888YQ6d+4su93uNeStsLBQGzduVLdu3aqbCgAAAAAAAM5C1R6B1blzZ3300Ude8ccee0wnTpzQiy++qDZt2ig2NlaDBw/Wu+++q8cff1wNGjSQJL3zzjvKycnR6NGjq5sKAAAAAAAAzkLVbmA1btxYv/nNb7ziL7zwgiR5vDZjxgz16dNHAwYM0B133KH09HQ999xzGjJkiIYOHVrdVAAAAAAAAHAWqvYthFVx8cUXa8WKFYqKitKDDz6ouXPnatKkSVqyZEldpgEAAAAAAIAQUu0RWP6kpqb6jPft21fffPNNbS0WAAAAAAAAZ5k6HYEFAAAAAAAAVBUNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYmj3YCQAAAAAAAJjG228HO4My48YFOwPTYAQWAAAAAAAATI0GFgAAAAAAAEyNBhYAAAAAAABMjQYWAAAAAAAATI0GFgAAAAAAAEyNBhYAAAAAAABMjQYWAAAAAAAATI0GFgAAAAAAAEyNBhYAAAAAAABMjQYWAAAAAAAATI0GFgAAAAAAAEyNBhYAAAAAAABMzR7sBAAAAACcfdb+EuwMyvROCXYGAIDqooEFAAAAhAAaQgCAcxm3EAIAAAAAAMDUaGABAAAAAADA1GhgAQAAAAAAwNRoYAEAAAAAAMDUaGABAAAAAADA1GhgAQAAAAAAwNRoYAEAAAAAAMDUaGABAAAAAADA1KrdwPrxxx81evRotW7dWvXq1VPjxo3Vv39/LV261Gvabdu2aejQoYqOjlajRo1066236siRI9VNAQAAAAAAAGcxe3VnsHfvXp04cULjx49X06ZNdfLkSX344YcaPny43njjDd1xxx2SpPT0dPXv31+xsbGaOXOmcnJyNHv2bG3ZskXr169XeHh4tYsBAAAAAADA2afaDaxhw4Zp2LBhHrHf//73uuSSSzRnzhx3A2vmzJnKzc3V999/rxYtWkiSevbsqSuvvFLz5893TwcAAAAAdWntL8HOoEzvlGBnAADmVCvPwLLZbEpOTtbx48fdsQ8//FDXXnutu3klSYMHD1a7du20aNGi2kgDAAAAAAAAZ4Fqj8AqlZubq7y8PDkcDn388cf6/PPPNXbsWEnS/v37dfjwYXXv3t3rfT179tRnn31WU2kAAAAAAADgLFNjDayHH35Yb7zxhiTJarVqxIgReuWVVyRJBw4ckCQlJSV5vS8pKUlZWVkqKChQRESEz3kXFBSooKDA/XN2drYkyel0yul0updptVrlcrnkcrnc05bGi4uLZRhGpXGbzSaLxeKeb/m4JBUXFwcUt9vtMgzDI26xWGSz2bxy9BenJmqiJmqiJmqiJmqSJLlcskiyWa1yGYZc5ZbpL249lafL5ZKr3LytFousFouKXS4ZAcRtFktJTaWfy6na/NZ0Kodiw/CI263WkpoCyL3GanK5Kl9P5da3zWLxmbu/eI3XVG678bWNGYZLUsn6KPn/8vzHSxgBxS0W66nlVRx3Op2V7k9VybEuaqroGFF+GRV/BrVfU/njh99jhFT3+5O/Y4RhVHzcc3nWWmf7k6/cAzmWu1zex71Kcq+1mpzOis9P0pkfy2u6Jqnyc+6p12rt/FSVmsptrz6vI0prOvWvsrj11D9/8WJ5HlH8xW2nluGxNzmdZ8210enHiaqqsQbWAw88oFGjRikjI0OLFi1ScXGxCgsLJUl5eXmS5LNBFRkZ6Z7GXwNr1qxZmj59ulc8LS1N9evXlyQlJCSoTZs22r17t8dfNmzevLmaN2+uHTt2yOFwuOOtW7dWYmKitm7d6s5Pkjp06KC4uDilpaV5rOwuXbooPDxcGzZs8Mihe/fuKiws1ObNm90xm82mHj16yOFwaPv27e54VFSUunbtqszMTO3atcsdj42NVceOHZWRkaH09HR3nJqoiZqoiZqoiZpqqaYfflB6uRwToqPVJj5eu48e1ZGcnLKaYmPVPC5OOw4flqNc7q3j45UYHa2tGRnKKyoqqykxUXFRUUrbt8/jS1uXpCSF2+3asG+fZ03JySps3rzymnJzFRUWpq5NmyozN1e7jh4tqykqSh0TE5XhcPiu6dgx3zVlZvqu6eBB3zXt319SU1ZWxeupUSMVOp3afOoXmFLJl7Ieycly5Odr++HDZeuptmuKi6t82zv1i9FK11Nd1FTus/S1PzmKchVli1eELVo5zoMqNsrWU317osIsUcou2i+j3NenBmFJssouR5FnTbFhyXLJqRNFZTVZZFVseLKcRr5ynWU12SxhahDWVIWuXOUVl9S0YUNWpceIvOJjKnSVradIW6wibXHKdWbKaZStj7qoqbJjhKMoV5Jkt0QpOixRBS6H8ovL1lO4NVr17PF1UtOGDVnuuN/jXsOGdb8/VXSMqOhYHqz9yVdNgZyfcnO9j3ulNdX1MSIrq+JzrnTmx/Karqldu8qvI3JzA1tPdVHTqXOZ3+uIyEh1zc9Xpt2uXeX+4FxscbE6FhQoIyxM6WFh7niC06k2hYXaHR6uI/ayNkvzoiI1LyrSjogIOU41mySpdWGhEp1ObY2MVJ617MlOHfLzFedyKS0qSsWnGm7asOGsud7LLnfOPRMWwzitLVlDhgwZouPHj+vbb7/V999/rx49eujtt9/Wrbfe6jHdI488omeffVb5+flVGoGVnJyso0ePKiYmRlII/OZU5uh4UhM1URM1URM1UZNNrp0762a0Urm45Oe3wSkplde0a5d5RmC1bl0S97eedu/2WWtQRmClpFS+7ZW7iA/6CKxTn63ke79Zv2KXzDICq+fg1pUeI9Z8sSPgHGu7pkuHtKnwGFHy2QbyGdT+CKyeg8u2A7/HvT17zDMCq23bio/lO3d6xoM5AqtVq8rPT7t2mWcEVuvWFZ9zd+0yzwisdu0qv444dbw1xQiscsdbn9cR771nnhFYN9981lzvZWdnKz4+Xg6Hw93LqYoaG4F1ulGjRunOO+/Ujh073LcOHijXvS114MABNWrUyG/zSioZueXrdbvdLrvds4TSD+10pSs20Pjp8z2TuMVi8Rn3l2NV49RETf7i1ERNEjX5y7GqcWo6S2s6dTHsc3ofy7T5mEdFcbu/uI9lyk/uHjWVm5/f3OuqptNy9cr9VA6+arVYLD7jtVbTqZ8r3PZ81OtzPfmJ12hNPraD8rlbLFaf/++Zj7+/0eS7Jl9xi8VSabz8eve3n1U1x9quqaJjxOnL8P8Z1H5NvvL0e4yoy/3JX9zivU2UV5XjYa3XFMj5qVy+VTqW+4lXq6YA9rNaPT/5ifutqbLrhdNeC8o5tzR+2vbq9xhx6l914763PP9xj0zK5RXq13v+8g+UvyNntZUOGXM4HGrWrJkSEhK8hrtJ0vr169WtW7faSgMAAAAAAAAhrtojsA4fPqzExESPWFFRkd5++21FRUXpggsukCSNHDlSCxYs0L59+5ScnCxJWrlypXbs2KEHH3ywumkAAAAAVbb2l2BnUKZ3SrAzAADAvKrdwLrzzjuVnZ2t/v37q1mzZjp48KAWLlyo7du367nnnlN0dLQkaerUqVq8eLEGDRqk+++/Xzk5OXr22Wd14YUXauLEidUuBAAAAAAAAGenajewxo4dq7feekuvvfaajh49qgYNGuiSSy7R008/reHDh7unS05O1ldffaWHHnpIf/rTnxQeHq5rrrlGzz33XIXPvwIAAAAAAMC5rdoNrBtvvFE33nhjQNN26tRJX375ZXUXCQAAAAAAgHNIrT3EHQAAAAAAAKgJNLAAAAAAAABgajSwAAAAAAAAYGo0sAAAAAAAAGBqNLAAAAAAAABgatX+K4QAAAAAgLqz9pdgZ1Cmd0qwMwBwrmAEFgAAAAAAAEyNBhYAAAAAAABMjQYWAAAAAAAATI0GFgAAAAAAAEyNBhYAAAAAAABMjQYWAAAAAAAATI0GFgAAAAAAAEyNBhYAAAAAAABMjQYWAAAAAAAATI0GFgAAAAAAAEyNBhYAAAAAAABMjQYWAAAAAAAATI0GFgAAAAAAAEyNBhYAAAAAAABMzR7sBAAAAAAAZ6e1vwQ7gzK9U4KdAYDqYAQWAAAAAAAATI0GFgAAAAAAAEyNBhYAAAAAAABMjQYWAAAAAAAATI0GFgAAAAAAAEyNBhYAAAAAAABMzR7sBAAAAHD2WPtLsDMo0zsl2BkAAICawggsAAAAAAAAmBojsMzi55+DnUGJFH5VCQAAAAAAzIURWAAAAAAAADA1GlgAAAAAAAAwNW4hBAAAAABA/CEKwMwYgQUAAAAAAABTo4EFAAAAAAAAU6OBBQAAAAAAAFOjgQUAAAAAAABTo4EFAAAAAAAAU6OBBQAAAAAAAFOjgQUAAAAAAABTo4EFAAAAAAAAU6OBBQAAAAAAAFOzBzsBAAAAAABQNWt/CXYGZXqnBDsDnAsYgQUAAAAAAABTYwQWAACoGT//HOwMyqTwq2AAAICzCSOwAAAAAAAAYGo0sAAAAAAAAGBqNLAAAAAAAABgajSwAAAAAAAAYGo0sAAAAAAAAGBqNLAAAAAAAABgavZgJ4AQxJ9JB4C6wfEWAACcJdb+EuwMyvTmsiYkMQILAAAAAAAApkYDCwAAAAAAAKZGAwsAAAAAAACmRgMLAAAAAAAApkYDCwAAAAAAAKbGXyEEAAAAAAA45ZfMYGdQpk2wEzARRmABAAAAAADA1GhgAQAAAAAAwNSqfQvhd999pwULFmjVqlXas2eP4uPjdemll+pvf/ub2rVr5zHttm3b9OCDD+q///2vwsPDdc0112jOnDlKSEiobhoAAABnrbW/BDuDMr1Tgp0BAAA4F1W7gfX000/rm2++0ejRo9WlSxcdPHhQr7zyii6++GKtW7dOnTt3liSlp6erf//+io2N1cyZM5WTk6PZs2dry5YtWr9+vcLDw6tdDAAAAAAAAM4+1W5gPfTQQ3rvvfc8GlBjx47VhRdeqKeeekrvvvuuJGnmzJnKzc3V999/rxYtWkiSevbsqSuvvFLz58/XHXfcUd1UAAAAAAAAcBaq9jOw+vTp4zV6qm3bturUqZO2bdvmjn344Ye69tpr3c0rSRo8eLDatWunRYsWVTcNAAAAAAAAnKVq5SHuhmHo0KFDaty4sSRp//79Onz4sLp37+41bc+ePZWWllYbaQAAAAAAAOAsUO1bCH1ZuHCh9u/fryeeeEKSdODAAUlSUlKS17RJSUnKyspSQUGBIiIifM6voKBABQUF7p+zs7MlSU6nU06nU5JktVpltVrlcrnkcrnc05bGi4uLZRhGpXGbzSaLxeKeb/m4JBUXFwcUt9vtMgzDI26xWGSz2bxytFgssklyGYZc5XM8lafL5ZKr3LytFousFouKXS4ZAcRtFktJTa7ycymJS1JxuWXK6ay8pvK5S7JZrV65+4vXeE11vZ58xEN+26MmaqIm89ZUbvoqHcsriNut1pKaAjhme8TLfZZ+azKM2js/VbWm4uKK15MZzrml8dO2Mcl72zMM16n8rae2F8/5VBz3zEUqyfFM46X7lb/9pmx7rkqOtVOTy+Wq9Bjh+R6Lz9z9xWu6JqeP/ax87iW5Vn391UZNTqez0uNeTW971a2pomN5+WXU5f7kK/fy24G//UxSne9P/uKGYVR4zg10/dXFMSKQ64jK9jNfuddWTU6ns8LriLJ8vWut62OEpEqvjbz3s+AdI8pvr76u91wWyWqUzMGweM7FZ9wouZZwlV+MJItR8qPrtHlUJe6s4Du6aa9h/ZxzTz9OVFWNN7C2b9+ue++9V71799b48eMlSXl5eZLks0EVGRnpnsZfA2vWrFmaPn26VzwtLU3169eXJCUkJKhNmzbavXu3jhw54p6mefPmat68uXbs2CGHw+GOt27dWomJidq6das7P0nq0KGD4uLilJaW5rGyu3TpovDwcG3YsMEjh+7du6uwsFCbN292x2w2m3r06CGHw6Ht27e741FRUeratasyMzO1a9cudzw2NlYdw8KU4XAovVyOCdHRahMfr93HjulITk5ZTbGxah4Xpx2ZmXKUy711fLwSo6O19eBB5RUVldWUmKi4qCil7d/v0XzqkpSkcLtdG/btKysoK6vymspNHxUWpq5NmyozN1e7jh4tqykqSh0TE2u/prpeTx07KiMjQ+np6WU1hfq2R03UdK7VlJ7uedyT1D05WYVOpzaf+oWLVNK46ZGcLEdenrYfPlxWU+lxLyfH93Hv+HHfx72jR72Pe927V1xTZmZZTVU5lldWU36+75oqOpaX2w78rie7vfbOT1WtKS+v4m3PDOfc0pry8irdnxxFubJZwtQgrKkKXbnKKy5bT3ZLlKLDElXgcii/uKymcGu06tnjlVd8TIWuspoibbGKtMUp15kpp1FWU5QtXhG2aOU4D6rYKKupvj1RYZYoZRftlyGXNmzIKqnJzzFCaiSXnDpRVLaeLLIqNjxZTiNfuc6y9VTbNWVmxlV6jHAUZbvjDcKSZJVdjiLP9RQbllwnNZX/LH0d9xxFuQGvp9quacOGrEqP5TW97VWnpsrOT46i3IDXU23XVLqPSf7PuVLDOt+f/NXkcCRWeB0RrP3JV02BXEc4inLrfH/yV9OGDVkVXhtJCsr+5KsmqV2l13ul+1ld7k/+airdz/xdwxbFR6ppZr5youzKii17ZFJkQbHOO1YgR3SYHNFh7nh0nlPxjkIdiw1XTlRZmyU2p0hxOUU6Eheh/AibO97IUagGeU4djI9Ukb3sxrjErHxFFbqUnhgl49Qvv45u2HDWXJeXDkY6UxajfGusmg4ePKjLLrtMRUVFWrdunZo2bSpJ2rBhg3r06KG3335bt956q8d7HnnkET377LPKz8+v0gis5ORkHT16VDExMZLOgt/a795tjt8Gt25deU07d5blriCPwGrZ0rOms6QzTU3URE21WNPPP9f+aKVAj3tt21Zc0y+/eOQY1BFYrVp55ei1nnbvNs8IrDZtKt72du4M/jm3NJ6SUun+tH7FrlP5B38EVs/BrUty93MsWL9i96n/C/4IrEuHpFR6jCj9bEvn4yv3uhoxUvrZSr6PbyW5mmMEVs/BrSs9lq/5YkfAOdZ2TZcOaVPh+an8dhDsEVjltwN/+9l3K/eYZgRW76vaVngdsfbLnfIUvBFYPQe3qvQ6orL9zFfutVVTz8GtK7w2+nb5LtOMwOoztF2l13ve+1nwRmCV3898XcPufvk904zAanXfzWfNdXl2drbi4+PlcDjcvZyqqLERWA6HQ1dffbWOHz+u1atXu5tXUtmtgwfK/ca01IEDB9SoUSO/zSupZOSWr9ftdrvsds8SSj+005Wu2EDjp8/3TOIWi8Vn3F+OpRfDPqf3sUybj3lUFLf7i5dfZrl8/dZUldxru6ZgrKcqxkNi26MmavKTY1XjIVGTxeJ53Cs/vY+4xc/0NXbcq6gmH59BQMfySuJnVFMg6/XUe2vl/FRJ3KumU5+rqc+5pfzsN+X3J4vF6hH3uDquNO47lzONn57r6T9b3DVWJcfaqal03Vd0jPA9L9/bXm3X5Gs7KJ+753ZQtfVX0zWVz9XfflbT256PVwKOV3Z+On0ZdbU/+XjFZ57+jhF1uT/5i5fu8/6uF6qy/mq7pkCuIwLZz+rqGFGX+1lN1FTZdZ33thO8Y4Svc5fH522UzcHiY8iPv7hV8nV3pXt+ZxIvn1eoX5f7yz9QNdLAys/P13XXXacdO3ZoxYoVuuCCCzxeb9asmRISEnwMMZfWr1+vbt261UQaAAAAAAAAOAtV+68QFhcXa+zYsVq7dq0WL16s3r17+5xu5MiR+uSTT7Sv3LMfVq5cqR07dmj06NHVTQMAAAAAAABnqWqPwHr44Yf18ccf67rrrlNWVpbeffddj9dvueUWSdLUqVO1ePFiDRo0SPfff79ycnL07LPP6sILL9TEiROrmwYAAAAAAADOUtVuYG3cuFGStHTpUi1dutTr9dIGVnJysr766is99NBD+tOf/qTw8HBdc801eu655yp8/hUAAAAAAADObdVuYKWmpgY8badOnfTll19Wd5EAAAAAAAA4h1T7GVgAAAAAAABAbaKBBQAAAAAAAFOjgQUAAAAAAABTo4EFAAAAAAAAU6OBBQAAAAAAAFOjgQUAAAAAAABTo4EFAAAAAAAAU6OBBQAAAAAAAFOjgQUAAAAAAABTo4EFAAAAAAAAU6OBBQAAAAAAAFOjgQUAAAAAAABTswc7AQAAgLq29pdgZ1Cmd0qwMwAAADA/RmABAAAAAADA1GhgAQAAAAAAwNRoYAEAAAAAAMDUaGABAAAAAADA1GhgAQAAAAAAwNRoYAEAAAAAAMDUaGABAAAAAADA1OzBTgAl1v4S7AxK9E4JdgYAAAAAAACeaGChyszSbJNouAEAAAAAcC7gFkIAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJgaDSwAAAAAAACYGg0sAAAAAAAAmBoNLAAAAAAAAJiaPdgJALVt2dZgZ1BiSOdgZwAAAAAAQGhiBBYAAAAAAABMjQYWAAAAAAAATI1bCAEAQI1Y+0uwMyjTOyXYGQAAAKAmMQILAAAAAAAApkYDCwAAAAAAAKZGAwsAAAAAAACmRgMLAAAAAAAApsZD3HHWa7D/52CnUKIzTxQGAAAAAOBMMAILAAAAAAAApkYDCwAAAAAAAKZGAwsAAAAAAACmRgMLAAAAAAAApkYDCwAAAAAAAKZGAwsAAAAAAACmZg92AgDK+fnnYGdQJiUl2BkAAAAAACCJBhZgKmt/CXYGZXrTvwIAAAAAmAS3EAIAAAAAAMDUaGABAAAAAADA1LiFEAAAk+K2YgAAAKAEI7AAAAAAAABgajSwAAAAAAAAYGo0sAAAAAAAAGBqNLAAAAAAAABgajSwAAAAAAAAYGo0sAAAAAAAAGBqNLAAAAAAAABgajSwAAAAAAAAYGo0sAAAAAAAAGBqNLAAAAAAAABgajSwAAAAAAAAYGo10sDKycnRtGnTNHToUDVq1EgWi0Xz58/3Oe22bds0dOhQRUdHq1GjRrr11lt15MiRmkgDAAAAAAAAZyF7TcwkMzNTTzzxhFq0aKGuXbsqNTXV53Tp6enq37+/YmNjNXPmTOXk5Gj27NnasmWL1q9fr/Dw8JpIBwAAAAAAAGeRGmlgJSUl6cCBA2rSpIk2bNigHj16+Jxu5syZys3N1ffff68WLVpIknr27Kkrr7xS8+fP1x133FET6QAAAAAAAOAsUiO3EEZERKhJkyaVTvfhhx/q2muvdTevJGnw4MFq166dFi1aVBOpAAAAAAAA4CxTZw9x379/vw4fPqzu3bt7vdazZ0+lpaXVVSoAAAAAAAAIITVyC2EgDhw4IKnkdsPTJSUlKSsrSwUFBYqIiPB6vaCgQAUFBe6fs7OzJUlOp1NOp1OSZLVaZbVa5XK55HK53NOWxouLi2UYRqVxm80mi8Xinm/5uCQVFxcHFLfb7TIMwyNusVhks9m8crRYLJJ0Kg/DYz4Wi1WG4ZIniywWS43ES5Qt0+l0VlrT6fMpydFf7rVbUyDrqeS93rWeee5nVtPp26qvba8sX8/5+Mq9tmuSFLL7k694qB8jqKnmalr7s6/tPTjHiD4pqqQml8f0gR7La6Om8p+lv/VkGEatnZ+qWlNxcXGF254Zzrml8dP3G8l7fyqdXzDPuaefz/wdC8q25+Cdc0u5XK5KjxGn72e+cq+rY4Sv/ax87qXXNHW9P/mKO53OSo/lwdifKqqpovNT+WXU5f7kK/fy24G//Uyq6LtD3R4jSo/9/q4jAl1/dXGMCOQ6orL9zFfutVWT0+ms8NqoLF/vWuv6GCF5f3eofD8L3jGi/Pbq6xrWZZGsRskcDIvnXHzGjZLRQa7yi5FkMUp+dJ02j6rEK/qOHmrX5acfJ6qqzhpYeXl5kuSzQRUZGemextfrs2bN0vTp073iaWlpql+/viQpISFBbdq00e7duz3+qmHz5s3VvHlz7dixQw6Hwx1v3bq1EhMTtXXrVnduktShQwfFxcUpLS3NY2V36dJF4eHh2rBhg0cO3bt3V2FhoTZv3uyO2Ww29ejRQw6HQ9u3b3fHo6Ki1LVrV2VmZmrXrl3ueGxsrKQwFbgcyi8uyzHcGq169njlFR9ToSun7POyxSrSFqdcZ6acRlnuUbZ4RdiileM8qGKjyB2vb09UmCVK2UX7Zahsw2sQliSr7HIU7XPHNmzIqrSm8tPbLGFqENZUha5c5RUfdcftlihFhyXWek2BrCdHUa5iw5LlklMnig644xZZFRueLKeRr1zn4VqvacOGLEkVb3uSAlpPkmq9JkmV7k/HjuR6rKcTRRne68kaJUfhvmrXVOTK81lTQXGOIhvll80jNlYdO3ZURkaG0tPT3fFQP0ZQU83VJBl1vj/5O0Z</t>
+          <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAAChb0lEQVR4nOzdeXxU9dn///eZmWxkNSGRLSghKpuAsigIIoqIuLQqCLYoUHtra9VatbZqW0RvodaltvV29ytu/VmhtZVWBUGwVEGMRhCBghKRHUJgQkKWWc7vjzBbZiYzIcucwOv5ePiQXHPmzHXNOZ9zzlz5zIlhmqYpAAAAAAAAwKJsiU4AAAAAAAAAaAoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAANqRYRjN/u+8885LdNp+J598sgzD0DfffJPoVFrE996ibX3zzTcyDEMnn3xyolMBAAAdnCPRCQAAcDyZPn16WGz37t1atGhR1Mf79OnTrNdYvny5xo4dqzFjxmj58uVHlWdHdt555+mDDz7QsmXLLNX8i8TXRDNNs81f67777tPs2bM1a9Ys3XfffW3+egAAAK2JBhYAAO1o3rx5YbHly5f7G1iRHkfr27BhQ6JTAAAAQDPQwAIAAMed5s5qAwAAQGJxDywAACxu+/btuuWWW3TKKacoNTVV2dnZOuecc/TMM8/I4/GELHveeedp7NixkqQPPvgg5F5awfch2rdvn/74xz9q4sSJ6tWrl9LS0pSVlaWhQ4fqoYceUm1tbavlP2PGDBmGoXnz5mnNmjW68sorlZ+fr7S0NA0cOFB/+MMfwuqQpEOHDum5557TlVdeqVNOOUXp6elKT0/X6aefrnvvvVcHDx4MWX758uUyDEMffPCBJGns2LEh9QfPbmvqHlhut1vPP/+8zjvvPOXm5iolJUW9evXSj3/8Y23bti1sed/rnnfeeXK5XHrooYfUv39/paWlKS8vT1deeWXYjK/77rsv5PUb3/cs+B5j8+fP17hx45SXl6ekpCTl5eWpX79++p//+R+tXbs21tvvX//s2bMlSbNnzw55rRkzZoQsW1FRoXvuuUf9+/dXp06dlJmZqSFDhuh3v/udampq4nq9SNxut373u9/535vOnTvr6quv1saNG6M+p6amRo8++qjOPvts5eTkKDU1Vaeddpruuusu7d+/v9k5LFmyRJdddplOPPFEJSUl6YQTTtApp5yiadOm6d///nfE5yxdulRXXnmlunbtquTkZBUUFOiKK67QypUrWy3vefPm+bdFdXW17r77bhUXFyslJUVdunTR9OnTtWPHjmbXCwDAsYQZWAAAWNgnn3yiCRMmqKKiQj179tR3v/tdOZ1OLV++XB999JHefPNNvfXWW0pOTpYkTZgwQampqVq0aJFOPPFETZgwwb+uzp07+/+9aNEi/fSnP1X37t1VXFyss88+W/v27dPHH3+sX/7yl/rHP/6hZcuWKSUlpdVqWb16tX784x+rS5cuuuCCC3TgwAEtX75ct912m/7zn//ojTfeCGnqrFmzRjfccIPy8/N12mmnaciQITpw4IA+/fRTzZkzR2+88YZWrVqlvLw8SfJ/0H/33Xe1Z88eXXTRRerSpYt/fcXFxTFzPHTokC6//HItX75cGRkZGjJkiPLz8/XFF1/o6aef1vz58/Xee+/pjDPOCHuuy+XSxIkT9dFHH+ncc89V3759tXr1ar355ptatmyZSktL/U3EwYMHa/r06XrppZckhd/7LCMjQ5J0//33a9asWXI4HBo5cqS6d+8up9Opb7/9Vi+88IL69++vgQMHxqxr+vTp+vzzz7VmzRoNGjRIgwcP9j82atQo/7+3bNmi888/X1u3blV+fr4mTpwol8ulZcuW6Re/+IX+8pe/aMmSJTrhhBNivmZjU6ZM0cKFCzVmzBgNHDhQq1ev1vz58/XOO+9o8eLFGjFiRMjyO3fu1IQJE/TFF18oNzdXw4YNU2Zmpj777DM9/PDDmj9/vpYvX66TTjoprtd/6aWXNHPmTEnS8OHDNXbsWNXU1Gj79u16/fXX1blzZ5177rkhz7nzzjv16KOPymazaejQoRo9erS+/fZb/eMf/9DChQv13HPP+dfZGnk7nU6NHDlS3377rUaPHq0BAwZo5cqVevnll/XBBx9ozZo1ys7Obs7bDgDAscMEAAAJtWzZMlOS2fi0XFtba5500kmmJPNHP/qRWV9f73/s66+/Nk8++WRTknnPPfdEXN+YMWOivub69evNlStXhsUrKirM8ePHm5LM3/3ud2GP+/IpKyuLu77p06f767vppptMl8vlf2zdunVmfn6+Kcl8+umnQ563bds2c8mSJabH4wmJV1dXm9ddd51/fY2NGTPGlGQuW7Ysak6R3m/TNM3vfe97piTz0ksvNffs2RPy2O9//3tTknnKKaeYbrfbHw/efmeccYa5a9cu/2M1NTXmRRddZEoyb7jhhrjzMM2G7Z+WlmZmZGSYGzduDHv8m2++MTds2BC1xsZmzZplSjJnzZoVdZmzzjrLlGRefvnlZlVVlT++d+9e88wzzzQlmd/73vfifs2ysjJ/jZ07dzbXrFnjf8ztdpu33HKLKck86aSTzNraWv9jXq/XPOecc0xJ5vXXX29WVlb6H3O5XOYdd9xhSjLHjh0bdy69evUyJZkrVqwIe2zPnj3mZ599FhJ79tlnTUlmcXFxSN6maZoffPCBmZmZaSYnJ5ubNm1qcd4vvvii/3266KKLTKfT6X+soqLCHDx4sCnJnDNnTtz1AgBwrKGBBQBAgkVrYL3yyiumJLNbt24hH+59FixYYEoyMzMzzZqamrD1NdXAasp///tfU5I5bNiwsMda0sDq2rVrSJ4+f/rTn/yNoXhVV1ebDofDzM/PD3vsaBtY69evNw3DMLt16xbSeAg2ceJEU5K5cOFCf8z3fhuGYX7++edhz1m1apUpySwqKoorD5+9e/eaksyBAwdGraM5YjWwVqxYYUoyO3XqZO7evTvs8ZKSElOSabPZzG3btsX1msENrMcffzzs8draWrN79+6mJPO1117zx9955x1Tkjl48OCQhqePx+MxBwwYYEoyv/jii7hy6dSpk5mdnR3Xsh6Px+zWrZspySwpKYm4zO9+9ztTknnHHXe0OG9fAys9Pd3cuXNn2PNef/11U5J5/vnnx5U/AADHIu6BBQCARS1fvlySNHXq1Ihf5bvyyit1wgkn6NChQ/r000+bvX6Px6OlS5fqgQce0E033aSZM2dqxowZevDBByVJ//3vf1uUf2NXX321UlNTw+K+r89t3rxZO3fuDHv8o48+0kMPPaSf/OQn/hxvuukmJScna9++fTpw4ECr5Pf222/LNE1dfPHFyszMjLjMeeed58+psZ49e2rQoEFh8b59+0pSs+9hlJ+fr5NPPllr167VHXfcofXr1zfr+c3l298mTJigE088MezxIUOGaNCgQfJ6vf77jDVH469JSlJKSoqmTJkS8vqS9K9//UuSdNVVV8nhCL/jhc1m83/dL9K2iGT48OFyOp267rrr9Omnn8rr9UZdtrS0VDt37lTv3r01ZMiQiMtE2hdamvfQoUPVtWvXsPjR7kMAABxLuAcWAAAW5fuw2qtXr4iPG4ahXr166cCBA83+YLt582ZdccUV+vLLL6MuU1lZ2ax1xhKtjszMTOXl5Wn//v3avn27unXrJknau3evrrrqKv3nP/9pcr2VlZVHdU+mxrZs2SJJeuGFF/TCCy80uey+ffvCYj179oy4bFZWliSprq6u2Tm9/PLLmjRpkh577DE99thjys3N1VlnnaULL7xQ1157bch9zVoq1v4mSb1799aaNWuavb/l5OQoJycn4mO+19u+fbs/5tsWv/71r/XrX/+6yXVH2haRPPnkk7r00kv1yiuv6JVXXlFmZqaGDRum888/X9dee23I9vO9/tdffx31Zv+RXr+lecfah1rzjysAANDR0MACAOA4NGnSJH355Ze69NJLddddd6lfv37KyspSUlKS6uvrW/Xm7c1hmqb/3z/84Q/1n//8RyNGjNDs2bM1aNAgnXDCCUpKSpIkdevWTbt27Qp5Tkv4ZuQMHjw44kyqYGeddVZYzGZr/Ynto0eP1jfffKN//etf+uCDD/TRRx9p0aJFeueddzRr1iy9+eabuuCCC1r9dRMheDv6tsWoUaPUu3fvJp/Xv3//uNbft29f/fe//9XixYv1/vvv66OPPtKKFSv0/vvv6/7779cLL7ygadOmhbx+ly5ddNFFFzW53uAmYkvzbot9CACAYwUNLAAALKp79+6SArM6IikrKwtZNh4bN27U2rVrVVBQoDfffDPsq06bN28+imxj8+Xa2KFDh7R//35JUo8ePSRJ1dXVevvtt2Wz2fT222+Hzd6prq7W7t27WzW/wsJCSdI555yjJ554olXX3RJpaWmaNGmSJk2aJKlh5s6vfvUrPfvss/rBD36grVu3tsrrxLO/+R5rzv4mSQcPHtTBgwcjzsL65ptvJAW2vRTYFt/5znd05513Nuu1muJwODRx4kRNnDhRUsPsvccee0yzZ8/WjTfeqCuuuELp6en+18/Ly9O8efPiXn9b5Q0AACR+zQMAgEX57rHzl7/8JeJXh958800dOHBAmZmZIffpSU5OliS53e6I662oqJDUMIMp0n16Xn311ZamHtH8+fMjfo3ulVdekSQVFxf7GyNOp1Mej0dZWVkRmx6vvvpq1JlXseqP5uKLL5YkvfXWW+32VS3fbLLm5Jqfn6/f/e53kqRvv/027nuAxXpffPvbu+++qz179oQ9Xlpaqs8//zzkPk7N4dvOwerr6/WXv/wl5PWlwLaYP39+q82wiyQrK0v33XefcnJydPjwYW3atEmSNGzYMHXu3Fnr169v8mu2jbVX3gAAHI9oYAEAYFGTJ09Wz549tXPnTt1+++0hjYeysjLdcccdkqRbbrkl5ObovpksmzdvlsvlClvvqaeeKrvdri+++CLkxtmStHDhQv3+979vg2qknTt36s4775TH4/HHNmzYoPvvv1+S9LOf/cwfP/HEE3XCCSfo4MGDYY2PVatW6e677476Or76m9N4kKQzzjhDV111lbZt26Yrr7zSPzMoWHV1tV577bWIDZ6j0VSuW7du1fPPPx/xXmQLFy6UJJ1wwgn++yO15LWkhq+9nXXWWaqpqdGNN96ow4cP+x8rLy/XjTfeKKnhjwr4Zho1xwMPPKB169b5f/Z6vfrFL36h7du3q7CwUFdddZX/se985zsaNmyYVq9erZkzZ0a8X9SBAwf09NNPx9X8O3z4sB577LGI61mxYoUOHjwou93uf4+SkpI0a9YsmaapK664IuJ92Dwej95//32tWrWqzfIGAABBEvcHEAEAgGma5rJly0xJZqTT8urVq83c3FxTknnSSSeZU6ZMMSdOnGimpqaaksyLLrrIrKurC3ve0KFDTUnmaaedZn7/+983r7/+evMXv/iF//Gf/vSnpiTTZrOZY8aMMa+55hrzzDPPNCWZv/rVr6Lmc9JJJ5mSzLKysrjrmz59uinJ/NGPfmSmpqaavXr1MqdOnWpedNFFZnJysinJvOKKK0yv1xvyvN///vf+PM466yzzmmuuMc855xzTMAzz2muvjZrLP//5T1OSmZycbF566aXmD37wA/P66683P/zwQ/8y0eqrrKw0L7jgAv/zhw0bZl599dXm5MmTzWHDhvnz3bBhg/85vu03ZsyYqO9BtNe78847TUlm586dzauvvtq8/vrrzeuvv94sLy83S0tLTUlmUlKSP4+rr77aPOOMM0xJpmEY5vPPPx/nVjDN3bt3m+np6aYk85xzzjFnzJhhXn/99eb/+3//z7/M119/7X9fCwoKzEmTJpnf+c53zKysLFOSeeaZZ5oVFRVxv2ZZWZkpyezZs6d5xRVXmElJSeaFF15oTp061ezdu7cpyUxPTzdXrFgR9twdO3aYgwcP9i8zcuRIc+rUqeaVV15pDh482LTb7aYks6amJmYeBw4c8O/vgwYNMidNmmRec8015ogRI0zDMExJ5m9+85uw5/385z/3b7v+/fub3/nOd8ypU6ea5513npmTk2NKMp966qkW5/3iiy+akszp06c3+T6edNJJMWsFAOBYRQMLAIAEa6qBZZqm+e2335o/+clPzKKiIjM5OdnMzMw0R4wYYT711FOmy+WK+JytW7ea3/ve98yuXbuaDocj7MOv1+s1X3jhBXPIkCFmRkaGmZ2dbY4aNcp8/fXXTdOM3nBpSQPrxRdfND/77DPzsssuM/Py8syUlBSzf//+5mOPPRa1jr///e/myJEjzZycHDMjI8McOnSo+eSTT5per7fJXJ577jnzzDPPNDt16uSv5cUXX/Q/3tT77fF4zD//+c/mxIkTzRNPPNFMSkoy8/LyzAEDBpgzZ84033zzTbO+vt6/fEsaWDU1NeZdd91lFhcX+5tjvpoqKyvNxx9/3LziiivMU045xczIyDDT09PNU0891bzuuuvMkpKSqK8Xzb///W9z3Lhx5gknnGDabLaITZP9+/ebd999t9m3b18zNTXV7NSpk3nGGWeYv/3tb83Dhw836/WCGy8ul8t88MEHzT59+pgpKSlmbm6uedVVV5lffvll1OfX1taaTz/9tDl27FgzLy/PdDgcZkFBgTl48GDzJz/5iblo0aK48nC5XObTTz9tXnPNNWafPn3M7OxsMy0tzezdu7d51VVXmUuXLo363A8//ND8/ve/b5500klmSkqKmZmZaZ566qnmd7/7XfP555+P2NBrbt40sAAAiM0wTb6gDwAA2s6MGTP00ksv6cUXX9SMGTMSnQ4AAAA6IO6BBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS+MeWAAAAAAAALA0ZmABAAAAAADA0mhgAQAAAAAAwNIciU7gaHi9Xu3cuVOZmZkyDCPR6QAAAAAAAKAJpmnq0KFD6tatm2y25s+n6pANrJ07d6qwsDDRaQAAAAAAAKAZtm3bph49ejT7eR2ygZWZmSmpoeisrKwEZwMAAAAAAICmVFZWqrCw0N/Taa4O2cDyfW0wKyuLBhYAAAAAAEAHcbS3guIm7gAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsLQ2aWA9+OCDMgxDAwYMCHvso48+0qhRo9SpUyd16dJFt956q6qqqtoiDQAAAAAAABwDWv0m7tu3b9ecOXOUnp4e9tjnn3+uCy64QH379tVjjz2m7du365FHHtHmzZv1zjvvtHYqAAAAAAAAOAa0egPrzjvv1Nlnny2Px6Py8vKQx+655x6dcMIJWr58uf+vB5588sn6n//5Hy1evFjjx49v7XQAAAAAAEArMU1THo9Hbrc70anAIhwOh+x2+1H/dcG4X6c1V/bvf/9bCxYsUGlpqW655ZaQxyorK/Xee+/pZz/7mb95JUnXXXedfvazn+mNN96ggQUAAAAAgAWZpqmDBw9q37598ng8iU4HFmO321VQUKDs7Ow2a2S1WgPL4/Holltu0Q9/+EOdfvrpYY9/8cUXcrvdGjp0aEg8OTlZgwcPVmlpaWulAgAAAAAAWtHu3bt18OBBZWVlKSsrSw6Ho81n3MD6TNOU2+1WZWWldu3apZqaGnXt2rVNXqvVGlhPP/20tm7dqiVLlkR8fNeuXZIUsZCuXbtqxYoVUdddV1enuro6/8+VlZWSJLfb7Z+2aLPZZLPZ5PV65fV6/cv64h6PR6Zpxoz7pr01ng5pt9slKazTHC3ucDj8Uyt9DMOQ3W4PyzFanJqoiZqoiZqoiZqoiZqoiZqoiZqoKdE1eTweHTx4UPn5+crLy1NjhmGEvF6i481htdw7ak0ZGRlKSUnRvn37lJub69+Hgve9ln7ttFUaWPv379dvfvMb/frXv1Z+fn7EZWpqaiRJKSkpYY+lpqb6H49k7ty5mj17dli8tLTUf7P4/Px89e7dW2VlZdq3b59/mR49eqhHjx7atGmTnE6nP15UVKSCggKtW7cu5LX79OmjnJwclZaWhgzigQMHKjk5WSUlJSE5DB06VPX19Vq7dq0/ZrfbNWzYMDmdTm3cuNEfT0tL06BBg1ReXq4tW7b449nZ2erbt6927typ7du3++PURE3URE3URE3URE3URE3URE3URE1WqCk1NVXp6enyeDyqra31x202mzp16iS32x0y8cRutystLU0ul0v19fX+uMPhUGpqqurq6kIaGsnJyUpOTlZtbW1IjikpKUpKSlJNTU1IEy81NVUOh0OHDx8OaaakpaXJZrOpuro6pKb09HR5vd6Q98UwDGpqxZrS09O1Y8eOkG/YBe97vslIR8swW9rak/TjH/9YS5Ys0Zdffqnk5GRJ0nnnnafy8nKtW7dOkrRgwQJNnjxZ//73vzV69OiQ51999dVasWKFf5ZWY5FmYBUWFmr//v3++2lZpTPtcyx126mJmqiJmqiJmqiJmqiJmqiJmqjp+K2ptrZW3377rYqKiiJOSmG2EjVJDb2bLVu2qGfPnkpNTZUUuu9VVlYqLy9PTqcz5N7ocdfV0gbW5s2b1adPHz3++OO67LLL/PGpU6fqwIEDWrRokbKysrRhwwaNGjVKf/nLX3T11VeHrGP06NE6fPiwPv3007hes7KyUtnZ2UddNAAAAAAAiE9tba3KysrUq1cvf2MCaCzWftLSXo6tpQnu2LFDXq9Xt956q3r16uX/7+OPP9amTZvUq1cv3X///RowYIAcDkfY1MT6+np9/vnnGjx4cEtTAQAAAAAAQCuaMWOGTj755ESn0fIG1oABA/Tmm2+G/de/f3/17NlTb775pq6//nplZ2dr3LhxevXVV3Xo0CH/81955RVVVVVp8uTJLU0FAAAAAACgWebNmyfDMKL+t2rVqkSnGNP69et133336Ztvvkl0Km2mxTdx79y5s7773e+GxR9//HFJCnnswQcf1MiRIzVmzBjdcMMN2r59ux599FGNHz9eEyZMaGkqAAAAAAAAR+X+++9Xr169wuLFxcUJyKZ51q9fr9mzZ+u8886zxGypttAqf4UwXmeeeaaWLFmiX/ziF/rZz36mzMxMXX/99Zo7d257pgEAAAAAAFrJ4nWJzkAaP6Dl67j44os1dOjQlq8IbaLFXyGMZvny5f6/QBhs1KhR+vDDD1VTU6O9e/fqiSeeUGZmZlulAQAAAAAA0CKzZs2SzWbT0qVLQ+I33HCDkpOTtWbNGkkNvRDDMPSXv/xF99xzj7p06aL09HRdfvnl2rZtW9h6P/74Y02YMEHZ2dnq1KmTxowZow8//DBsuR07duj6669Xt27dlJKSol69eunHP/6x6uvrNW/ePP9tmcaOHev/6uPy5cv9z3/nnXc0evRopaenKzMzU5dccom+/PLLsNf5+9//rgEDBig1NdV/yyiraNcZWAAAAAAAAFbkdDpVXl4eEjMMQ3l5efrVr36lhQsX6vrrr9cXX3yhzMxMLVq0SM8995weeOABDRo0KOR5Dz74oAzD0C9+8Qvt3btXjz/+uMaNG6fPP/9caWlpkqT3339fF198sYYMGeJvkL344os6//zztWLFCg0fPlyStHPnTg0fPlwHDx7UDTfcoD59+mjHjh1asGCBDh8+rHPPPVe33nqr/vjHP+qee+5R3759Jcn//1deeUXTp0/XRRddpIceekiHDx/WU089pVGjRqm0tNT/lcPFixfrqquuUr9+/TR37lzt379fM2fOVI8ePdrybY+bYZqmmegkmqulf3oRAAAAAADEp7a2VmVlZerVq5dSU1PDHu/oXyGcN2+eZs6cGfGxlJQU1dbWSpLWrVunIUOG6LrrrtPDDz+sAQMGqGvXrlq5cqUcjob5QcuXL9fYsWPVvXt3bdiwwf+Ns/nz5+vqq6/WH/7wB916660yTVOnnXaaioqK9M4778gwDElSTU2N+vfvr+LiYi1evFiSNH36dL366qv6+OOPw77iaJqmDMPQggULNHnyZC1btkznnXee//GqqioVFhZq8uTJevbZZ/3xPXv26LTTTtPVV1/tj59xxhnas2ePNmzYoOzsbEnSe++9p/Hjx+ukk06KeYP4WPtJS3s5zMACAAAAAADHvf/7v//TqaeeGhKz2+3+fw8YMECzZ8/W3XffrbVr16q8vFyLFy/2N6+CXXfddSG3S5o0aZK6du2qt99+W7feeqs+//xzbd68Wb/61a+0f//+kOdecMEFeuWVV+T1eiU1fK3vsssui3h/Ll/jK5r33ntPBw8e1DXXXBMyu8xut+uss87SsmXLJEm7du3S559/rl/+8pf+5pUkXXjhherXr5+qq6ubfJ32QAMLAAAAAAAc94YPHx7zJu4///nP9frrr2v16tWaM2eO+vXrF3G5U045JeRnwzBUXFzsn8W0efNmSQ2zq6JxOp2qr69XZWWlBgw4uilmvtc5//zzIz7umwm1devWiHlL0mmnnabPPvvsqF6/NdHAQvN99VWiMwjoAH/OFAAAAABwbNiyZYu/KfTFF18c9Xp8s6sefvhhDR48OOIyGRkZqqioOOrXCH6dV155RV26dAl7PNLsMavqOJkCAAAAAAAkiNfr1YwZM5SVlaXbbrtNc+bM0aRJk3TllVeGLetrcvmYpqmvvvpKAwcOlCT17t1bUsMMqHHjxkV9zfz8fGVlZWnduqZvNBbtq4S+1ykoKGjydU466aSIeUvSf//73yZfu73YEp0AAAAAAACA1T322GP66KOP9Oyzz+qBBx7QyJEj9eMf/zjsLxdK0ssvv6xDhw75f16wYIF27dqliy++WJI0ZMgQ9e7dW4888oiqqqrCnr9v3z5Jks1m03e/+10tXLhQJSUlYcv5/i5fenq6JOngwYMhj1900UXKysrSnDlz5HK5or5O165dNXjwYL300ktyOp3+x9977z2tX7++yfelvTADCwAAAAAAHPfeeecdbdy4MSw+cuRI1dXV6de//rVmzJihyy67TFLDXy8cPHiwbrrpJr3xxhshz8nNzdWoUaM0c+ZM7dmzR48//riKi4v1P//zP5IaGlPPP/+8Lr74YvXv318zZ85U9+7dtWPHDi1btkxZWVlauHChJGnOnDlavHixxowZoxtuuEF9+/bVrl27NH/+fP3nP/9RTk6OBg8eLLvdroceekhOp1MpKSk6//zzVVBQoKeeekrXXnutzjzzTE2dOlX5+fn69ttv9a9//UvnnHOOnnjiCUnS3Llzdckll2jUqFH6wQ9+oIqKCv3pT39S//79IzbZ2hsNLAAAAAAAcNz7zW9+EzH+/PPP65lnnlHnzp31+OOP++OnnHKK5s6dq5/+9Kd64403dPXVV/sfu+eee7R27VrNnTtXhw4d0gUXXKAnn3xSnTp18i9z3nnnaeXKlXrggQf0xBNPqKqqSl26dNFZZ52lG2+80b9c9+7d9fHHH+vXv/61XnvtNVVWVqp79+66+OKL/evr0qWLnn76ac2dO1fXX3+9PB6Pli1bpoKCAn3ve99Tt27d9Nvf/lYPP/yw6urq1L17d40ePVozZ870v86ECRM0f/58/epXv9Ldd9+t3r1768UXX9Q//vEPLV++vJXe5aNnmL75Zh1IZWWlsrOz5XQ6/XfMRzviJu4AAAAAcNyora1VWVmZevXqpdTU1ESnY2nLly/X2LFjNX/+fE2aNCnR6bSrWPtJS3s53AMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWxk3cAQAAAAAAWsF5552nDnir8Q6BGVgAAAAAAACwNBpYAAAAAAAAsDS+QmgVX32V6AwaFBcnOgMAAAAAAIAQzMACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAADHrXnz5skwDKWmpmrHjh1hj5933nkaMGBAAjJDMEeiEwAAAAAAAB3Yu+8mOgNpwoQWr6Kurk6//e1v9ac//akVEkJrYwYWAAAAAAA47g0ePFjPPfecdu7cmehUEAENLAAAAAAAcNy755575PF49Nvf/rbJ5dxutx544AH17t1bKSkpOvnkk3XPPfeorq7Ov8ztt9+uvLw8mabpj91yyy0yDEN//OMf/bE9e/bIMAw99dRTrV/QMYYGFgAAAAAAOO716tVL1113XcxZWD/84Q/1m9/8RmeeeaZ+//vfa8yYMZo7d66mTp3qX2b06NGqqKjQl19+6Y+tWLFCNptNK1asCIlJ0rnnntsGFR1baGABAAAAAABIuvfee+V2u/XQQw9FfHzNmjV66aWX9MMf/lDz58/XTTfdpJdeekl33nmn/v73v2vZsmWSpFGjRkkKNKicTqe++OILXXXVVWENrNzcXPXr16+NK+v4aGABAAAAAABIKioq0rXXXqtnn31Wu3btCnv87bffltTwFcFgd9xxhyTpX//6lyQpPz9fffr00b///W9J0ocffii73a6f//zn2rNnjzZv3iypoYE1atQoGYbRZjUdK2hgAQAAAAAAHPGrX/1Kbrc74r2wtm7dKpvNpuLi4pB4ly5dlJOTo61bt/pjo0eP9s+2WrFihYYOHaqhQ4cqNzdXK1asUGVlpdasWaPRo0e3bUHHCBpYAAAAAAAARxQVFWnatGlRZ2FJimvG1KhRo7Rjxw5t2bJFK1as0OjRo2UYhkaNGqUVK1boo48+ktfrpYEVJxpYAAAAAAAAQXyzsBrfC+ukk06S1+v1fwXQZ8+ePTp48KBOOukkf8zXmHrvvff0ySef+H8+99xztWLFCq1YsULp6ekaMmRIG1dzbKCBBQAAAAAAEKR3796aNm2annnmGe3evdsfnzhxoiTp8ccfD1n+sccekyRdcskl/livXr3UvXt3/f73v5fL5dI555wjqaGx9fXXX2vBggU6++yz5XA42riaYwMNLAAAAAAAgEbuvfdeuVwu/fe///XHBg0apOnTp+vZZ5/VlClT9OSTT2rGjBn63e9+p+9+97saO3ZsyDpGjx6t//73vxowYIBOOOEESdKZZ56p9PR0bdq0ia8PNgMNLAAAAAAAgEaKi4s1bdq0sPjzzz+v2bNn65NPPtFtt92m999/X3fffbdef/31sGV9DapRo0b5Yw6HQyNGjAh5HLEZpmmaiU6iuSorK5WdnS2n06msrKxEp9M6vvoq0Rk0aPSXFCKySq5SfPkCAAAAAI5abW2tysrK1KtXL6WmpiY6HVhUrP2kpb0cZmABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSWtzA+vLLLzV58mQVFRWpU6dO6ty5s84991wtXLgwZLkZM2bIMIyw//r06dPSFAAAAAAAAHAMc7R0BVu3btWhQ4c0ffp0devWTYcPH9Zf//pXXX755XrmmWd0ww03+JdNSUnR888/H/L87OzslqYAAAAAAACAY1iLG1gTJ07UxIkTQ2I333yzhgwZosceeyykgeVwODRt2rSWviQAAAAAAECHYBiGZs2apfvuuy/RqXRobXIPLLvdrsLCQh08eDDsMY/Ho8rKyrZ4WQAAAAAAgLhFutVRpP+WL1+e6FSPey2egeVTXV2tmpoaOZ1OvfXWW3rnnXc0ZcqUkGUOHz6srKwsHT58WCeccIKuueYaPfTQQ8rIyGitNAAAAAAAQHv66qtEZyAVFx/V01555ZWQn19++WW99957YfG+ffsedWpoHa3WwLrjjjv0zDPPSJJsNpuuvPJKPfHEE/7Hu3btqrvuuktnnnmmvF6v3n33XT355JNas2aNli9fLocjeip1dXWqq6vz/+ybweV2u+V2u/2vabPZ5PV65fV6/cv64h6PR6Zpxozb7XYZhuFfb3BcaphBFk/c4XDINM2QuGEYstvtYTkahiG7JK9pyhuc45E8vV6vvEHrthmGbIYhj9crM464/UjH2O0NXktDXJI8Qa8ptzt2TcG5S7LbbGG5R4u3ek3tvZ0ixDv8vkdN1ERN1ERN1ERN1ERN1ERN1NRE3O12+9cXvF5//tHihtF+8QiPx2PatGkh6165cqXee++9sHjDS5hHlaPvucGPN3c9zdGu73sjpmmG9GqC973G+19ztVoD67bbbtOkSZO0c+dOvfHGG/J4PKqvr/c/Pnfu3JDlp06dqlNPPVX33nuvFixYoKlTp0Zd99y5czV79uyweGlpqdLT0yVJ+fn56t27t8rKyrRv3z7/Mj169FCPHj20adMmOZ1Of7yoqEgFBQVat26dampq/PE+ffooJydHpaWlIYN44MCBSk5OVklJSUgOQ4cOVX19vdauXeuP2e12DRs2TE6nUxs3bvTH09LSNGjQIJWXl2vLli3+eHZ2tvomJWmn06ntQTnmZ2Sod16eyg4c0L6qqkBN2dnqkZOjTeXlcgblXpSXp4KMDK3bvVs1LlegpoIC5aSlqXTHjpDm08CuXZXscKhk27ZAQRUVsWsKWj4tKUmDunVTeXW1tuzfH6gpLU19Cwravqb23k59+2rnzp3avn17oKaOvu9REzVREzVREzVREzVREzVREzXFqCk1NVVSQ1OrtrbWH7fZbOokye3xyBXUA7DZ7UpNSZHb7ZYr6LOc3eFQSnKy6l0ueYIaGklJSUpKSlJdfb28QTkmJScryeFQbV2dzKDPs8kpKXLY7aqtrZVpmvJWV/vfY5vNpuojP/ukp6fL6/WGvC+GYSg9PT2kpuAmi9vtVl1dnaqrq/W///u/evPNN7Vv3z6ddNJJmj59um699VYZhiGHw6HU1FRVVlbq3nvv1euvv666ujqNGTNGTz/9tCTJ5XL5c9q9e7cee+wxLVmyRNu2bVNaWprGjBmjhx9+WMXFxTp8+LC2bNmigQMHau7cufr5z38eUtOqVat04YUX6rXXXtOUKVNi1uTfTp06+Wvybw+7XWlpaXK5XCE9HF9NdXV1Ie9JcnKykpOTVVtbG7IvpaSk+Otct26dPx6877X0dlKG2dLWXhTjx4/XwYMH9fHHH/s7jo3V1NQoIyNDM2fODPvrhMEizcAqLCzU/v37lZWVJck6nWmfZnfby8qsMQOrqCh2TZs3B3JXgmdgnXxyaE3H8W9FqImaqImaqImaqImaqImaqIma2qKm2tpaffvttyoqKvI3KoIZX3+d+BlYR/kVwsbrvvnmm/Xkk0/6Z0yZpqkLL7xQy5Yt0w9+8AOdccYZWrRokRYuXKif/vSn+v3vf+9fz7XXXqtXX31V3/ve9zRixAgtW7ZMX331ldauXavf/OY3uu/ITdwXLFigBx98UJdffrl69Oihb775Rk8//bSysrK0fv16paWlSZJGjx6t2tpaffLJJyE5/+QnP9Grr76qXbt2qVOnTq37PrYgXldXpy1btqhnz57+hmfwvldZWam8vDw5nU5/L6c52qyB9eyzz+rGG2/Uxo0bddppp0VdrqCgQKNGjdLf/va3uNddWVmp7Ozsoy7akqzwnWEpvkFvlVyloz5IAQAAAADiU1tbq7KyMvXq1cvfmAhhhc+IrfTZ8Oabb9b//d//+Rs0//jHP/Td735X//u//6t7773Xv9zkyZP117/+VZs3b1bv3r21Zs0aDR48WDfddJP+7//+z7/c97//ff35z38O+SuENTU1/iaVz6pVqzRixAi9/PLLuvbaayUF+iobNmxQnz59JDXMcOrWrZsuueQSzZs3r1Vqbi2x9pOW9nLa5K8QSvJPYQueztjYoUOHVF5ervz8/LZKAwAAAAAA4Ki8/fbbstvtuvXWW0Pid9xxh0zT1DvvvONfTlLYcrfddlvYOoObVy6XS/v371dxcbFycnL02Wef+R+7+uqrlZqaqtdee80fW7RokcrLyzVt2rQW19bRtLiBtXfv3rCYy+XSyy+/rLS0NPXr10+1tbU6dOhQ2HIPPPCATNPUhAkTWpoGAAAAAABAq9q6dau6deumzMzMkLjvrxJu3brV/3+bzabevXuHLBfpG2k1NTX6zW9+o8LCQqWkpKhz587Kz8/XwYMHQyYB5eTk6LLLLtOf//xnf+y1115T9+7ddf7557dajR1Fi2/ifuONN6qyslLnnnuuunfvrt27d+u1117Txo0b9eijjyojI0PffPONzjjjDF1zzTX+aW+LFi3S22+/rQkTJug73/lOiwsBAAAAAACwultuuUUvvviibrvtNo0YMULZ2dkyDENTp04NudeZJF133XWaP3++PvroI51++ul66623dNNNN8lma7Mv1FlWixtYU6ZM0QsvvKCnnnpK+/fvV2ZmpoYMGaKHHnpIl19+uaSGruGll16q9957Ty+99JI8Ho+Ki4s1Z84c3XnnncflGw8AAAAAAKztpJNO0pIlS3To0KGQWVi+vy550kkn+f/v9Xr19ddfh8y6+u9//xu2zgULFmj69Ol69NFH/bHa2lodPHgwbNkJEyYoPz9fr732ms466ywdPnzYf4+s402LG1hTp07V1KlTm1wmJydHr7zySktfCgAAAAAAoN1MnDhRzz77rJ544gndfffd/vjvf/97GYahiy++WJJ08cUX65577tEf//jHkJu4P/7442HrtNvtYX/F709/+lPYX4OUGv6a5TXXXKM///nP2rBhg04//XQNHDiwlarrWFrcwAIAAAAAADgWXXbZZRo7dqzuvfdeffPNNxo0aJAWL16sf/zjH7rtttv897waPHiwrrnmGj355JNyOp0aOXKkli5dqq8i/IXGSy+9VK+88oqys7PVr18/rVy5UkuWLFFeXl7EHK677jr98Y9/1LJly/TQQw+1ab1WRgMLAAAAAAAgApvNprfeeku/+c1v9Je//EUvvviiTj75ZD388MO64447Qpb9f//v//m/7vf3v/9d559/vv71r3+psLAwZLk//OEPstvteu2111RbW6tzzjlHS5Ys0UUXXRQxhyFDhqh///7asGGDvv/977dZrVZnmI3nrXUAlZWVys7OltPpVFZWVqLTaR0RurIJUVwcexmr5CrFly8AAAAA4KjV1taqrKxMvXr1UmpqaqLTOS6dccYZys3N1dKlSxOdSlSx9pOW9nK4ezoAAAAAAIBFlZSU6PPPP9d1112X6FQSiq8QAgAAAAAAWMy6dev06aef6tFHH1XXrl01ZcqURKeUUMzAAgAAAAAAsJgFCxZo5syZcrlc+v/+v//vuP/6Jg0sAAAAAAAAi7nvvvvk9Xq1YcMGjRkzJtHpJBwNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAQk2maiU4BFtbW+wcNLAAAAAAAEJXdbpckuVyuBGcCK/PtH779pbXRwAIAAAAAAFElJSUpJSVFTqeTWViIyDRNOZ1OpaSkKCkpqU1ew9EmawUAAAAAAMeMzp07a8eOHdq+fbuys7OVlJQkwzASnRYSzDRNuVwuOZ1OVVVVqXv37m32WjSwAAAAgA5g8bpEZxAwfkDsZTpavgCalpWVJUkqLy/Xjh07EpwNrCYlJUXdu3f37ydtgQYWAAAAAACIKSsrS1lZWXK5XPJ4PIlOBxZht9vb7GuDwWhgAQAAAACAuCUlJbVLwwIIxk3cAQAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaY5EJwC0ua++SnQGDYqLE50BAAAAAAAdEjOwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaY5EJwAAAAAAibR4XaIzCBg/INEZAIA1MQMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlsZN3AEAAIAOIHPHV4lOIWBAcaIzAAAcZ2hgAQAA4LjFX58DAKBj4CuEAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsLQWN7C+/PJLTZ48WUVFRerUqZM6d+6sc889VwsXLgxbdsOGDZowYYIyMjKUm5ura6+9Vvv27WtpCgAAAAAAADiGtfivEG7dulWHDh3S9OnT1a1bNx0+fFh//etfdfnll+uZZ57RDTfcIEnavn27zj33XGVnZ2vOnDmqqqrSI488oi+++EKrV69WcnJyi4sBAAAAAADAsafFDayJEydq4sSJIbGbb75ZQ4YM0WOPPeZvYM2ZM0fV1dX69NNP1bNnT0nS8OHDdeGFF2revHn+5QAAAAAAAIBgbXIPLLvdrsLCQh08eNAf++tf/6pLL73U37ySpHHjxunUU0/VG2+80RZpAAAAAAAA4BjQ4hlYPtXV1aqpqZHT6dRbb72ld955R1OmTJEk7dixQ3v37tXQoUPDnjd8+HC9/fbbrZUGAAAAAAAAjjGt1sC644479Mwzz0iSbDabrrzySj3xxBOSpF27dkmSunbtGva8rl27qqKiQnV1dUpJSYm47rq6OtXV1fl/rqyslCS53W653W7/a9psNnm9Xnm9Xv+yvrjH45FpmjHjdrtdhmH41xsclySPxxNX3OFwyDTNkLhhGLLb7WE5GoYhuySvacobnOORPL1er7xB67YZhmyGIY/XKzOOuN0wGmryBq+lIS5JnqDXlNsdu6bg3CXZbbaw3KPFW72meLaT1xu5VkkOm62hpjhyb3FNjfZVy+x7EeIdfjxREzVREzVREzXFWZMZfPI2GnKXGZp7tLhha6gpNG7IsNllml41WnnkuGGTYdhkml653U3XZJrehvUYxpF/K3T9UeJHko8r3pCLGTPudrtjbqeotXo9oeuPGm/YTqY3dN872u3U1L4XSDP2dmrrmoKHWkcbT8GOlWMENVETNbVeTY3raq5Wa2DddtttmjRpknbu3Kk33nhDHo9H9fX1kqSamhpJitigSk1N9S8TrYE1d+5czZ49OyxeWlqq9PR0SVJ+fr569+6tsrKykL9s2KNHD/Xo0UObNm2S0+n0x4uKilRQUKB169b585OkPn36KCcnR6WlpSEbe+DAgUpOTlZJSUlIDkOHDlV9fb3Wrl3rj9ntdg0bNkxOp1MbN270x9PS0jRo0CCVl5dry5Yt/nh2drb6JiVpp9Op7UE55mdkqHdensoOHNC+qqpATdnZ6pGTo03l5XIG5V6Ul6eCjAyt271bNS5XoKaCAuWkpal0x46Q5tPArl2V7HCoZNu2QEEVFbFrClo+LSlJg7p1U3l1tbbs3x+oKS1NfQsK2r6meLZTdbWGFhaq3u3W2iPNVKmhGTWssFDO2lpt3Lu37WuqqGioyWr7Xt++2rlzp7Zv3x6oqaOPJ2qiJmqiJmqipjhrqj8YqCmp80AZ9mTV7wmtKfnEoTI99XKVB2oyDLuSuwyTWe+UqyJQk+FIU3L+IHlryuV2BmqypWQrKbevPFU75akK1GRPy5cjp7c8zjKVlDRdk9NVrTR7nlLsGapy75bHDFwbpTsKlGSkqdK1Q2bQr9Qyk7rKJoecrqDrPUnZSYXyyq1DrsC1kSGbspML5TZrVe0OXBvZjSRlJnVTvbdaNZ6Ga6OSkoqY28njLJOnJlCTPaOHHJk95D64Sd66wHZyZBfJ3qlArv3rZLoD2ykpt4+MlBy59pbKNFu2nWLte/WH4t9ObV1TyeFATR1tPB2LxwhqoiZqar2afJORjpZhBrfGWtH48eN18OBBffzxx/r00081bNgwvfzyy7r22mtDlrvrrrv08MMPq7a2tlkzsAoLC7V//35lZWVJOgY6nmVl1piBVVQUu6bNmwO5K8EzsE4+ObSmSLlv2WKNGVhFRQ1xq+17/AaBmqiJmqiJmo7jmpauD0oywTOwLujbdE2rl2yRVWZgDR9XFHM7LfrCOjOwLuzf9L4X2A8SPwPrgn6BcEcbT8GOlWMENVETNbVeTZWVlcrLy5PT6fT3cpqj1WZgNTZp0iTdeOON2rRpk/+rg7uCZr/47Nq1S7m5uVGbV1LDzK1IjzscDjkcoSX43rTGfBs23njj9R5N3DCMiPFoOfoaHhGXj/Ca9gjraCruiBYPfs2gfKPW1Jzc27qmeLZH0HMdEXIxDCNivNVrapSrpfa9ZsY7xHiiJmqKkmNz49RETRI1RcuxuXEr1mREOnkbUS6RI8QNw4gStynSypuKOxxN12QEPc+ImHj0eKBhFTtuGEbMePB2jLY9otZqi7w9osfj3x7R4rH2vcZpNnv7tWJNkYZURxlPLY1TEzVJ1BQtx+bGrVhTtPzj1SZ/hVAKfG3Q6XSqe/fuys/PD5vuJkmrV6/W4MGD2yoNAAAAAAAAdHAtbmDtDbp3kI/L5dLLL7+stLQ09evXMAf2qquu0j//+U9tC7p/0tKlS7Vp0yZNnjy5pWkAAAAAAADgGNXirxDeeOONqqys1Lnnnqvu3btr9+7deu2117Rx40Y9+uijysjIkCTdc889mj9/vsaOHauf/vSnqqqq0sMPP6zTTz9dM2fObHEhAAAAAAAAODa1uIE1ZcoUvfDCC3rqqae0f/9+ZWZmasiQIXrooYd0+eWX+5crLCzUBx98oNtvv12//OUvlZycrEsuuUSPPvpok/e/AgAAAAAAwPGtxQ2sqVOnaurUqXEt279/fy1atKilLwkAAAAAAIDjSJvdxB0AAAAAAABoDTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaS2+iTsAAADQUWXu+CrRKQQMKE50Bq2K9xYA0JpoYAEAAABAB7J4XaIzCBg/INEZADhe8BVCAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWJoj0QkACPLVV4nOIKC4ONEZAAAAAAAgiQYWAAAAWtHidYnOIGD8gERnAAAAWgtfIQQAAAAAAICl0cACAAAAAACApfEVQgAAAABAm+BrxQBaCzOwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpLW5gffLJJ7r55pvVv39/paenq2fPnrr66qu1adOmkOVmzJghwzDC/uvTp09LUwAAAAAAAMAxzNHSFTz00EP68MMPNXnyZA0cOFC7d+/WE088oTPPPFOrVq3SgAED/MumpKTo+eefD3l+dnZ2S1MAAAAAAADAMazFDazbb79df/7zn5WcnOyPTZkyRaeffrp++9vf6tVXXw28mMOhadOmtfQlAQAAAAAAcBxp8VcIR44cGdK8kqRTTjlF/fv314YNG8KW93g8qqysbOnLAgAAAAAA4DjRJjdxN01Te/bsUefOnUPihw8fVlZWlrKzs5Wbm6uf/OQnqqqqaosUAAAAAAAAcIxo8VcII3nttde0Y8cO3X///f5Y165dddddd+nMM8+U1+vVu+++qyeffFJr1qzR8uXL5XBET6Wurk51dXX+n30zuNxut9xutyTJZrPJZrPJ6/XK6/X6l/XFPR6PTNOMGbfb7TIMw7/e4LjUMIMsnrjD4ZBpmiFxwzBkt9vDcjQMQ3ZJXtOUNzjHI3l6vV55g9ZtMwzZDEMer1dmHHH7kRvmu73Ba2mIS5In6DXldseuKTh3SXabLSz3aPFWryme7eT1Rq5VksNma6gpjtxbXFOjfTXivifFt52aiLdaTVLHHU8R4h3+GEFN1ERN1NRBajJN+5F/hMYNW0NNoXFDhs0u0/RKpjd23LDJMGzR416PFHTF4PXGrsls9LpHkleoyPGGXMxWintD3uNI26Mh14ZroNC81WS8LWpyu90x973m5NgeNTU1ngIv0Tr7XvR4w75nekPHk4zAuAkeatHGmdT+4yla3DSbPkY0LB+51pBwOxwjOJZTEzUltqbGdTVXqzewNm7cqJ/85CcaMWKEpk+f7o/PnTs3ZLmpU6fq1FNP1b333qsFCxZo6tSpUdc5d+5czZ49OyxeWlqq9PR0SVJ+fr569+6tsrIy7du3z79Mjx491KNHD23atElOp9MfLyoqUkFBgdatW6eamhp/vE+fPsrJyVFpaWnIxh44cKCSk5NVUlISksPQoUNVX1+vtWvX+mN2u13Dhg2T0+nUxo0b/fG0tDQNGjRI5eXl2rJliz+enZ2tvklJ2ul0antQjvkZGeqdl6eyAwe0L2imWo/sbPXIydGm8nI5g3IvystTQUaG1u3erRqXK1BTQYFy0tJUumNHSPNpYNeuSnY4VLJtW6CgiorYNQUtn5aUpEHduqm8ulpb9u8P1JSWpr4FBW1fUzzbqbpaQwsLVe92a+2uXYGabDYNKyyUs7ZWG/fubfuaKioaampq35Pi205S29ckddzx1Levdu7cqe3btwdq6ujHCGqiJmqipg5SkzoNlempl6s8UJNh2JXcZZjMeqdcFYGaDEeakvMHyVtTLrczUJMtJVtJuX3lqdopT1WgJntavhw5veVxlslTE6jJntFDjswech/cJG9doKbyLrFrcroCt7bITOoqmxxyukLPudlJhfLKrUOuwDnXkE3ZyYVym7WqdgfOuXYjSZlJ3VTvrVaNJ3DOdRhpykgqUJ3XqVpPIMdkW4Y6OfJU4zkQ8l5G2k5OV7XS7HlKsWeoyr1bHjNwbZTuKFCSkaZK1w6ZQb9Sa6uaSkoqYu57NZ4DqvcGro1S7dlKteeo2l0utxnYHu1RU6zxVH+oId5a+54ju0j2TgVy7V8n0x2oNSm3j4yUHLn2lsoMatQkdR4ow56s+j0lKjkcqCnaMUJp7T+eotXk7Nn0MaJ+T+gxIvnExB0j4jnu7TvUsJ1sKTmq3x19O8Vbk7cuck2ew5Frch8K1JSfyfmJmo6tmlp6OynDDG6NtdDu3bt1zjnnyOVyadWqVerWrVuTy9fU1CgjI0MzZ84M++uEwSLNwCosLNT+/fuVlZUl6RjoeJaVWWMGVlFR7Jo2bw7krgTPwDr55NCaIuW+ZYs1ZmAVFTXEm9r3vv7aOjOwTj21444nfitCTdRETdSUsJqWbrDODKwLB8SuafWSwEV8omdgDR9X5I9F2h4NuVpjBtbwcUUx972P3t0Ud45tXdPZ43s3OZ6Wrg96zQTPwLqgXyAcbZy9v9E6M7DGn970MWLxF9aZgXVB39jHvaXrFdd2ao+aLujH+Ymajq2aKisrlZeXJ6fT6e/lNEerzcByOp26+OKLdfDgQa1YsSJm80pq6ADm5eWp4sjMlGhSUlKUkpISFnc4HGFfPfS9aY35Nmy88WhfaWxO3DCMiPFoOfoaHhGXj/Ca9gjraCruiBYPfs2gfKPW1Jzc27qmeLZH0HMdEXIxDCNivNVrapRr1H0vnu0UI96qNXXU8dTMODVRU7Q4NVGTRE3RcowU959OjMg1RY7bJCM8x2bHbaG5+8puqiYjwnoCjZDYccMwWilui/geB+cenGvkvKPHW7um4Fyj7WPNzbGta2pqPDV+iZbue7HjUT6GGY7Gl4ySoh8j2nM8RYv7xny0Y0RTtYbn0rY1xXPcC35ac3KPFm9JTaEfaTg/UVPHr6mpW0fFo1UaWLW1tbrsssu0adMmLVmyRP369Yv9JEmHDh1SeXm58vPzWyMNAAAAAAAAHINa3MDyeDyaMmWKVq5cqX/84x8aMWJE2DK1tbVyuVzKzMwMiT/wwAMyTVMTJkxoaRoAAAAAAAA4RrW4gXXHHXforbfe0mWXXaaKigq9+uqrIY9PmzZNu3fv1hlnnKFrrrlGffr0kSQtWrRIb7/9tiZMmKDvfOc7LU0DAAAAAAAAx6gWN7A+//xzSdLChQu1cOHCsMenTZumnJwcXXrppXrvvff00ksvyePxqLi4WHPmzNGdd94Z8fuUAAAAAAAAgNQKDazly5fHXCYnJ0evvPJKS18KAAAAAAAAxyGmPgEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSWnwTdwAAAMAnc8dXiU4hYEBxojMAAACthBlYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0/gohAAAAAAAdzOJ1ic4gYPyARGeA4wEzsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaY5EJwAAAICmLV6X6AwCxg9IdAYAAOB4xAwsAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYmiPRCQAAAAAAgGPb4nWJziBg/IBEZ4CjwQwsAAAAAAAAWBozsAAcva++SnQGDYqLE50BAMk6xwQp9nGhI+UqKXOHhfIdwDEXxx7GGABYHzOwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpjkQnAAAAAAAAYBWL1yU6g4DxAxKdgXUwAwsAAAAAAACWRgMLAAAAAAAAlsZXCAEcH776KtEZBBQXJzqD41tH2hc6Uq4AAABAG6KBZRErv050Bg1G8PkEAAAAAABYDF8hBAAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApXEPLDSbVe7XJXHPLgAAAAAAjgctnoH1ySef6Oabb1b//v2Vnp6unj176uqrr9amTZvClt2wYYMmTJigjIwM5ebm6tprr9W+fftamgIAAAAAAACOYS2egfXQQw/pww8/1OTJkzVw4EDt3r1bTzzxhM4880ytWrVKAwYMkCRt375d5557rrKzszVnzhxVVVXpkUce0RdffKHVq1crOTm5xcUAAAAAAADg2NPiBtbtt9+uP//5zyENqClTpuj000/Xb3/7W7366quSpDlz5qi6ulqffvqpevbsKUkaPny4LrzwQs2bN0833HBDS1MBAAAAAADAMajFXyEcOXJk2OypU045Rf3799eGDRv8sb/+9a+69NJL/c0rSRo3bpxOPfVUvfHGGy1NAwAAAAAAAMeoNvkrhKZpas+ePercubMkaceOHdq7d6+GDh0atuzw4cNVWlraFmkAAAAAAADgGNAmf4Xwtdde044dO3T//fdLknbt2iVJ6tq1a9iyXbt2VUVFherq6pSSkhJxfXV1daqrq/P/XFlZKUlyu91yu92SJJvNJpvNJq/XK6/X61/WF/d4PDJNM2bcbrfLMAz/eoPjkuTxeOKKOxwOmaYZEjcMQ3a7PSxHwzAk6UgeZsh6DMMm0/QqlCHDMFol3iDwmm63O2ZNjdfTkGO03Nu2pri2k9cr+5H32GOG5uKwNeQYHDck2W02eU1T3jjiNimw7wWt22YYshmGPF5vwzvQaF+NuO9JcntDa42We5vXJMUeT0ceC6s1KEfDMNq+pqD9INo4s3m98W2nGPFWqcntbvYxImJNHfy4l7CaGu1LUjuMp2j73pH3MWpNQe9Bu42nOMZZ1O1kmu0/nqLV5PE0ve8d7bG8LWpqNG6k8PHkOw8m8pzri/vGVbRjQWB/bk6ObVOT98ixv6ljROhzwq+Nmoq3dk3uCOMsOPeGXFt+vdcaNbnd7pjH8va8ho2npqbOT8Gv0Z7jKVLuwftBtHEmNRwjZAbHDRk2e8O6G+3XEeOGLVBTpLjXE/oeRImbZtPXEQ3LB6djP/LE0Lhha/ua4rmOaBhmDTWZ3tCaouXeVjW53U1fG0nxb6e2rkmKfb3nL7eV9r2W1BS8u0a6hjW9iRlPkWpyu4+d6/LGx4nmavUG1saNG/WTn/xEI0aM0PTp0yVJNTU1khSxQZWamupfJloDa+7cuZo9e3ZYvLS0VOnp6ZKk/Px89e7dW2VlZSF/2bBHjx7q0aOHNm3aJKfT6Y8XFRWpoKBA69at8+cnSX369FFOTo5KS0tDNvbAgQOVnJyskpKSkByGDh2q+vp6rV271h+z2+0aNmyYnE6nNm7c6I+npaVp0KBBKi8v15YtW/zx7OxsSUmq8zpV6wnkmGzLUCdHnmo8B1TvrQq8Z/ZspdpzVO0ul9sM5J5mz1OKPUNV7t3ymC5/PN1RoCQjTZWuHTKDLsszk7rKJoecrm3+WElJRcyagpe3G0nKTOqmem+1ajz7/XGHkaaMpII2rymu7VRdraGFhap3u7X2SDNVavhQNqywUM7aWm3cuzfwmklJGtStm8qrq7Vlf6Cm7LQ09S0o0E6nU9uD9qX8jAz1zstT2YED2lcVqKlHdrZ65ORoU3m5nDU1UkWFpBj7nqTSHTvkCTpADOzaVckOh0q2Bd53SW1fkxR7PFVXN9SUl6eCjAyt271bNa7AdupTUKCctLS2ryloe2dnZ6tv377auXOntm/fHqjJMOLbTke0aU1OZ7OPERFr6uDHvYTVZJrtP56i7XtS0zWVlwdqaq/xFK2moP0g6nZyONp/PEWrqaam6X3vaI/lbVFTTU3M8eR0VSf8nOu7jigpaTifRTtGSLnyyq1DrsB2MmRTdnKh3Gatqt2B7dTWNZWX58Q8Rjhdlf54pGsjScpOKmyXmoLfy0jHPaerulWu91qjppKSipjH8va8ho1VU6zzk9NVHfd2auuafGNMin7OVdowmfVOuSoCNRmONCXnD5K3plxuZ+C4Z0vJVlJuX3mqdspTFdhO9rR8OXJ6y+Msk6cmcCy3Z/SQI7OH3Ac3yVsXeA8c2UWydyqQa/86me5Arc6eTV9H1O8JPUYknzhUpqdervJATYZhV3KXtq8pnuuI+kNSUm4fGSk5cu0tlRnUBEnqPFCGvf1qKjnc9LWRFP92auuapNjXe/WH4ttO7VFTyeEjrxnlGtZVk5jxFKmmksPHznW5bzLS0TJM02z8q4ujtnv3bp1zzjlyuVxatWqVunXrJkkqKSnRsGHD9PLLL+vaa68Nec5dd92lhx9+WLW1tc2agVVYWKj9+/crKytLUsefibB6SZklZmANH1cUs6aVizZHyDExvw0edsHJIdGIuW/ZYo0ZWEVFDfGm9r2vv7bODKxTT409no4c+BI+A6tXr0A82m8QtmyxzgysoiLL/lYkJPdj5Dc9Ybl/9ZV1ZmCdckrTNX39dUiOCZ2BFTTOom6nsjLrzMDq3bvpfW/zZuvMwCoujjmeVi/ZciT/xM/AGj6u4XwW7ViweknZkX8lfgbW2eOLYx4jfO+tbz2Rcm+vGVi+91aKfHxryNUaM7CGjyuKeSz/6N1NcefY1jWdPb53k+en4P0g0TOwgveDaOPs/Y3WmYE1/vSmryMWf2GdGVgX9I19HbF0vSwzA+uCfk1fGy1Zb50ZWBcNjH29t3R9oxwTOAPrgn6BcKRr2KXrrTMD64J+x851eWVlpfLy8uR0Ov29nOZotRlYTqdTF198sQ4ePKgVK1b4m1dS4KuDu4J+Y+qza9cu5ebmRm1eSQ0ztyI97nA45HCEluB70xrzbdh4443XezRxwzAixqPl2PBVQiNCPPKtylorHvyawflGqynSeqLn3rY1xbU9gt5rhxE5x0hx34eTuOM2W8Sbytl9r98o16j7XoR9Q4qce7R4q9bU1Hhq9Jg9Wu5tXVM84+zIv2NupzjjLarpSL7NPUY0N94RjnsJqSnKviQl6BjRVE0R3oOEHSPi2a5Hntuu48n/0o1qOvK+Rt3HjvZYHme8WTVFGTfB4yn4PJioc64v3jjXxj8b/hqbk2Pb1OTb9k0dIyKvK/K+19Y1RdoPgnMP3Q+O/novVjye3INzjX5t237XsLHisc5PjV8jkdflkfKMdoyQESlukyJerzczbos8bhrHfUM+2vWCYYvykTNi7m1bUzzXEcFPa07u0eItqSn0I02UcRbndgrE266mWNd1jctt6b4XiDe/psa7a+NjhC+t9h5PgXjw53IF/btjX5dHyz9erdLAqq2t1WWXXaZNmzZpyZIl6tevX8jj3bt3V35+foQp5tLq1as1ePDg1kgDAAAAAAAAx6AW/xVCj8ejKVOmaOXKlZo/f75GjBgRcbmrrrpK//znP7Ut6N4PS5cu1aZNmzR58uSWpgEAAAAAAIBjVItnYN1xxx166623dNlll6miokKvvvpqyOPTpk2TJN1zzz2aP3++xo4dq5/+9KeqqqrSww8/rNNPP10zZ85saRoAAAAAAAA4RrW4gfX5559LkhYuXKiFCxeGPe5rYBUWFuqDDz7Q7bffrl/+8pdKTk7WJZdcokcffbTJ+18BLbXy69jLtIcRxYnOAAAAAACAjqnFDazly5fHvWz//v21aNGilr4kAAAAAAAAjiOt9lcIAQAAOgqrzM6VmKELAAAQjxbfxB0AAAAAAABoSzSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGmORCcAIGDl14nOIGBEcaIzANDRcAwDAABAW6GBBQBW9NVXic4goJhOAAAAODqZOyx0TTOAaxqgI+MrhAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwtFZpYFVVVWnWrFmaMGGCcnNzZRiG5s2bF7bcjBkzZBhG2H99+vRpjTQAAAAAAABwDHK0xkrKy8t1//33q2fPnho0aJCWL18eddmUlBQ9//zzIbHs7OzWSAMAAAAAAADHoFZpYHXt2lW7du1Sly5dVFJSomHDhkV/QYdD06ZNa42XBQAAAAAAwHGgVb5CmJKSoi5dusS9vMfjUWVlZWu8NAAAAAAAAI5xrTIDqzkOHz6srKwsHT58WCeccIKuueYaPfTQQ8rIyGjvVAAAsLSVXyc6g4ARxYnOAAAAAMezdm1gde3aVXfddZfOPPNMeb1evfvuu3ryySe1Zs0aLV++XA5H5HTq6upUV1fn/9k3e8vtdsvtdkuSbDabbDabvF6vvF6vf1lf3OPxyDTNmHG73S7DMPzrDY5LDbPH4ok7HA6ZphkSNwxDdrs9LEfDMCTpSB5myHoMwybT9CpUw83vWyPeIPCabrc7Zk2N19OQY7Tc27ameLZTw3PDaz363I+upsb7aqR9L5Bv6Hoi5d7WNUmKPZ6OPGYzDNkMQx6vN2Qt9iN/qMHtDa3JfmSf95hmXHGHrSHH4LghyW6zyWua8gbtB9HGmc3rDRwjgtYdLfc2rcntbt4xIrjW4OOY1D41xXk8bO5xL+J2ao9jeaN9KaTW5u57ccSb3E5H3sfoNQU/I/5jeVPxoz1GBL+X0baTaZptdn5qbk0ej6fJfc8K51xfvPG4kcLHk299iTznNj6fRTsWBPbnxJ1zfbxHjv1NHSMaj7NIubfXdUSkcRacu++apr3HU6S42+2OeSxPxHhqqqamzk/Br9Ge4ylS7sH7QbRxJjUcI2QGxw0ZNnvDuhufPyLFDVugpkhxryf0PYgSN82mPz/Fu/3a4xgRz3VEwzBrqMn0uhutxn4kdU9cccPWsu3kdjd9bSTFv53auiYp9vWev9xW2vdaUlPw7hrpGtb0JmY8RarJ7W77fkR7XZc3Pk40V7s2sObOnRvy89SpU3Xqqafq3nvv1YIFCzR16tSoz5s9e3ZYvLS0VOnp6ZKk/Px89e7dW2VlZdq3b59/mR49eqhHjx7atGmTnE6nP15UVKSCggKtW7dONTU1/nifPn2Uk5Oj0tLSkI09cOBAJScnq6SkJCSHoUOHqr6+XmvXrvXH7Ha7hg0bJqfTqY0bN/rjaWlpGjRokMrLy7VlyxZ/vOEm9kmq8zpV6wnkmGzLUCdHnmo8B1TvrfLHU+3ZSrXnqNpdLrcZyD3NnqcUe4aq3LvlMV3+eLqjQElGmipdO2QGfXzKTOoqmxxyurb5YyUlFTFrCl7ebiQpM6mb6r3VqvHs98cdRpoykgravKZ4tpPTVa3spEJ55dYh1y5/3JBN2cmFcpu1qnbvbfOaSkoqJDW970mKaztJavOaJMUeT9XVDTXl5akgI0Prdu9WjSuwnfoUFCgnLU2lO3bIE3TQG9i1q5IdDpVsC61paGGh6t1urd0VqMlus2lYYaGctbXauDdQU1pSkgZ166by6mptCdre2dnZ6tu3r3bu3Knt27f74/mGod55eSo7cED7qgLbqUd2tnrk5GhTebmcQdujTWtyOmMfI4LWk52Wpr4FBdrpdGp70HEsPyOjfWqKddyrrg5sp5qayNupqkpb9gf2PX9NBw9Grmn//sg17d0buaadOxtqOnJOaPJYbpqtt+9Fqqk520lq8vzkdJX74805lkutf4wI3g+inXPrvI42Oz81t6Z162qinnP79u1riXOur6aampqY1xFOV3XCz7m+mnzns2jXRlJuws+5PuXlOTGv95yuwG0tEnXO9dUU/F5GuoZ1uqoTMp4i1VRSUhH9nHvkGJGI8RStpljX5U5Xddzbqa1r8o0xKfpnDaUNk1nvlKsiUJPhSFNy/iB5a8rldgaOe7aUbCXl9pWnaqc8VYHtZE/LlyOntzzOMnlqAsdye0YPOTJ7yH1wk7x1gffAkV0ke6cCufavk+kO1Ors2fTnp0SNp0jbKZ7PhPWHpKTcPjJScuTaWyozqAmS1HmgDHuy6veEHveSTxwq01MvV3lgOxmGXcldWradSg43/TlXin87tXVNUvRzru8YUX+oId5a+15Laio5fOQ1o3x2d9UkZjxFqqnkcNv3I5o6lrdmj6Wlt5IyzODWWCvw3cT9xRdf1IwZM2IuX1NTo4yMDM2cOTPsrxP6RJqBVVhYqP379ysrK0tSx5+BtXpJmSV+Gzx8XFHMmlYu2hwhx8T8NnjYBSeHRCPlvnrJloi1Hn3uR1fT8HFFkpre91Yt/toyM7BGTjg19ng6cuBL+AysXr2C6onyG4QtW6wzA6uoKPYx4quvIteaiBlYQe+vFGGcHdkP2ny2Ujw1FRX5c4x6LP/qK+vMwDrllCbPTx+/F/wdwsTOwBo+LrAfRDvnrl5SZpkZWGdd2LvJ3zJ+9O7mKOtp/xkjIy4qjnkd0XAuS+w5t/H5LNr1wuolZRFrTcQMrLPHF8e83vO9t771RMq9va4jfO+tFPl6wXdNY4UZWMPHFcX8rf1H726KO8e2runs8b2bvC4P3g8SPQMreD+INs7e32idGVjjT2/681Pjzw6JvC4fPq5XzM+ES9erRTN7QsItnIF1Qb+mP+cuWW+dGVgXDYw9s2fp+kY5JnAG1gX9AuFI1+VL11tnBtYF/Y6dGViVlZXKy8uT0+n093Kao93vgdVYWlqa8vLyVFFREXWZlJQUpaSkhMUdDkfY1w59b1pjvg0bbzza1xmbEzcMI2I8Wo4NXyU0IsQj32u/teLBrxmcb7SaIq0neu5tW1M82yP0uc3JsXVrapxrtH0vnu0UK95aNcUcT40es0dYVmpoAkSMG5FrihQ3DCNi3GYYssUzzo7822azRfzrFdFyb5OajuTb3GOEr1kTcfkIr9lqNcUaZ0HPa3I7NSd+tDU1yjVi7lFylI5i32uNmpo4P0U+3ibmGBHPvur7SnxbnJ9ixRvn7ntfrXzODc4l1nVE8PoSdc6Ndj5r/LPh3/8Td8718W37pq73Iq+r/c+5hmGLuB8E5x66H7TfeIoUD841+jhr//EULR7rONb4NRJ5jIiUZ7RjhIxIcZsU7fzRnLgtyrVqo7hvyEe7Xmju8bAtjxHxfCYMfqphi/JxOcL7Hi3eku0U/JZGHWdxbqd</t>
         </is>
       </c>
     </row>
@@ -546,29 +546,29 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45656.95833333334</v>
+        <v>45657.875</v>
       </c>
       <c r="E3" t="n">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>31.22667878170933</v>
+        <v>32.42225622321715</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>45656.95833333334</v>
+        <v>45657.875</v>
       </c>
       <c r="H3" t="n">
-        <v>16.63721923752225</v>
+        <v>18.60852756012034</v>
       </c>
       <c r="I3" t="n">
-        <v>2.515352174341909</v>
+        <v>3.731138366033831</v>
       </c>
       <c r="J3" t="n">
-        <v>31.22667878170933</v>
+        <v>32.42225622321715</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACHNUlEQVR4nOzdeXhTZfrG8TttupcWKFQKLUspmyAgsgiyiwgoKJvgxiKOu7j91AHHcRkFHRBxGR0ZZ0AFR1ncUFFBQRERRFFAQUCWYYdSaGnpnvf3ByQ0JGlTuuQUvp/r8prhzUlyP8lZkqfvObEZY4wAAAAAAAAAiwoKdAAAAAAAAACgODSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAKIVRo0bJZrNp5MiRfi3//PPPy2az6fzzz6/gZCXr2bOnbDabli1bFpDnHzNmjGw2m2bNmhWQ5y8vgX4dzyUNGzaUzWbTjh07Ah0FAAAEGA0sAABKYdy4cZKkDz74QEeOHClx+ZkzZ7rdr6I8/vjjstlsevzxxyv0ec52Vel1rMxG2rJly2Sz2dSzZ88Kfy4AAABvaGABAFAK3bt3V0pKinJzczVnzpxil/3hhx+0fv16hYSE6MYbb6ykhL69+eab2rhxozp27BjoKFUaryMAAEDlo4EFAEAp2Gw23XTTTZJOza7yxXn7lVdeqfj4+ArPVpL69eurefPmioyMDHSUKo3XEQAAoPLRwAIAoJTGjBmj4OBg/fTTT1q3bp3XZXJycvTf//5Xkufpgz/++KOuv/561a9fX2FhYapZs6Yuv/xyffrpp14fq+h1gD788EP17t1bNWvWdJ0+ZrPZ9MQTT0iSnnjiCdlsNtd/Y8aMcT1OSaecffXVVxo+fLgSExMVFham2rVrq0OHDnrsscd0+PBh13L5+fmaPXu2rr/+ejVv3lwxMTGKiIhQs2bNNH78eO3du9ffl7JEs2bNctVx+PBh3Xnnna7XrUGDBrrvvvt8nsr53nvv6eabb1arVq1Uo0YNhYeHq1GjRrrpppv0+++/eyxfXq/jl19+qSFDhighIUGhoaGKj4/X4MGDtXLlSq/LO59DkhYsWKCuXbsqJiZGUVFRuuSSSzzWC+d7/vXXX0uSevXq5Za16DXGfvzxR40YMUKJiYkKDQ1VTEyMkpOTNXToUH344Yde85yuZ8+e6tWrlyTp66+/dnuuhg0bui1bUFCgf/7zn+rSpYtiY2MVHh6uJk2aaPz48dqzZ49fz+fL+++/73ptqlWrpp49e/rcZpzmz5+vfv36qXbt2goNDVW9evV0ww036Lfffiv182/ZskU33XSTGjVqpLCwMEVHR6tBgwa64oorfDazN2/erFtvvVWNGzdWeHi4YmNj1b17d82ePbvccu/YscP1XhhjNGPGDF100UWKiopSbGys+vbt63PdAwCgSjEAAKDUBg4caCSZ8ePHe719zpw5RpKpW7euKSgocI1Pnz7dBAUFGUmmbdu2ZtiwYaZr164mNDTUSDJPPPGEx2M1aNDASDJ33XWXkWTat29vrr32WtOjRw/zzTffmNGjR5s2bdoYSaZNmzZm9OjRrv/+9a9/uR6nR48eRpJZunSpx3PcfffdRpIr18iRI03//v1NcnKyx3127dplJJnY2Fhz8cUXm+HDh5sBAwaYunXrGkmmdu3aZsuWLR7PMXr0aCPJzJw50+/XeebMmUaSGTRokGncuLGpXr26ufrqq83gwYNNjRo1jCTTrFkzc/DgQY/7BgcHm8jISNO+fXszZMgQM2jQIFc9UVFRZsWKFR75yvo6PvDAA0aSCQoKMh07djTDhw83nTp1MjabzQQHB5v//Oc/Hvdxvu5//etfjc1mM5dccokZMWKEK4vNZjPvvfeea/mNGzea0aNHm/POO89IMpdffrlb1uXLlxtjjFmyZIkJCQlx1TNs2DAzePBg07FjRxMWFmauuuoqv96DyZMnm8svv9xIMuedd57bcz3wwAOu5XJyckyfPn2MJBMeHm769+9vRowYYZKSkowkU6tWLfPjjz/69ZxOznX/vvvuc1v3O3bs6HrdXnzxRY/75efnm2uuucZIMmFhYaZLly5m+PDhrtc0IiLCLFq0yO8c69evNzExMa71bciQIWb48OGmc+fOJjo62rRp08bjPnPnzjXh4eFGkmnevLkZPHiw6d27t4mKijKSzNixY8sl9/bt240k06BBAzN69GgTEhJievfuba655hrTtGlT12N9//33ftcLAIAV0cACAOAMfPDBB0aSiYuLM7m5uR63O7/IT5w40TX22WefGZvNZmrVqmW+/vprt+XXrVtnEhMTjSSzbNkyt9ucX+KDg4PNhx9+6DXPY489ZiSZxx57zGdmX42XF1980VXLV1995XG/VatWmf/973+uf2dkZJgPP/zQo+68vDwzYcIEI8kMGDDA43HK0sCSZC6++GJz+PBh121HjhwxXbp0MZLMyJEjPe77zjvvmMzMTLcxh8Nh/vGPfxhJpmXLlsbhcLjdXpbXccaMGUaSSUlJMb/88ovbbV9//bWpVq2aCQ0NNZs3b3a7zVlf9erVPZoMzjxNmzb1O4dTr169jCQze/Zsj9uOHj1qVq5c6bPG0y1dutRIMj169PC5zMMPP2wkmcaNG5vt27e7xvPy8sy4ceOMJNOoUSOv24svznXfZrN51PHOO+8Ym81m7Ha7Wb9+vdttEydONJJMp06dzLZt29xumzdvngkODjY1atQwR44c8SvH2LFjjSTz1FNPedx2/Phxr9tzWFiYCQ8PNwsWLHC7bceOHeaCCy4wkswbb7xR5tzOBpazifX777+7bisoKDA33XSTkWT69u3rV60AAFgVDSwAAM5Afn6+qVOnjpFk5s2b53bbzp07XbOsis5E6tSpk5Fk5s+f7/Ux586daySZoUOHuo07v8TfdNNNPvOcaeMlPz/f1K5d20jy+KJ9purWrWuCgoJMRkaG23hZG1hr1671uH3dunXGZrOZoKAgs2vXLr8ft3PnzkaS+fXXX93Gz/R1LCwsdM1AW7Nmjdf7/f3vfzeS3GYtGXOqgeVtJlFOTo6JjY01ktyaiL5yFHX++ecbSSYtLc1nLf4qqYGVnZ1toqOjjSTz0UcfedyelZXlmjE2Z84cv5/Xue5fffXVXm8fOnSokWT+9Kc/ucYOHz5sIiIiTHh4uNm9e7fX+91xxx1GknnppZf8yjFgwAAjyfz0009+LT9ixAgjyUydOtXr7atXrzaSzEUXXVTm3EUbWN5e+3379rlmYeXl5fmVHwAAK+IaWAAAnAG73a7Ro0dLkv7zn/+43TZz5kw5HA716NFDKSkpkqTU1FStXr1aERERGjhwoNfH7NmzpyTpu+++83r7sGHDyin9KT/++KMOHTqkWrVqafDgwaW67y+//KJp06bp7rvv1k033aQxY8ZozJgxKigokMPh0NatW8stZ5s2bdS2bVuP8QsuuEAXXnihHA6HvvnmG4/bt27dqpdffln33nuvxo0b58p44MABSfJ6LawzsXbtWu3du1eNGzfWRRdd5HWZkt5fb+tFWFiYkpOTJanU15By/kri9ddfr2+//VYFBQWlun9prFmzRpmZmapZs6bXOiIjIzVy5EhJ0tKlS0v9+M5tzdd40euRLV26VNnZ2brkkktUr149r/cr6b04nfO1vP322/X5558rJyfH57IOh0OLFi2SJI0YMcLrMu3bt1d0dLTWrl3reqyy5rbb7erXr5/HeJ06dVSjRg3l5ua6XcsOAICqxh7oAAAAVFU33XSTnn32WX3xxRfas2eP6tWrJ2OM6yLaRS/evn37dhljlJ2drbCwsGIf99ChQ17HT79gdnnYuXOnJKlZs2auC4mXJCsrSzfeeKPef//9YpfLyMgocz6nRo0aFXvbTz/9pN27d7vGCgsLddddd+m1116TMabCM27btk2S9Mcff5T4Ovp6f+vXr+91PCYmRpKKbZp4M3nyZK1bt06LFi3SokWLFBERoXbt2qlnz566/vrr1aJFi1I9XnGczbXi3qfGjRu7LVsavh7XOV70vXe+F19++eUZvxene/DBB/Xtt99qyZIl6tevn0JCQtSmTRt1795dI0eOVIcOHVzLHj582LVeJSUllfjYhw8fVr169cqcOyEhQSEhIV6Xj4mJ0ZEjR0q9DgEAYCU0sAAAOENNmzZVt27dtHz5cr355puaMGGCli5dqh07dig2NtZtxpTD4ZAkRUdHa+jQoWf0fBEREeWSu6wmTJig999/X82bN9czzzyjDh06qFatWgoNDZUkdenSRStXriy2cVQRij7fCy+8oH/+85+qU6eOpk2bpi5duui8885TeHi4JOm6667Tf//733LL6Hx/69Spo8svv7zYZWvVquV1PCiofCfG16lTR2vWrNHXX3+tJUuWaMWKFVq1apVWrFihSZMmafLkyXr44YfL9TkDpej76HwvUlJSdMkllxR7v+bNm/v1+JGRkVq8eLF++OEHffbZZ/ruu+/03Xffac2aNZo2bZruuOMO/eMf/3B7fsn3zLGinA3tsuYu7/UHAACroYEFAEAZjBs3TsuXL9fMmTM1YcIE1+mEI0eOdGs4OWdi2Gw2/ec//7HMl03nrJ/NmzfLGOPXLKy5c+dKkt599121bt3a4/YtW7aUb0idmMHmy44dOyRJiYmJrjFnxtdee02DBg3yuE95Z3S+v3Fxca4ZeFZgs9nUs2dP16lnOTk5mjVrlu68805NnDhRw4YNc82MKgvnKW/FvU/OGUa+To8rzvbt29WmTRuPcW/vvfO9aNasWbm/Fx06dHDNtiooKNAHH3ygUaNG6ZVXXtGwYcPUq1cv1apVSxEREcrOztbUqVN9NixPV5G5AQA4G1jj0zMAAFXU8OHDFRMToy1btujjjz/We++9J8n99EFJqlu3rlq3bq1jx47ps88+K/ccztlPpb3OUfv27VWrVi0dOnRIH3zwgV/3SUtLkyQ1aNDA47bPP/9cqamppcrgj3Xr1mndunUe47/++qt++uknBQUFqXv37n5l/PXXX/Xzzz97fZ4zfR2ds9B+++03/frrr6W675k6k6zh4eG67bbb1Lp1azkcDq+v6Zk8l/OaTmlpafroo488bs/OztY777wjSerVq5ffeZ3eeustr+NvvvmmpFPXhpKkSy+9VKGhoVq2bJkOHjxY6ufyl91u17Bhw1wz7pzrVHBwsC677DJJpxqp/qis3AAAVFU0sAAAKIPIyEhde+21kk5cEys7O1sXXHCB2zVxnJ566ilJ0tixY7Vw4UKP240xWrVqlb744otS53DOQClt88Rut+uRRx6RJN1yyy1eL4T+ww8/uF1jyHntpJdeesltud9//1233XZbqZ7fX8YY3X777Tpy5IhrLD09XbfffruMMRo6dKjb9YacGf/xj3+4ndK1b98+jRo1ymcj5kxfx5CQED322GMyxmjw4MH69ttvPZYpLCzUV199pe+//75Uj+1LSVmnTp2q//3vfx7jmzZtcs1A89bgK+65tmzZovz8fI/bw8PDdeedd0qSHnjgAde11SQpPz9f99xzj/bv369GjRqd0Y8RvP/++64GmNP8+fO1YMEC2e123X333a7x8847T3fffbeysrI0cOBArV+/3uPxcnNz9dFHH2nTpk1+Pf8rr7zi9YL/+/fv15o1ayS5v5aPPfaYQkND9eCDD+qNN95wWwedNmzY4Gp4V1RuAADOKoH58UMAAM4eq1evdv2MvSQzffp0n8u+8MILxm63G0kmJSXFXHHFFea6664zl112mYmPjzeSzMMPP+x2nwYNGhhJZvv27T4fd//+/SYqKspIMpdccokZM2aMGTdunPnPf/7jWqZHjx5Gklm6dKnbfR0Oh7nttttc+S+88EIzcuRIM2DAAJOcnOxxnwULFhibzWYkmQsuuMCMHDnS9O7d24SEhJjevXubLl26eH2e0aNHG0lm5syZJb2kLjNnzjSSzKBBg0xycrKpXr26GTx4sBkyZIipWbOmkWSaNGliDhw44Ha/77//3oSGhrpe52uuucb069fPREREmJYtW5rBgwd7zVKW19EYYx588EHX69iyZUtz1VVXmZEjR5qePXua6tWrG0nm1VdfdbuPc3lffD3fxx9/bCSZ0NBQc+WVV5qbbrrJjBs3zqxYscIYY0xsbKyRZJo3b24GDx5srrvuOtOzZ0/X+jdq1Cg/3oFT2rdvbySZZs2ameuvv96MGzfObV3Nyckxl156qZFkIiIizIABA8yIESNM/fr1jSQTFxdn1qxZU6rndK779957r5FkOnToYK677jrTqVMn1+s2bdo0j/vl5+eb6667zkgyQUFB5sILLzRDhw41I0aMMJdcconrPV60aJFfOdq0aWMkmUaNGpmBAwea66+/3vTt29dEREQYSaZ3794mPz/f7T5z5841kZGRRpJJTEw0ffv2Nddff73p37+/SUxMNJLMiBEjypx7+/btRpJp0KBBia9jcfsQAACsjgYWAADl4IILLnA1E1JTU4tddv369eaWW24xTZo0MeHh4SYyMtIkJyebyy+/3Lz44otmz549bsv7++Xzm2++MX369DE1atQwQUFBRpIZPXq06/biGi/GGLNo0SJz1VVXmfPOO8+EhISY2rVrm44dO5onnnjCHD582OO5Lr30UlOrVi0TGRlpWrVqZZ5++mmTm5vr83nK0sAaPXq0OXjwoLn11ltNYmKiCQ0NNUlJSWb8+PEe2ZzWrVtnBg0aZBISEkx4eLhp0qSJeeihh0xGRkaxWcr6Oq5YscJcf/31pkGDBiYsLMxUq1bNNG3a1Fx99dXm9ddfN2lpaW7Ln2kDyxhj/vWvf5l27dq5GiVFa5o9e7YZO3asadWqlalZs6YJCwszDRo0MP379zfvv/++cTgcPp/Tm507d5rrrrvOJCQkuJpgpzdN8vPzzSuvvGIuvvhiU61aNRMaGmoaN25s7r77brN79+5SPZ8x7uv+3LlzTefOnU10dLSJiooy3bp1MwsXLiz2/p9++qkZMmSIqVevngkJCTHVq1c3LVq0MCNHjjRvv/22ycrK8ivHxx9/bG6//XZz4YUXmtq1a5vQ0FCTmJhoevbsad544w2Tl5fn9X7bt2839913n2nVqpWJiooy4eHhpkGDBqZnz57mmWeeMVu3bi1zbhpYAIBzhc2YSv6JIAAAAD/NmjVLY8eO1ejRo7mwNQAAwDmMa2ABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSuAYWAAAAAAAALI0ZWAAAAAAAALA0GlgAAAAAAACwNHugA5wJh8OhvXv3qlq1arLZbIGOAwAAAAAAgGIYY3Ts2DHVrVtXQUGln09VJRtYe/fuVVJSUqBjAAAAAAAAoBR27dqlxMTEUt+vSjawqlWrJulE0TExMQFOAwAAAAAAgOJkZGQoKSnJ1dMprSrZwHKeNhgTE0MDCwAAAAAAoIo400tBcRF3AAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFhalfwVQgAAAAAAUPmMMSosLFRBQUGgo8Ai7Ha7goODz/jXBf1+ngp9dAAAAAAAUOUZY3T06FEdOnRIhYWFgY4DiwkODlZ8fLxiY2MrrJFFAwsAAAAAABRr//79Onr0qGJiYhQTEyO73V7hM25gfcYYFRQUKCMjQ/v27VN2drYSEhIq5LloYAEAAAAAAJ8KCwuVnp6u2rVrq1atWoGOAwuqVq2awsLClJqaqvj4eAUHB5f7c3ARdwAAAAAA4FN+fr6MMYqKigp0FFhYVFSUjDHKz8+vkMengQUAAAAAAErEKYMoTkWvHzSwAAAAAAAAYGk0sAAAAAAAAODVmDFj1LBhw0DHoIEFAAAAAADOXbNmzZLNZvP53/fffx/oiCX67bff9Pjjj2vHjh2BjlJh+BVCAAAAAABwznvyySfVqFEjj/GUlJQApCmd3377TU888YR69uxpidlSFYEGFgAAAAAAOGNfbAh0Aqlvq7I/Rv/+/dW+ffuyPxAqBKcQAgAAAAAAFOOxxx5TUFCQvvzyS7fxW265RaGhofrll18kScuWLZPNZtO7776riRMnqk6dOoqKitKgQYO0a9cuj8ddtWqV+vXrp9jYWEVGRqpHjx5asWKFx3J79uzRuHHjVLduXYWFhalRo0a6/fbblZeXp1mzZmn48OGSpF69erlOfVy2bJnr/osWLVK3bt0UFRWlatWq6YorrtCvv/7q8TwffPCBWrVqpfDwcLVq1Urvv/9+WV62csUMLAAAAAAAcM5LT09Xamqq25jNZlNcXJz+8pe/aOHChRo3bpzWr1+vatWq6fPPP9e//vUv/e1vf1ObNm3c7vf000/LZrPp4Ycf1sGDBzV9+nT16dNHP//8syIiIiRJX331lfr376+LLrrI1SCbOXOmevfureXLl6tjx46SpL1796pjx446evSobrnlFjVv3lx79uzR/Pnzdfz4cXXv3l3jx4/Xiy++qIkTJ6pFixaS5Prft956S6NHj9bll1+uZ599VsePH9err76qrl27au3ata5TDr/44gsNHTpU559/viZPnqzDhw9r7NixSkxMrMiX3W82Y4wJdIjSysjIUGxsrNLT0xUTExPoOAAAAAAAnLVycnK0fft2NWrUSOHh4R63V/VTCGfNmqWxY8d6vS0sLEw5OTmSpA0bNuiiiy7SqFGjNGXKFLVq1UoJCQlauXKl7PYT84OWLVumXr16qV69etq4caOqVasmSZo3b56uueYavfDCCxo/fryMMWrWrJmSk5O1aNEi2Ww2SVJ2drZatmyplJQUffHFF5Kk0aNHa/bs2Vq1apXHKY7GGNlsNs2fP1/Dhw/X0qVL1bNnT9ftmZmZSkpK0vDhwzVjxgzX+IEDB9SsWTNdc801rvELL7xQBw4c0MaNGxUbGytJWrx4sfr27asGDRqUeIH4ktaTsvZymIEFAAAAAADOef/4xz/UtGlTt7Hg4GDX/2/VqpWeeOIJTZgwQevWrVNqaqq++OILV/OqqFGjRrmaV5I0bNgwJSQk6NNPP9X48eP1888/a8uWLfrLX/6iw4cPu9330ksv1VtvvSWHwyHpxGl9AwcO9Hp9Lmfjy5fFixfr6NGjuvbaa91mlwUHB6tTp05aunSpJGnfvn36+eef9ec//9nVvJKkyy67TOeff76ysrKKfZ7KQAMLAAAAAACc8zp27FjiRdwffPBBvfPOO1q9erUmTZqk888/3+tyTZo0cfu3zWZTSkqKaxbTli1bJJ2YXeVLenq68vLylJGRoVatzmyKmfN5evfu7fV250yonTt3es0tSc2aNdNPP/10Rs9fnmhgAQAAADi3bd0a6ASnpKQEOgGAYmzbts3VFFq/fv0ZP45zdtWUKVPUtm1br8tER0crLS3tjJ+j6PO89dZbqlOnjsft3maPWVXVSQoAAAAAABAgDodDY8aMUUxMjO69915NmjRJw4YN05AhQzyWdTa5nIwx2rp1q1q3bi1Jaty4saQTM6D69Onj8zlr166tmJgYbdhQ/IXGfJ1K6Hye+Pj4Yp+nQYMGXnNL0u+//17sc1eWoEAHAAAAAAAAsLpp06bpu+++04wZM/S3v/1NXbp00e233+7xy4WS9Oabb+rYsWOuf8+fP1/79u1T//79JUkXXXSRGjdurKlTpyozM9Pj/ocOHZIkBQUF6eqrr9bChQu1Zs0aj+Wcv8sXFRUlSTp69Kjb7ZdffrliYmI0adIk5efn+3yehIQEtW3bVm+88YbS09Ndty9evFi//fZbsa9LZWEGFgAAAAAAOOctWrRImzZt8hjv0qWLcnNz9eijj2rMmDEaOHCgpBO/Xti2bVvdcccdmjt3rtt9atasqa5du2rs2LE6cOCApk+frpSUFP3pT3+SdKIx9frrr6t///5q2bKlxo4dq3r16mnPnj1aunSpYmJitHDhQknSpEmT9MUXX6hHjx665ZZb1KJFC+3bt0/z5s3Tt99+q+rVq6tt27YKDg7Ws88+q/T0dIWFhal3796Kj4/Xq6++qhtvvFHt2rXTyJEjVbt2bf3vf//TJ598oksuuUQvv/yyJGny5Mm64oor1LVrV910001KS0vTSy+9pJYtW3ptslU2GlgAAAAAAOCc99e//tXr+Ouvv67XXntNtWrV0vTp013jTZo00eTJk3XPPfdo7ty5uuaaa1y3TZw4UevWrdPkyZN17NgxXXrppXrllVcUGRnpWqZnz55auXKl/va3v+nll19WZmam6tSpo06dOunWW291LVevXj2tWrVKjz76qObMmaOMjAzVq1dP/fv3dz1enTp19M9//lOTJ0/WuHHjVFhYqKVLlyo+Pl7XXXed6tatq2eeeUZTpkxRbm6u6tWrp27dumns2LGu5+nXr5/mzZunv/zlL5owYYIaN26smTNn6sMPP9SyZcvK6VU+czbjnG9WhWRkZCg2Nlbp6emuK+YDAAAAwBnhIu5AsXJycrR9+3Y1atRI4eHhgY5jacuWLVOvXr00b948DRs2LNBxKlVJ60lZezlcAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJbGRdwBAAAAAADKQc+ePVUFLzVeJTADCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAnLNmzZolm82m8PBw7dmzx+P2nj17qlWrVgFIhqLsgQ4AAAAAAACqsM8+C3QCqV+/Mj9Ebm6unnnmGb300kvlEAjljRlYAAAAAADgnNe2bVv961//0t69ewMdBV7QwAIAAAAAAOe8iRMnqrCwUM8880yxyxUUFOhvf/ubGjdurLCwMDVs2FATJ05Ubm6ua5n7779fcXFxMsa4xu6++27ZbDa9+OKLrrEDBw7IZrPp1VdfLf+CzjI0sAAAAAAAwDmvUaNGGjVqVImzsG6++Wb99a9/Vbt27fT888+rR48emjx5skaOHOlaplu3bkpLS9Ovv/7qGlu+fLmCgoK0fPlytzFJ6t69ewVUdHahgQUAAAAAACDpkUceUUFBgZ599lmvt//yyy964403dPPNN2vevHm644479MYbb+j//u//9MEHH2jp0qWSpK5du0o61aBKT0/X+vXrNXToUI8GVs2aNXX++edXcGVVHw0sAAAAAAAAScnJybrxxhs1Y8YM7du3z+P2Tz/9VNKJUwSLeuCBByRJn3zyiSSpdu3aat68ub755htJ0ooVKxQcHKwHH3xQBw4c0JYtWySdaGB17dpVNputwmo6W9DAAgAAAAAAOOkvf/mLCgoKvF4La+fOnQoKClJKSorbeJ06dVS9enXt3LnTNdatWzfXbKvly5erffv2at++vWrWrKnly5crIyNDv/zyi7p161axBZ0laGABAAAAAACclJycrBtuuMHnLCxJfs2Y6tq1q/bs2aNt27Zp+fLl6tatm2w2m7p27arly5fru+++k8PhoIHlJxpYAAAAAAAARThnYZ1+LawGDRrI4XC4TgF0OnDggI4ePaoGDRq4xpyNqcWLF+uHH35w/bt79+5avny5li9frqioKF100UUVXM3ZgQYWAAAAAABAEY0bN9YNN9yg1157Tfv373eNDxgwQJI0ffp0t+WnTZsmSbriiitcY40aNVK9evX0/PPPKz8/X5dccomkE42tP/74Q/Pnz9fFF18su91ewdWcHWhgAQAAAAAAnOaRRx5Rfn6+fv/9d9dYmzZtNHr0aM2YMUMjRozQK6+8ojFjxujvf/+7rr76avXq1cvtMbp166bff/9drVq1Uo0aNSRJ7dq1U1RUlDZv3szpg6VAAwsAAAAAAOA0KSkpuuGGGzzGX3/9dT3xxBP64YcfdO+99+qrr77ShAkT9M4773gs62xQde3a1TVmt9vVuXNnt9tRMpsxxgQ6RGllZGQoNjZW6enpiomJCXQcAAAAAFXZ1q2BTnDKab9sBlhBTk6Otm/frkaNGik8PDzQcWBRJa0nZe3lMAMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAKCC2Gw2Pf7444GOUeXRwAIAAAAAAOckm83m13/Lli0LdNRznj3QAQAAAAAAQBW2dWugE0gpKWd0t7feesvt32+++aYWL17sMd6iRYszjobyQQMLAAAAAACck2644Qa3f3///fdavHixxzgCj1MIAQAAAAAAfMjKytIDDzygpKQkhYWFqVmzZpo6daqMMW7L5ebm6r777lPt2rVVrVo1DRo0SLt37/Z4vJ07d+qOO+5Qs2bNFBERobi4OA0fPlw7duxwLbNt2zbZbDY9//zzHvf/7rvvZLPZ9N///rfca7UyZmABAAAAQFVihdO1nM7wtC2gqjDGaNCgQVq6dKnGjRuntm3b6vPPP9eDDz6oPXv2uDWYbr75Zs2ePVvXXXedunTpoq+++kpXXHGFx2P+8MMP+u677zRy5EglJiZqx44devXVV9WzZ0/99ttvioyMVHJysi655BLNmTNH9913n9v958yZo2rVqumqq66q8PqthAYWAAAAAACAFx999JG++uorPfXUU3rkkUckSXfeeaeGDx+uF154QXfddZcaN26sX375RbNnz9Ydd9yhf/zjH67lrr/+eq1bt87tMa+44goNGzbMbWzgwIHq3LmzFixYoBtvvFGSNGrUKN16663atGmTmjdvLknKz8/X3LlzNWTIEEVGRlZ0+ZbCKYQAAAAAAABefPrppwoODtb48ePdxh944AEZY7Ro0SLXcpI8lrv33ns9HjMiIsL1//Pz83X48GGlpKSoevXq+umnn1y3XXPNNQoPD9ecOXNcY59//rlSU1PPyWt0lbmBtWzZMp8/M/n999+7Lfvdd9+pa9euioyMVJ06dTR+/HhlZmaWNQIAAAAAAEC527lzp+rWratq1aq5jTt/lXDnzp2u/w0KClLjxo3dlmvWrJnHY2ZnZ+uvf/2r65patWrVUu3atXX06FGlp6e7lqtevboGDhyot99+2zU2Z84c1atXT7179y63GquKcjuFcPz48erQoYPbWEqR86F//vlnXXrppWrRooWmTZum3bt3a+rUqdqyZYurYwkAAAAAAHA2u/vuuzVz5kzde++96ty5s2JjY2Wz2TRy5Eg5HA63ZUeNGqV58+bpu+++0wUXXKCPPvpId9xxh4KCzr0T6sqtgdWtWzePcziLmjhxomrUqKFly5YpJiZGktSwYUP96U9/0hdffKG+ffuWVxQAAAAAAIAya9CggZYsWaJjx465zcLatGmT63bn/zocDv3xxx9us65+//13j8ecP3++Ro8ereeee841lpOTo6NHj3os269fP9WuXVtz5sxRp06ddPz4cdc1ss415dqyO3bsmAoKCjzGMzIytHjxYt1www2u5pV0opMYHR2tuXPnlmcMAAAAAACAMhswYIAKCwv18ssvu40///zzstls6t+/vyS5/vfFF190W2769OkejxkcHCxjjNvYSy+9pMLCQo9l7Xa7rr32Ws2dO1ezZs3SBRdcoNatW5elpCqr3GZgjR07VpmZmQoODla3bt00ZcoUtW/fXpK0fv16FRQUuP7tFBoaqrZt22rt2rXlFQMAAAAAAKBcDBw4UL169dIjjzyiHTt2qE2bNvriiy/04Ycf6t5773Vd86pt27a69tpr9corryg9PV1dunTRl19+qa1bt3o85pVXXqm33npLsbGxOv/887Vy5UotWbJEcXFxXjOMGjVKL774opYuXapnn322Quu1sjI3sEJDQzV06FANGDBAtWrV0m+//aapU6eqW7du+u6773ThhRdq3759kqSEhASP+yckJGj58uXFPkdubq5yc3Nd/87IyJAkFRQUuGZ8BQUFKSgoSA6Hw+2cUed4YWGhW4fT13hwcLBsNpvHTLLg4GBJ8uiI+hq32+0yxriN22w2BQcHe2T0NU5N1ERN1ERN1ERN1ERN1ERNlVDTyZw2ScFBQXIYI0fRjCdzOhwOFb06TZDNpiCbTYUOh4wf48Enf+yq4LRr3ATbbCeyGyMVqddnTdKJmopk9JW9wmsyhnXvHKipoKDA9XinzxySTqxnXsdttsob93K7P05/7NP/v81m04cffqi//vWvmjt3rmbOnKmGDRvq73//u+uXCJ2P8+9//1u1atXS22+/rQ8++EC9e/fWJ598oqSkJBljXMtOnz5dwcHBmjNnjnJycnTJJZdo8eLF6tevn0cGSWrXrp1atmypjRs36rrrrvP6WhRXU2WNO7MX7dUUXfe8nbFXGjZTUuVnYOvWrWrdurW6d++uzz77TG+99ZZGjRqlVatWqWPHjm7Ljho1Sh999JHXcz2dHn/8cT3xxBMe40uWLFFUVJQkqXbt2mrcuLH++OMPHTp0yLVMYmKiEhMTtXHjRrer+ScnJys+Pl6//PKLsrOzXePNmzdX9erV9cMPP7htxK1bt1ZoaKjWrFnjlqF9+/bKy8vTunXrXGPBwcHq0KGDjh496jovVjrxU5lt2rTRwYMHtW3bNtd4bGysWrRood27d2v37t2ucWqiJmqiJmqiJmqiJmqiJmqqhJqysk7UFBGhFvHx2n30qHYXyVg7OlqN4+L0x+HDOlTkV9QTY2OVWL26Nh48qPQi2ZPj4hQfHa1f9u5Vdn7+qZri41U9IkI/7NqlwiLNiNYJCQq127Vm1y7p5PebYmuqUUNHs7O16eDBUzWFhKhN3bo6mJmpbYcPn3qfKrqmiy5i3TtHagoPD1fz5s1lt9uVk5PjGg8KClJkZKTy8/PdJp4EBwcrIiJCeXl5ysvLc43b7XaFh4crJyfHraERGhqq0NBQZWdnu2UMCwtTSEiIjh8/7tbECw8Pl91uV1ZWllszJSIiQkFBQco6uV07RUVFyeFwuL0uNptNUVFRKigosHxN7du3V2xsrD7++GPL1lRYWKjff//d57qXkZGhPn36KD093e3yUv6qkAaWJF177bV67733dPz4cb3//vsaPny4vvnmG3Xr1s1tuWuuuUbLly93zdLyxtsMrKSkJB0+fNhVtFU6005nU7edmqiJmqiJmqiJmqiJmqjprK7pZCPBEjOwkpNLrmnHDuvMwGrShHXvHKgpJydH//vf/5ScnKywsDCdLlAzfoqbCeQvq2X3Nr5mzRp17NhRM2fO1OjRo4utJ5DZc3NztW3bNtWvX1/h4eGS3Ne9jIwMxcXFnXEDq9yugXW6pKQk5eXlKSsry3XqoLcm1b59+1S3bt1iHyssLMzrRmK322W3u5fg3GBP59wA/R0//XHPZNxms3kd95WxtOPURE2+xqmJmiRq8pWxtOPURE0SNfnKWNpxaqImyaI1nZbT2azxuryX5wz2Umdx43Zf4zab5CWnz5q8ZfSVvaJqOvmYrHtnd012u122k++1zct6ZMXx0rBaduf4hg0b9OOPP+q5555TQkKCRo4c6Xe9gczurVfjbay0yvVXCIvatm2bwsPDFR0drVatWslut3tMS8zLy9PPP/+stm3bVlQMAAAAAACAKmf+/PkaO3as8vPz9d///tc1q+lcVeYGVtHzcJ1++eUXffTRR+rbt6+CgoIUGxurPn36aPbs2Tp27JhrubfeekuZmZkaPnx4WWMAAAAAAACcNR5//HE5HA5t3LhRPXr0CHScgCvzKYQjRoxQRESEunTpovj4eP3222+aMWOGIiMj9cwzz7iWe/rpp9WlSxf16NFDt9xyi3bv3q3nnntOffv2dV1pHwAAAAAAADhdmWdgXX311UpNTdW0adN0xx136N1339WQIUO0Zs0atWjRwrVcu3bttGTJEkVEROi+++7TjBkzNG7cOM2fP7+sEQAAAAAAAHAWK/MMrPHjx2v8+PF+Ldu1a1etWLGirE8JAAAAAAAqWVl/8Q9nt4pePyrsVwgBAAAAnMO2bg10glNSUgKdAKjSnL9qmJ+fr4iIiACngVXl5+dL8v0rmGVVYb9CCAAAAAAAqr6QkBCFhYUpPT2dWVjwyhij9PR0hYWFKSQkpEKegxlYAAAAAACgWLVq1dKePXu0e/duxcbGKiQkRDabLdCxEGDGGOXn5ys9PV2ZmZmqV69ehT0XDSwAAAAAAFCsmJgYSVJqaqr27NkT4DSwmrCwMNWrV8+1nlQEGlgAAAAAAKBEMTExiomJUX5+vgoLCwMdBxYRHBxcYacNFkUDCwAAAAAA+C0kJKRSGhZAUVzEHQAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlmYPdAAAAAAAfti6NdAJTklJCXQCAMA5hhlYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0e6ADAAAAAADOUlu3BjrBKSkpgU4AoAyYgQUAAAAAAABLq5AG1tNPPy2bzaZWrVp53Pbdd9+pa9euioyMVJ06dTR+/HhlZmZWRAwAAAAAAACcBcr9FMLdu3dr0qRJioqK8rjt559/1qWXXqoWLVpo2rRp2r17t6ZOnaotW7Zo0aJF5R0FAAAAAAAAZ4Fyb2D93//9ny6++GIVFhYqNTXV7baJEyeqRo0aWrZsmWJiYiRJDRs21J/+9Cd98cUX6tu3b3nHAQAAAAAAQBVXrqcQfvPNN5o/f76mT5/ucVtGRoYWL16sG264wdW8kqRRo0YpOjpac+fOLc8oAAAAAAAAOEuUWwOrsLBQd999t26++WZdcMEFHrevX79eBQUFat++vdt4aGio2rZtq7Vr15ZXFAAAAAAAAJxFyu0Uwn/+85/auXOnlixZ4vX2ffv2SZISEhI8bktISNDy5ct9PnZubq5yc3Nd/87IyJAkFRQUqKCgQJIUFBSkoKAgORwOORwO17LO8cLCQhljShwPDg6WzWZzPW7RcelEo86fcbvdLmOM27jNZlNwcLBHRl/j1ERN1ERN1ERN1ERN1ERNruwOh4JsNgXZbCp0OHSqIinYZjtRU5HHcI5LUqExfo3bg4JO1FRk3CYpOChIDmPkcI4XFPhXU5HH9pW90moq7n06+Rxea9WJv/pXWk1F1kuf657k3/tUGTUZU/z25Of75/e6V5aazvZ9BDVRk8VrOr2u0iqXBtbhw4f117/+VY8++qhq167tdZns7GxJUlhYmMdt4eHhrtu9mTx5sp544gmP8bVr17ouFl+7dm01btxY27dv16FDh1zLJCYmKjExUZs3b1Z6erprPDk5WfHx8dqwYYPbczdv3lzVq1fX2rVr3d7s1q1bKzQ0VGvWrHHL0L59e+Xl5WndunWuseDgYHXo0EHp6enatGmTazwiIkJt2rRRamqqtm3b5hqPjY1VixYttHfvXu3evds1Tk3URE3URE3URE3URE0VXNPJP4xKUuuEBIXa7Vqza5d7TUlJyiso0LqTf5CVTnx57pCUpPTsbG06ePBUTSEhalO3rlIzM7Xt8OFTNUVEqEV8vPYePardRTLWjo5W47g4bT98WIeKfOD3WlNWlpLj4hQfHa0N+/crOz//VE3x8aoeEaG1e/a4NQzOqKacHO81ZWWdqiktreT36cgRHSrya+OJsbFKrF5dm1NTlV7k/aiUmkpa97Ky3N+n9HTv71Nl1JSWdqomX9tTjRr+vU+VVVNx+4jyXvfKUhP7PWqipoDWlFHkmHsmbMac1vo+A7fffruWLFmiX3/9VaGhoZKknj17KjU1VRs2bJAkzZ8/X8OHD9c333yjbt26ud3/mmuu0fLly12ztE7nbQZWUlKSDh8+7LqeFh1PaqImaqImaqImaqImaip1TUU+xFfYbKVixt1mjCQnF5992zbrzMBKTi75fdq82TozsBo3Ln7dO7keWGIGVpH1wOf2tGOHdWZgNWlS/D5iyxbftRatqTJmYDVqxH6PmqgpgDVlZGQoLi5O6enpbtdG91eZZ2Bt2bJFM2bM0PTp07V3717XeE5OjvLz87Vjxw7FxMS4Th301qTat2+f6tat6/M5wsLCvM7cstvtstvdS3C+aKdzvrH+jp/+uGcybrPZvI77yljacWqiJl/j1ERNEjX5yljacWqiJomafGUs7bgla/LyOPaTX7D9GbfZbF7HnV+Y/R4PClKQl9fGLXuRrMFecksnmgD+Zvc17ldNRbIW+z55eU5f2Su8puLWvdOeo9j3yctzlmtNXnL63J7Ka93zksXvmk4+ps99QSnevwqvif0eNfkYp6bKqclXfn+V+SLue/bskcPh0Pjx49WoUSPXf6tWrdLmzZvVqFEjPfnkk2rVqpXsdrvHlLe8vDz9/PPPatu2bVmjAAAAAAAA4CxU5hlYrVq10vvvv+8x/pe//EXHjh3TCy+8oMaNGys2NlZ9+vTR7Nmz9eijj6patWqSpLfeekuZmZkaPnx4WaMAAAAAAADgLFTmBlatWrV09dVXe4xPnz5dktxue/rpp9WlSxf16NFDt9xyi3bv3q3nnntOffv2Vb9+/coaBQAAAAAAAGehMp9CWBrt2rXTkiVLFBERofvuu08zZszQuHHjNH/+/MqMAQAAAAAAgCqkzDOwfFm2bJnX8a5du2rFihUV9bQAAAAAAAA4y1RYAwsAAADnoK1bA53glJSUQCcAUNVUpX1YVcoKlINKPYUQAAAAAAAAKC0aWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDR7oAMAAACgBFu3BjrBKSkpgU4AAADOQczAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl2QMdAAAAAAAAnOW2bg10glNSUgKdAGeAGVgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsLQyN7B+/fVXDR8+XMnJyYqMjFStWrXUvXt3LVy40GPZjRs3ql+/foqOjlbNmjV144036tChQ2WNAAAAAAAAgLOYvawPsHPnTh07dkyjR49W3bp1dfz4cS1YsECDBg3Sa6+9pltuuUWStHv3bnXv3l2xsbGaNGmSMjMzNXXqVK1fv16rV69WaGhomYsBAAAAAADA2afMDawBAwZowIABbmN33XWXLrroIk2bNs3VwJo0aZKysrL0448/qn79+pKkjh076rLLLtOsWbNcywEAAAAAAABFVcg1sIKDg5WUlKSjR4+6xhYsWKArr7zS1bySpD59+qhp06aaO3duRcQAAAAAAADAWaDMM7CcsrKylJ2drfT0dH300UdatGiRRowYIUnas2ePDh48qPbt23vcr2PHjvr000/LKwYAAAAAAADOMuXWwHrggQf02muvSZKCgoI0ZMgQvfzyy5Kkffv2SZISEhI87peQkKC0tDTl5uYqLCzM62Pn5uYqNzfX9e+MjAxJUkFBgQoKClzPGRQUJIfDIYfD4VrWOV5YWChjTInjwcHBstlsrsctOi5JhYWFfo3b7XYZY9zGbTabgoODPTL6GqcmaqImaqImaqImapIkORyySQoOCpLDGDmKPKev8aCTOR0OhxxFHjvIZlOQzaZCh0PGj/Fgm+1ETc7X5WRtPms6maHQGLdxe1DQiZr8yF5uNTkcJb9PRd7vYJvNa3Zf4+VeU5H1xus65nD4/z5VdE0FBf5tT0Ueu8zrXllrKm4fcfI5Kn178pa9yHrgcx8hVf725KsmY4rf7/n5/lXKPsKffbnDUfnbk6/xgoLij09S4Lan07NLJR9zT95WqduTr/Ei6+s58TnCIjWdXldplVsD695779WwYcO0d+9ezZ07V4WFhcrLy5MkZWdnS5LXBlV4eLhrGV8NrMmTJ+uJJ57wGF+7dq2ioqIkSbVr11bjxo21fft2t182TExMVGJiojZv3qz09HTXeHJysuLj47VhwwZXPklq3ry5qlevrrVr17q92a1bt1ZoaKjWrFnjlqF9+/bKy8vTunXrXGPBwcHq0KGD0tPTtWnTJtd4RESE2rRpo9TUVG3bts01HhsbqxYtWmjv3r3avXu3a5yaqImaqImaqImaqEmSlJWliJAQtalbV6lZWdp2+PCpmiIi1CI+XnvT07W7SMba0dFqHBen7UeO6FBm5qmaYmOVWL26NqemKr1I9uS4OMVHR2vD/v3Kzs8/VVN8vKpHRGjtnj0nvoimpRVfU82ayiso0LqTf8CUTnwp65CUpPScHG06ePDU+1TRNVWvXvL7dPIPo5LUOiFBoXa71uza5V5TUlLl1FTktfS67mVl+f8+VXRNaWklb0/lve6VpaaS9hFZWf6/TxVd08ltTCpmH1GjRuVvT8XVVNx+L1Dbk7ea/NmXZ2VV/vbkq6a0tOKPT1JgtidvNTVtWvIx9+R2Vqnbk6+aTm5n58znCIvUlFHkmHsmbMac1pYsJ3379tXRo0e1atUq/fjjj+rQoYPefPNN3XjjjW7LPfTQQ5oyZYpycnJKNQMrKSlJhw8fVkxMjCQ6ntRETdRETdRETdR0Fte0bZt1ZmAlJxdf0/btJ8atMAMrJaXk96nIh/iAz8A6+dpKPtaxbdusMwMrObnk7WnzZuvMwGrcuPh9xMn1wBIzsIqsBz73ETt2WGcGVpMmxe/3tmzxXWvRmipjH9GoUcn78m3brDMDKzm5+OPTtm3WmYHVtGnJx9yT25klZmAV2c7Oic8RFqkpIyNDcXFxSk9Pd/VySqPcZmCdbtiwYbr11lu1efNm16mD+4p0b5327dunmjVr+mxeSSdmbnm73W63y253L8H5op3O+cb6O376457JuM1m8zruK2Npx6mJmnyNUxM1SdTkK2Npx6mJmiQL1FQkk/OD/Ol8jgcFef3VnmAvdRY3bneOn5bVI/vJDHYvWWw2m9fxCqvp5L+LfZ+81Osto6/xcq3Jy3rglr1I1hLfJz+y+xr3q6YiWYvdnrw85xmve6ePl7am4vYRpz1HpW1Pp4/bbB7bmFTMPqIytydf485t3tf+rRTvX4XX5M++vEjeStuefI37sZ0FbHvy9boXd2w9fTsL5D7itPX1rP8c4UfGyqjJV35/VcivEEqnThtMT09XvXr1VLt2bY/pbpK0evVqtW3btqJiAAAAAAAAoIorcwPrYJFzX53y8/P15ptvKiIiQueff74kaejQofr444+1q8h5qF9++aU2b96s4cOHlzUGAAAAAAAAzlJlPoXw1ltvVUZGhrp376569epp//79mjNnjjZt2qTnnntO0dHRkqSJEydq3rx56tWrl+655x5lZmZqypQpuuCCCzR27NgyFwIAAAAAAICzU5kbWCNGjNC///1vvfrqqzp8+LCqVaumiy66SM8++6wGDRrkWi4pKUlff/217r//fv35z39WaGiorrjiCj333HPFXv8KAAAAAAAA57YyN7BGjhypkSNH+rVsy5Yt9fnnn5f1KQEAAAAAAHAOqbCLuAMAAAAAAADlgQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALM0e6AAAAACVbuvWQCc4JSUl0AkAAEBRb74Z6ASnjBoV6ASWwQwsAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFiaPdABAAAAAJx9Vv4R6ASndE4JdAIAQFnRwAIAAACqABpCAIBzGacQAgAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0uyBDgAAAAAAgbTyj0AnOKVzSqATAIA1MQMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWZg90AAAAACBQVv4R6ASndE4JdAIAAKyLGVgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNHugAwAAAAAA/Lfyj0AnOKVzSqATADhXMAMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlmYPdAAAAAAAwNlp5R+BTnBK55RAJwBQFszAAgAAAAAAgKXRwAIAAAAAAICllbmB9cMPP+iuu+5Sy5YtFRUVpfr16+uaa67R5s2bPZbduHGj+vXrp+joaNWsWVM33nijDh06VNYIAAAAAAAAOIuV+RpYzz77rFasWKHhw4erdevW2r9/v15++WW1a9dO33//vVq1aiVJ2r17t7p3767Y2FhNmjRJmZmZmjp1qtavX6/Vq1crNDS0zMUAAAAAAADg7FPmBtb999+vt99+260BNWLECF1wwQV65plnNHv2bEnSpEmTlJWVpR9//FH169eXJHXs2FGXXXaZZs2apVtuuaWsUQAAAAAAAHAWKnMDq0uXLh5jTZo0UcuWLbVx40bX2IIFC3TllVe6mleS1KdPHzVt2lRz586lgQUAAHAW4BfHAABARaiQi7gbY3TgwAHVqlVLkrRnzx4dPHhQ7du391i2Y8eOWrt2bUXEAAAAAAAAwFmgzDOwvJkzZ4727NmjJ598UpK0b98+SVJCQoLHsgkJCUpLS1Nubq7CwsK8Pl5ubq5yc3Nd/87IyJAkFRQUqKCgQJIUFBSkoKAgORwOORwO17LO8cLCQhljShwPDg6WzWZzPW7RcUkqLCz0a9xut8sY4zZus9kUHBzskdHXODVREzVREzVREzVVUE3GyFE048mcDodDjiKPHWSzKchmU6HDIePHeLDNdqImR9FHOTEuSYXGeI6flt1rTQ6HbJKCg4I8svsar7CaTr5fvt6PU++xe602W9DJ28pj3P31lU5kPH3c4XCUuO6538fmNbuv8fKuqei24G27OZHVe63FjVdETQUFBSXuI0qTsTJqKm4fUfQ5ymPdK0tNRdcDX9uZpErfnnyNG2OK3Zf7+/5Vxj7Cr+OTw3Fm+3Iv4/agk+ueH/tsr+MFBcUfc6WKPT6Vpiap5M8RJ28L6DHXOV5kffX6OcJZ08n/ShoPOvmfr/FCua+pvsaDTz6H29ZUUHDWfN47fT9RWuXewNq0aZPuvPNOde7cWaNHj5YkZWdnS5LXBlV4eLhrGV8NrMmTJ+uJJ57wGF+7dq2ioqIkSbVr11bjxo21fft2t182TExMVGJiojZv3qz09HTXeHJysuLj47VhwwZXPklq3ry5qlevrrVr17q92a1bt1ZoaKjWrFnjlqF9+/bKy8vTunXrXGPBwcHq0KGD0tPTtWnTJtd4RESE2rRpo9TUVG3bts01HhsbqxYtWmjv3r3avXu3a5yaqImaqImaqKlK1WS3K7F6dW0+eFDpRbInx8UpPjpaG/buVXZ+/qma4uNVPSJCa3ftUmGRD0atExIUardrza5d7jUlJSmvoEDrTv5hTDrxYb9DUpLSs7O16eDBUzXVqlV8Tenp2l3kda8dHa3GcXHafuSIDmVmnqopNvZETamp3mvav997TXv2+F9TdnbJ71NWliJCQtSmbl2lZmVp2+HDp2qKiFCL+PjKqykt7URNPtY9qaYcKtCx/FPvk01Big1NUoHJUVbBqfcp2BaiaiF1lefIUnbhqZrstghFh8Qr15GunMJTNYUGRSvSHqfswiPKc5yqKTw4VuHB1ZVVkKoCc6qm1NTqJW5P6fkZrvFqIQkKkl3p+e7vU2xIUqXUVPS19LaPSM/PUkRwnMKCo5VZsF+F5tT7FGWPV4gtQhn5e2SKfH2qqJrWrEkrcR/h7/tUGTWVtN9Lz8/y+32q6JrWrElzjfval0s1Kn178lVTenp8scenQG1P3mry65iblXVm+3Jfx6ecHPfjU2n25WlpxX+OkCr2+FSampo2LflzRNaJ7Sygx1xnTSePZT4/G4WHq01OjlLtdm0rcr3v2MJCtcjN1d6QEO0OCXGN1y4oUOO8PG0PDdUh+6k2S2J+vhLz87U5LEzpJ5tNkpScl6f4ggJtCA9XdtCpE+Oa5+SousOhtRERKjzZcNOaNdb6vFeGz7DOyUhnymbMaW3JMti/f78uueQS5efn6/vvv1fdunUlSWvWrFGHDh305ptv6sYbb3S7z0MPPaQpU6YoJyenVDOwkpKSdPjwYcXExEg6S/4afDb+hZuaqImaqImazp2atm+vvL+cFq3J21+DGzcuvqYtW6wzAyslpeT3ads268zASk4+Me5jHVu9ZPvJ/xf4GVgX900pcXtavWSb2+N4y15ZM0Y69kl2jXnbF5zIao0ZWB37JJe4j/jus81+Z6zomi7u27jY/V7R9SDQM7CKrge+trMfvtxhmRlYnS9vUuzxaeXnW3zWWvbspaupY59GJR9zt22zzgys5OTiP0ds22aNY66k4KZNS/4ccbJpYokZWMmntjOvn43efts6M7Cuu85an/fK8Bk2IyNDcXFxSk9Pd/VySqPcZmClp6erf//+Onr0qJYvX+5qXkmnTh3cV6R767Rv3z7VrFnTZ/NKOjFzy9vtdrtddrt7Cc4X7XTON9bf8dMf90zGbTab13FfGUs7Tk3U5GucmqhJoiZfGUs7Tk2lGD/5wTDYy7LFjdt9jTv/8ujHuM1mcx8/+fr5zH7yw7DHeFCQ1wuEVmhNPt4Pt/epyOP5zF5ZNZ2W9fTsNlcG7+9T+Yx7z3j6uPO9L2578v5Y3te9iq7J23pQNHvRrP6+BkVu8Xvcn+xFs/razkqbsaJrKm6/d/pzlHXdO9NxyXtOX/uIytyefI07t3lfx6HSvH8VXZNfx9wi63KFHJ+cT+PPvtyP7cwSx9wSMrrGgzz30ZV+zHWOezl2ed1HnPyvrOPe1zzf425JiuSyxOe9k87kM6yv/P4qlwZWTk6OBg4cqM2bN2vJkiU6//zz3W6vV6+eateu7WWKubR69Wq1bdu2PGIAAAAAAHDG+CVVwLrK/CuEhYWFGjFihFauXKl58+apc+fOXpcbOnSoPv74Y+0qch7ql19+qc2bN2v48OFljQEAAAAAAICzVJlnYD3wwAP66KOPNHDgQKWlpWn27Nlut99www2SpIkTJ2revHnq1auX7rnnHmVmZmrKlCm64IILNHbs2LLGAAAAAAAAwFmqzA2sn3/+WZK0cOFCLVy40ON2ZwMrKSlJX3/9te6//379+c9/VmhoqK644go999xzxV7/CgAAAAAAAOe2Mjewli1b5veyLVu21Oeff17WpwQAAAAAAMA5pNx+hRAAgCph69ZAJzglpYSrs1alrAAAAEAFKvNF3AEAAAAAAICKRAMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlsavEAIAAAAAUMWs/CPQCU7pzI8VoxIwAwsAAAAAAACWxgwsq9i6NdAJTkihdQ4AAAAAAKyFGVgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0e6ADAAAAAACAs9vKPwKd4JTOKYFOgDPBDCwAAAAAAABYGjOwUHpbtwY6wSkptM4BAAAAADjb0cACAACwOE67AAAA5zpOIQQAAAAAAIClMQMLAAAAAADgpD9SA53glMaBDmAhzMACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdkDHQAAAKCyrfwj0AlO6ZwS6AQAAADWxwwsAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoXcUepceFbAAAAAABQmZiBBQAAAAAAAEujgQUAAAAAAABL4xRCi7DKaXln4yl5X2wIdIIT+rYKdAIAAAAAAKomZmABAAAAAADA0piBhbNetT1bAx3hhFZ+TG/bapGskpRyFk7HAwAAAABUSczAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKVxEXcAAFAuVv4R6ASndOZ3KAAAAM4qzMACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXxK4SAhfALXgAAAAAAeGIGFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjV8hBADAovhlUgAAAOCEcpmBlZmZqccee0z9+vVTzZo1ZbPZNGvWLK/Lbty4Uf369VN0dLRq1qypG2+8UYcOHSqPGAAAAAAAADgLlcsMrNTUVD355JOqX7++2rRpo2XLlnldbvfu3erevbtiY2M1adIkZWZmaurUqVq/fr1Wr16t0NDQ8ogDAAAAAACAs0i5NLASEhK0b98+1alTR2vWrFGHDh28Ljdp0iRlZWXpxx9/VP369SVJHTt21GWXXaZZs2bplltuKY84AAAAAAAAOIuUyymEYWFhqlOnTonLLViwQFdeeaWreSVJffr0UdOmTTV37tzyiAIAAAAAAICzTKX9CuGePXt08OBBtW/f3uO2jh07au3atZUVBQAAAAAAAFVIpf0K4b59+ySdON3wdAkJCUpLS1Nubq7CwsI8bs/NzVVubq7r3xkZGZKkgoICFRQUSJKCgoIUFBQkh8Mhh8PhWtY5XlhYKGNMiePBwcGy2Wyuxy06LkmFhYV+jdvtdhlj3MZtNpuCg4M9MtpsNkk6mcO4PY7NFiRjHHJnk81mK5fxE049Z0FBQYk1nf44JzL6yl6xNfnzPp24r2etZ579zGo6fV31tu6dyuv+ON6yV3RNkqrs9uRtvKrvI6ipHGsyRoXGfX0PPrkfPn3cHnRi+yg6bpMUHBQkhzFy+DEedDKnw+FQ0a07yGZT0MnX0XdNRe/h/768uPEz3UcUfS19vU/GmAo7PpW2psLCwmLXPSscc53jp283kuf25Hy8QB5zTz+e+doXnFqfA3fMdXI4HCXuI07fzrxlr6zPEd62s6LZnZ9pKnt78jZeUFBQ4r48ENtTcTUVd3wq+hyVuT15y150PfC1nUnFfXeo3H2Ec9/v63OEv+9fZewj/PkcUdJ25i17RdVUUFBQ7GejU3k9a63sfYTk+d2h5O0scPuIouurt8+wDpsUZE48grG5P4rXcXPiM5+j6NNIspkT/3Sc9hilGS/uO3pV+1x++n6itCqtgZWdnS1JXhtU4eHhrmW83T558mQ98cQTHuNr165VVFSUJKl27dpq3Lixtm/f7varhomJiUpMTNTmzZuVnp7uGk9OTlZ8fLw2bNjgyiZJzZs3V/Xq1bV27Vq3N7t169YKDQ3VmjVr3DK0b99eeXl5WrdunWssODhYHTp0UHp6ujZt2uQaj4iIUJs2bZSamqpt27a5xmNjYyWFKNeRrpzCUxlDg6IVaY9TduER5TkyT71ewbEKD66urIJUFZhT2SOC4xQWHK3Mgv0qNPmu8Sh7vEJsEcrI3yNT5OtTtZAEBcmu9PxdrrE1a9JKrKno8sG2EFULqas8R5ayCw+7xu22CEWHxFd4Tf68T+n5WYoNSZJDBTqWv881blOQYkOTVGBylFVwsMJrWrMmTVLx654kv94nSRVek6Qquz21aNFCe/fu1e7du13jVX0fQU3lWJMxWrPLfXtqn5SkvIICrdt3ansKDgpSh6QkpefkaNPBU9tTREiI2tStq9SsLG07fGp7io2IUIv4eO1NT9fuIhlrR0ercVycth85okOZp/YRibGxSpSKrSk9P9U1Xpp9uVT++4ii64Gv9ynXYa+w41Npa9qwIbvYdc8Kx1xnTdnZ2SVuT+n5WQE/5jprch7PfO0jpJoBP+Y6paZWL3EfkZ6f4df7VBk1FX0tve330vOzArI9eatpzZq0EvflgdiefNVU0vEpPT/L7/epomtybmOS72OuVKPStydfNaWnxxf7OSJQ25O3mvz5HJGenxXwY66zpjVr0or9bCTJEsfcYFuIpKYlft5zbmeBPOY6a3JuZ74+w+bHhatuao4yI+xKiz31Y3PhuYU670iu0qNDlB4d4hqPzi5QXHqejsSGKjPiVJslNjNf1TPzdah6mHLCgl3jNdPzVC27QPvjwpVvP3ViXHxajiLyHNodHyFz8g+sh9esOWs+lzsnI50pmynaGisHzou4z5w5U2PGjPEYf/PNN3XjjTe63eehhx7SlClTlJOT4/cMrKSkJB0+fFgxMTGSqv5MhNVLtlvir8Ed+ySXWNPKz7d4yRiYvwZ3uLSh26i37KuXbPNa65lnP7OaOvZJllT8uvf9F38E/C89Tl36Na2y2xOzlaip2Jq2brXODKwmTYqtadXiP4rcI7B/De7Yp5FHxtPfp9VLtltmBlanyxoXu+5999kWH49T+X8N7nx5Sonb04ljWWCPuacfz3ztC1Yv2e611kDMwLq4b0qJ+wjna+t8HG/ZK+tzhPO1lbzv35yfaawwA6tjn+QS9+XffbbZ74wVXdPFfRsXe3wquh4EegZW0fXA13b2w5c7LDMDq/PlTYr9HHH6d4dAfi7v2KdRiZ8jStrOvGWvqJo69kku9rPRqsXbLHHMlbx/dyh5OwvcDKyi25m3z7DbX3rbMjOwGt193VnzuTwjI0NxcXFKT0939XJKo9JmYDlPHdxX5K/bTvv27VPNmjW9Nq+kE7O2vN1mt9tlt7uX4HzRTud8Y/0dP/1xz2TcZrN5HfeV8cSphDYv494vVVZe40Wfs2heXzV5exzf2Su2Jn/eD/f7liZj+dZ0elZf654/71NJ4+VVU1Xenko7Tk3nUE02m+w279uTt3Gbj+WDbDYFlWY8KMjrhSeLq8n7/jYw+wh/3lfbybor4vhU0vjp2Z2vq5WPuUWzlLQ9FX28QB1zfR3PTv+3zbX+B+6Y6+R874vbR3h/rMo/5tpsQV7Xg6LZ3deDytuevI0Xzep7O6v87cnXeEn7sdOfI5D7CG85fe0jKnN78jXu3OZ9fV4o7f6wImvy53OEP9tZZe0jKnM7K4+aSvpc57nuBG4f4e3Y5fZ6m1OPYPMy5cfXeJDk7exK1+OdyXhJ39F9jVvxc7mv/P6qtIu416tXT7Vr1/YyzVxavXq12rZtW1lRAAAAAAAAUIVUWgNLkoYOHaqPP/5Yu4pce+TLL7/U5s2bNXz48MqMAgAAAAAAgCqi3E4hfPnll3X06FHt3btXkrRw4ULXBcDuvvtuxcbGauLEiZo3b5569eqle+65R5mZmZoyZYouuOACjR07tryiAAAAAAAA4CxSbg2sqVOnaufOna5/v/fee3rvvfckSTfccINiY2OVlJSkr7/+Wvfff7/+/Oc/KzQ0VFdccYWee+45n9e/AgAAAAAAwLmt3BpYO3bs8Gu5li1b6vPPPy+vpwUQQF9sCHSCE/q2CnQCAAAAAEBFqrRfIQQAwApW/hHoBKd0Tgl0AgAAAKBqoIEF4IxV27M10BFOaEUXAAAAAADOZpX6K4QAAAAAAABAadHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXZAx0AAFC1fbEh0AlO6dsq0AkAAAAAVARmYAEAAAAAAMDSmIEF4JzALCEAAAAAqLqYgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS+NXCAHAgvjVRAAAAAA4hQYWgHNCtT1bAx3hlFYpgU5QrnhtAQAAAFQ0TiEEAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXZAx0AAOCp2p6tgY5wSquUQCcAAAAAcI5jBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsrdIbWLm5uXr44YdVt25dRUREqFOnTlq8eHFlxwAAAAAAAEAVUekNrDFjxmjatGm6/vrr9cILLyg4OFgDBgzQt99+W9lRAAAAAAAAUAXYK/PJVq9erXfeeUdTpkzR//3f/0mSRo0apVatWumhhx7Sd999V5lxAAAAAAAAUAV</t>
+          <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACQaklEQVR4nOzdeXhU5fn/8c+ZmWwQkpiQyBaQgCyC4MIiuABKERewCghuLNKfdaVWq1Zta91Aq3WvrdZvwYVWEXfrBhQsVRCjKCJSVJayYwhMCGSbmef3R5jJTGYmmZBlzuD7dV1eLfecOXPfc85zzpk7z5yxjDFGAAAAAAAAgE054p0AAAAAAAAAUBcaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAADTA5MmTZVmWJk2aFNPyDz/8sCzL0jHHHNPMmdVv+PDhsixLS5YsicvrT506VZZlac6cOXF5/aYS7/fxx+Soo46SZVnauHFjvFMBAABxRgMLAIAGmD59uiTp9ddf1549e+pdfvbs2SHPay6///3vZVmWfv/73zfr6xzuEul9bMlG2pIlS2RZloYPH97srwUAABAJDSwAABrgtNNOU/fu3VVRUaG5c+fWueynn36qr776SklJSbrssstaKMPonnvuOX3zzTcaNGhQvFNJaLyPAAAALY8GFgAADWBZli6//HJJNbOrovE/fu655yovL6/Zc6tP586d1atXL7Vq1SreqSQ03kcAAICWRwMLAIAGmjp1qpxOpz7//HOtWrUq4jLl5eX6xz/+ISn864OfffaZLrnkEnXu3FkpKSnKzs7WmWeeqXfeeSfiuoLvA/TGG2/o9NNPV3Z2duDrY5Zl6c4775Qk3XnnnbIsK/Df1KlTA+up7ytn//rXvzRhwgR16tRJKSkpys3N1cCBA3XHHXdo9+7dgeWqqqr0wgsv6JJLLlGvXr2UkZGhtLQ09ezZUzNmzNC2bdtifSvrNWfOnEAdu3fv1jXXXBN437p06aJf/vKXUb/K+eqrr+pnP/uZ+vbtqyOOOEKpqanq2rWrLr/8cv33v/8NW76p3sdFixbpggsuUPv27ZWcnKy8vDydf/75WrZsWcTl/a8hSa+88opOOeUUZWRkqHXr1jr55JPD9gv/Nv/www8lSSNGjAjJNfgeY5999pkmTpyoTp06KTk5WRkZGSooKNC4ceP0xhtvRMyntuHDh2vEiBGSpA8//DDktY466qiQZT0ej/7yl79o6NChyszMVGpqqo4++mjNmDFDW7dujen1onnttdcC702bNm00fPjwqGPGb/78+Ro9erRyc3OVnJysjh076tJLL9WaNWsa/PrffvutLr/8cnXt2lUpKSlKT09Xly5ddM4550RtZq9bt04///nP1a1bN6WmpiozM1OnnXaaXnjhhSbLe+PGjYFtYYzR008/rRNPPFGtW7dWZmamRo0aFXXfAwAgoRgAANBgY8aMMZLMjBkzIj4+d+5cI8l06NDBeDyeQPyRRx4xDofDSDLHHXecGT9+vDnllFNMcnKykWTuvPPOsHV16dLFSDLXXnutkWQGDBhgLrroIjNs2DDz73//20yZMsX079/fSDL9+/c3U6ZMCfz317/+NbCeYcOGGUlm8eLFYa9x3XXXGUmBvCZNmmTOOussU1BQEPaczZs3G0kmMzPTnHTSSWbChAnm7LPPNh06dDCSTG5urvn222/DXmPKlClGkpk9e3bM7/Ps2bONJDN27FjTrVs3k5WVZX7605+a888/3xxxxBFGkunZs6fZtWtX2HOdTqdp1aqVGTBggLngggvM2LFjA/W0bt3afPTRR2H5NfZ9vPHGG40k43A4zKBBg8yECRPM4MGDjWVZxul0mr/97W9hz/G/77/73e+MZVnm5JNPNhMnTgzkYlmWefXVVwPLf/PNN2bKlCnmyCOPNJLMmWeeGZLr0qVLjTHGLFy40CQlJQXqGT9+vDn//PPNoEGDTEpKijnvvPNi2gazZs0yZ555ppFkjjzyyJDXuvHGGwPLlZeXm5EjRxpJJjU11Zx11llm4sSJJj8/30gybdu2NZ999llMr+nn3/d/+ctfhuz7gwYNCrxvjz32WNjzqqqqzIUXXmgkmZSUFDN06FAzYcKEwHualpZm3n333Zjz+Oqrr0xGRkZgf7vgggvMhAkTzJAhQ0x6errp379/2HPmzZtnUlNTjSTTq1cvc/7555vTTz/dtG7d2kgy06ZNa5K8N2zYYCSZLl26mClTppikpCRz+umnmwsvvND06NEjsK7ly5fHXC8AAHZEAwsAgEPw+uuvG0kmJyfHVFRUhD3u/yB/2223BWLvvfeesSzLtG3b1nz44Ychy69atcp06tTJSDJLliwJecz/Id7pdJo33ngjYj533HGHkWTuuOOOqDlHa7w89thjgVr+9a9/hT3vk08+Mf/73/8C/y4pKTFvvPFGWN2VlZXm1ltvNZLM2WefHbaexjSwJJmTTjrJ7N69O/DYnj17zNChQ40kM2nSpLDnvvjii6a0tDQk5vP5zJ/+9CcjyfTp08f4fL6QxxvzPj799NNGkunevbv58ssvQx778MMPTZs2bUxycrJZt25dyGP++rKyssKaDP58evToEXMefiNGjDCSzAsvvBD22N69e82yZcui1ljb4sWLjSQzbNiwqMvccsstRpLp1q2b2bBhQyBeWVlppk+fbiSZrl27Rhwv0fj3fcuywup48cUXjWVZxuVyma+++irksdtuu81IMoMHDzbr168Peezll182TqfTHHHEEWbPnj0x5TFt2jQjydxzzz1hjx04cCDieE5JSTGpqanmlVdeCXls48aN5thjjzWSzLPPPtvovP0NLH8T67///W/gMY/HYy6//HIjyYwaNSqmWgEAsCsaWAAAHIKqqirTrl07I8m8/PLLIY9t2rQpMMsqeCbS4MGDjSQzf/78iOucN2+ekWTGjRsXEvd/iL/88suj5nOojZeqqiqTm5trJIV90D5UHTp0MA6Hw5SUlITEG9vAWrlyZdjjq1atMpZlGYfDYTZv3hzzeocMGWIkma+//jokfqjvo9frDcxAKywsjPi8P/zhD0ZSyKwlY2oaWJFmEpWXl5vMzEwjKaSJGC2PYMccc4yRZIqLi6PWEqv6GlhlZWUmPT3dSDJvvvlm2OP79+8PzBibO3duzK/r3/d/+tOfRnx83LhxRpL5f//v/wViu3fvNmlpaSY1NdVs2bIl4vOuvvpqI8k8/vjjMeVx9tlnG0nm888/j2n5iRMnGknmwQcfjPj4ihUrjCRz4oknNjrv4AZWpPd++/btgVlYlZWVMeUPAIAdcQ8sAAAOgcvl0pQpUyRJf/vb30Iemz17tnw+n4YNG6bu3btLkoqKirRixQqlpaVpzJgxEdc5fPhwSdLHH38c8fHx48c3UfY1PvvsM/3www9q27atzj///AY998svv9RDDz2k6667TpdffrmmTp2qqVOnyuPxyOfz6bvvvmuyPPv376/jjjsuLH7sscfq+OOPl8/n07///e+wx7/77js98cQTuv766zV9+vRAjjt37pSkiPfCOhQrV67Utm3b1K1bN5144okRl6lv+0baL1JSUlRQUCBJDb6HlP9XEi+55BL95z//kcfjadDzG6KwsFClpaXKzs6OWEerVq00adIkSdLixYsbvH7/WIsWD74f2eLFi1VWVqaTTz5ZHTt2jPi8+rZFbf738qqrrtL777+v8vLyqMv6fD69++67kqSJEydGXGbAgAFKT0/XypUrA+tqbN4ul0ujR48Oi7dr105HHHGEKioqQu5lBwBAonHFOwEAABLV5Zdfrvvvv18ffPCBtm7dqo4dO8oYE7iJdvDN2zds2CBjjMrKypSSklLnen/44YeI8do3zG4KmzZtkiT17NkzcCPx+uzfv1+XXXaZXnvttTqXKykpaXR+fl27dq3zsc8//1xbtmwJxLxer6699lo99dRTMsY0e47r16+XJH3//ff1vo/Rtm/nzp0jxjMyMiSpzqZJJLNmzdKqVav07rvv6t1331VaWppOOOEEDR8+XJdccol69+7doPXVxd9cq2s7devWLWTZhoi2Xn88eNv7t8WiRYsOeVvUdtNNN+k///mPFi5cqNGjRyspKUn9+/fXaaedpkmTJmngwIGBZXfv3h3Yr/Lz8+td9+7du9WxY8dG592+fXslJSVFXD4jI0N79uxp8D4EAICd0MACAOAQ9ejRQ6eeeqqWLl2q5557TrfeeqsWL16sjRs3KjMzM2TGlM/nkySlp6dr3Lhxh/R6aWlpTZJ3Y91666167bXX1KtXL913330aOHCg2rZtq+TkZEnS0KFDtWzZsjobR80h+PUeffRR/eUvf1G7du300EMPaejQoTryyCOVmpoqSbr44ov1j3/8o8ly9G/fdu3a6cwzz6xz2bZt20aMOxxNOzG+Xbt2Kiws1IcffqiFCxfqo48+0ieffKKPPvpIM2fO1KxZs3TLLbc06WvGS/B29G+L7t276+STT67zeb169Ypp/a1atdKCBQv06aef6r333tPHH3+sjz/+WIWFhXrooYd09dVX609/+lPI60vRZ44F8ze0G5t3U+8/AADYDQ0sAAAaYfr06Vq6dKlmz56tW2+9NfB1wkmTJoU0nPwzMSzL0t/+9jfbfNj0z/pZt26djDExzcKaN2+eJOmll15Sv379wh7/9ttvmzZJVc9gi2bjxo2SpE6dOgVi/hyfeuopjR07Nuw5TZ2jf/vm5OQEZuDZgWVZGj58eOCrZ+Xl5ZozZ46uueYa3XbbbRo/fnxgZlRj+L/yVtd28s8wivb1uLps2LBB/fv3D4tH2vb+bdGzZ88m3xYDBw4MzLbyeDx6/fXXNXnyZD355JMaP368RowYobZt2yotLU1lZWV68MEHozYsa2vOvAEAOBzY4+oZAIAENWHCBGVkZOjbb7/V22+/rVdffVVS6NcHJalDhw7q16+f9u3bp/fee6/J8/DPfmrofY4GDBigtm3b6ocfftDrr78e03OKi4slSV26dAl77P3331dRUVGDcojFqlWrtGrVqrD4119/rc8//1wOh0OnnXZaTDl+/fXX+uKLLyK+zqG+j/5ZaGvWrNHXX3/doOceqkPJNTU1VVdeeaX69esnn88X8T09lNfy39OpuLhYb775ZtjjZWVlevHFFyVJI0aMiDlfv+effz5i/LnnnpNUc28oSTrjjDOUnJysJUuWaNeuXQ1+rVi5XC6NHz8+MOPOv085nU795Cc/kVTTSI1FS+UNAECiooEFAEAjtGrVShdddJGk6ntilZWV6dhjjw25J47fPffcI0maNm2a3nrrrbDHjTH65JNP9MEHHzQ4D/8MlIY2T1wul26//XZJ0hVXXBHxRuiffvppyD2G/PdOevzxx0OW++9//6srr7yyQa8fK2OMrrrqKu3ZsycQc7vduuqqq2SM0bhx40LuN+TP8U9/+lPIV7q2b9+uyZMnR23EHOr7mJSUpDvuuEPGGJ1//vn6z3/+E7aM1+vVv/71Ly1fvrxB646mvlwffPBB/e9//wuLr127NjADLVKDr67X+vbbb1VVVRX2eGpqqq655hpJ0o033hi4t5okVVVV6Re/+IV27Nihrl27HtKPEbz22muBBpjf/Pnz9corr8jlcum6664LxI888khdd9112r9/v8aMGaOvvvoqbH0VFRV68803tXbt2phe/8knn4x4w/8dO3aosLBQUuh7eccddyg5OVk33XSTnn322ZB90G/16tWBhndz5Q0AwGElPj9+CADA4WPFihWBn7GXZB555JGoyz766KPG5XIZSaZ79+7mnHPOMRdffLH5yU9+YvLy8owkc8stt4Q8p0uXLkaS2bBhQ9T17tixw7Ru3dpIMieffLKZOnWqmT59uvnb3/4WWGbYsGFGklm8eHHIc30+n7nyyisD+R9//PFm0qRJ5uyzzzYFBQVhz3nllVeMZVlGkjn22GPNpEmTzOmnn26SkpLM6aefboYOHRrxdaZMmWIkmdmzZ9f3lgbMnj3bSDJjx441BQUFJisry5x//vnmggsuMNnZ2UaSOfroo83OnTtDnrd8+XKTnJwceJ8vvPBCM3r0aJOWlmb69Oljzj///Ii5NOZ9NMaYm266KfA+9unTx5x33nlm0qRJZvjw4SYrK8tIMn/+859DnuNfPppor/f2228bSSY5Odmce+655vLLLzfTp083H330kTHGmMzMTCPJ9OrVy5x//vnm4osvNsOHDw/sf5MnT45hC9QYMGCAkWR69uxpLrnkEjN9+vSQfbW8vNycccYZRpJJS0szZ599tpk4caLp3LmzkWRycnJMYWFhg17Tv+9ff/31RpIZOHCgufjii83gwYMD79tDDz0U9ryqqipz8cUXG0nG4XCY448/3owbN85MnDjRnHzyyYFt/O6778aUR//+/Y0k07VrVzNmzBhzySWXmFGjRpm0tDQjyZx++ummqqoq5Dnz5s0zrVq1MpJMp06dzKhRo8wll1xizjrrLNOpUycjyUycOLHReW/YsMFIMl26dKn3fazrGAIAgN3RwAIAoAkce+yxgWZCUVFRnct+9dVX5oorrjBHH320SU1NNa1atTIFBQXmzDPPNI899pjZunVryPKxfvj897//bUaOHGmOOOII43A4jCQzZcqUwON1NV6MMebdd9815513njnyyCNNUlKSyc3NNYMGDTJ33nmn2b17d9hrnXHGGaZt27amVatWpm/fvubee+81FRUVUV+nMQ2sKVOmmF27dpmf//znplOnTiY5Odnk5+ebGTNmhOXmt2rVKjN27FjTvn17k5qaao4++mhz8803m5KSkjpzaez7+NFHH5lLLrnEdOnSxaSkpJg2bdqYHj16mJ/+9KfmmWeeMcXFxSHLH2oDyxhj/vrXv5oTTjgh0CgJrumFF14w06ZNM3379jXZ2dkmJSXFdOnSxZx11lnmtddeMz6fL+prRrJp0yZz8cUXm/bt2weaYLWbJlVVVebJJ580J510kmnTpo1JTk423bp1M9ddd53ZsmVLg17PmNB9f968eWbIkCEmPT3dtG7d2px66qnmrbfeqvP577zzjrngggtMx44dTVJSksnKyjK9e/c2kyZNMn//+9/N/v37Y8rj7bffNldddZU5/vjjTW5urklOTjadOnUyw4cPN88++6yprKyM+LwNGzaYX/7yl6Zv376mdevWJjU11XTp0sUMHz7c3Hfffea7775rdN40sAAAPxaWMS38E0EAAAAxmjNnjqZNm6YpU6ZwY2sAAIAfMe6BBQAAAAAAAFujgQUAAAAAAABbo4EFAAAAAAAAW+MeWAAAAAAAALA1ZmABAAAAAADA1mhgAQAAAAAAwNZc8U7gUPh8Pm3btk1t2rSRZVnxTgcAAAAAAAB1MMZo37596tChgxyOhs+nSsgG1rZt25Sfnx/vNAAAAAAAANAAmzdvVqdOnRr8vIRsYLVp00ZSddEZGRlxzgYAAAAAAAB1KSkpUX5+fqCn01AJ2cDyf20wIyODBhYAAAAAAECCONRbQXETdwAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYWkL+CiEAAAAAAGh5xhh5vV55PJ54pwKbcLlccjqdh/zrgjG/TrOuHQAAAAAAJDxjjPbu3asffvhBXq833unAZpxOp/Ly8pSZmdlsjSwaWAAAAAAAoE47duzQ3r17lZGRoYyMDLlcrmafcQP7M8bI4/GopKRE27dvV1lZmdq3b98sr0UDCwAAAAAAROX1euV2u5Wbm6u2bdvGOx3YUJs2bZSSkqKioiLl5eXJ6XQ2+WtwE3cAAAAAABBVVVWVjDFq3bp1vFOBjbVu3VrGGFVVVTXL+mlgAQAAAACAevGVQdSlufcPGlgAAAAAAACwNRpYAAAAAAAAiGjq1Kk66qij4p0GDSwAAAAAAPDjNWfOHFmWFfW/5cuXxzvFeq1Zs0a///3vtXHjxnin0mz4FUIAAAAAAPCjd9ddd6lr165h8e7du8chm4ZZs2aN7rzzTg0fPtwWs6WaAw0sAAAAAABwyD5YHe8MpFF9G7+Os846SwMGDGj8itAs+AohAAAAAABAHe644w45HA4tWrQoJH7FFVcoOTlZX375pSRpyZIlsixLL730km677Ta1a9dOrVu31tixY7V58+aw9X7yyScaPXq0MjMz1apVKw0bNkwfffRR2HJbt27V9OnT1aFDB6WkpKhr16666qqrVFlZqTlz5mjChAmSpBEjRgS++rhkyZLA8999912deuqpat26tdq0aaNzzjlHX3/9ddjrvP766+rbt69SU1PVt29fvfbaa41525oUM7AAAAAAAMCPntvtVlFRUUjMsizl5OToN7/5jd566y1Nnz5dX331ldq0aaP3339ff/3rX3X33Xerf//+Ic+79957ZVmWbrnlFu3atUuPPPKIRo4cqS+++EJpaWmSpH/9618666yzdOKJJwYaZLNnz9bpp5+upUuXatCgQZKkbdu2adCgQdq7d6+uuOIK9erVS1u3btX8+fN14MABnXbaaZoxY4Yee+wx3Xbbberdu7ckBf73+eef15QpU3TmmWfq/vvv14EDB/TnP/9Zp5xyilauXBn4yuEHH3ygcePG6ZhjjtGsWbO0e/duTZs2TZ06dWrOtz1mljHGxDuJhiopKVFmZqbcbrcyMjLinQ4AAAAAAIet8vJybdiwQV27dlVqamrY44n+FcI5c+Zo2rRpER9LSUlReXm5JGn16tU68cQTNXnyZD3wwAPq27ev2rdvr2XLlsnlqp4ftGTJEo0YMUIdO3bUN998ozZt2kiSXn75ZV144YV69NFHNWPGDBlj1LNnTxUUFOjdd9+VZVmSpLKyMvXp00fdu3fXBx98IEmaMmWKXnjhBX3yySdhX3E0xsiyLM2fP18TJkzQ4sWLNXz48MDjpaWlys/P14QJE/T0008H4jt37lTPnj114YUXBuLHH3+8du7cqW+++UaZmZmSpAULFmjUqFHq0qVLvTeIr28/aWwvhxlYAAAAAADgR+9Pf/qTevToERJzOp2B/9+3b1/deeeduvXWW7Vq1SoVFRXpgw8+CDSvgk2ePDnQvJKk8ePHq3379nrnnXc0Y8YMffHFF/r222/1m9/8Rrt37w557hlnnKHnn39ePp9PUvXX+saMGRPx/lz+xlc0CxYs0N69e3XRRReFzC5zOp0aPHiwFi9eLEnavn27vvjiC/36178ONK8k6Sc/+YmOOeYY7d+/v87XaQk0sAAAAAAAwI/eoEGD6r2J+0033aQXX3xRK1as0MyZM3XMMcdEXO7oo48O+bdlWerevXtgFtO3334rqXp2VTRut1uVlZUqKSlR376HNsXM/zqnn356xMf9M6E2bdoUMW9J6tmzpz7//PNDev2mRAPLLr77Lt4ZVIvl50HtkqsUW74AAAAAADSB9evXB5pCX3311SGvxz+76oEHHtBxxx0XcZn09HQVFxcf8msEv87zzz+vdu3ahT0eafaYXSVOpgAAAAAAAHHi8/k0depUZWRk6Prrr9fMmTM1fvx4XXDBBWHL+ptcfsYYfffdd+rXr58kqVu3bpKqZ0CNHDky6mvm5uYqIyNDq1fXfaOxaF8l9L9OXl5ena/TpUuXiHlL0n//+986X7ulOOKdAAAAAAAAgN099NBD+vjjj/X000/r7rvv1tChQ3XVVVeF/XKhJD333HPat29f4N/z58/X9u3bddZZZ0mSTjzxRHXr1k0PPvigSktLw57/ww8/SJIcDod++tOf6q233lJhYWHYcv7f5WvdurUkae/evSGPn3nmmcrIyNDMmTNVVVUV9XXat2+v4447Ts8++6zcbnfg8QULFmjNmjV1vi8thRlYAAAAQAKww698+cXya1+Jli8AvPvuu1q7dm1YfOjQoaqoqNBvf/tbTZ06VWPGjJFU/euFxx13nK6++mrNmzcv5DnZ2dk65ZRTNG3aNO3cuVOPPPKIunfvrv/3//6fpOrG1DPPPKOzzjpLffr00bRp09SxY0dt3bpVixcvVkZGht566y1J0syZM/XBBx9o2LBhuuKKK9S7d29t375dL7/8sv7zn/8oKytLxx13nJxOp+6//3653W6lpKTo9NNPV15env785z/rsssu0wknnKBJkyYpNzdX//vf//TPf/5TJ598sp544glJ0qxZs3TOOefolFNO0eWXX67i4mI9/vjj6tOnT8QmW0ujgQUAAAAAAH70fve730WMP/PMM3rqqafUtm1bPfLII4H40UcfrVmzZukXv/iF5s2bpwsvvDDw2G233aZVq1Zp1qxZ2rdvn8444ww9+eSTatWqVWCZ4cOHa9myZbr77rv1xBNPqLS0VO3atdPgwYP185//PLBcx44d9cknn+i3v/2t5s6dq5KSEnXs2FFnnXVWYH3t2rXTX/7yF82aNUvTp0+X1+vV4sWLlZeXp4svvlgdOnTQfffdpwceeEAVFRXq2LGjTj31VE2bNi3wOqNHj9bLL7+s3/zmN7r11lvVrVs3zZ49W2+88YaWLFnSRO/yobOMf75ZAikpKVFmZqbcbnfgjvkJzy43Rucm7gAAALaUaDOaEi1fANGVl5drw4YN6tq1q1JTU+Odjq0tWbJEI0aM0Msvv6zx48fHO50WVd9+0theDvfAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArXETdwAAAAAAgCYwfPhwJeCtxhMCM7AAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAMCP1pw5c2RZllJTU7V169awx4cPH66+ffvGITMEc8U7AQAAAAAAkMDeey/eGUijRzd6FRUVFbrvvvv0+OOPN0FCaGrMwAIAAAAAAD96xx13nP76179q27Zt8U4FEdDAAgAAAAAAP3q33XabvF6v7rvvvjqX83g8uvvuu9WtWzelpKToqKOO0m233aaKiorAMjfccINycnJkjAnErrvuOlmWpcceeywQ27lzpyzL0p///OemL+gwQwMLAAAAAAD86HXt2lWTJ0+udxbWz372M/3ud7/TCSecoIcffljDhg3TrFmzNGnSpMAyp556qoqLi/X1118HYkuXLpXD4dDSpUtDYpJ02mmnNUNFhxcaWAAAAAAAAJJuv/12eTwe3X///REf//LLL/Xss8/qZz/7mV5++WVdffXVevbZZ/WrX/1Kr7/+uhYvXixJOuWUUyTVNKjcbre++uorjRs3LqyBlZ2drWOOOaaZK0t8NLAAAAAAAAAkFRQU6LLLLtPTTz+t7du3hz3+zjvvSKr+imCwG2+8UZL0z3/+U5KUm5urXr166d///rck6aOPPpLT6dRNN92knTt36ttvv5VU3cA65ZRTZFlWs9V0uKCBBQAAAAAAcNBvfvMbeTyeiPfC2rRpkxwOh7p37x4Sb9eunbKysrRp06ZA7NRTTw3Mtlq6dKkGDBigAQMGKDs7W0uXLlVJSYm+/PJLnXrqqc1b0GGCBhYAAAAAAMBBBQUFuvTSS6POwpIU04ypU045RVu3btX69eu1dOlSnXrqqbIsS6eccoqWLl2qjz/+WD6fjwZWjGhgAQAAAAAABPHPwqp9L6wuXbrI5/MFvgLot3PnTu3du1ddunQJxPyNqQULFujTTz8N/Pu0007T0qVLtXTpUrVu3VonnnhiM1dzeHA1dgWffvqpnn32WS1evFgbN25UTk6OTjrpJN1zzz3q0aNHYLmpU6fq2WefDXt+z549tXbt2samAQAAAACH5IPV8c6gxqi+8c4AgCR169ZNl156qZ566il16dJFLld1++Tss8/WbbfdpkceeURPPfVUYPmHHnpIknTOOecEYl27dlXHjh318MMPq6qqSieffLKk6sbWr371K82fP18nnXRSYN2oW6Pfpfvvv18fffSRJkyYoH79+mnHjh164okndMIJJ2j58uXq27fmCJySkqJnnnkm5PmZmZmNTQEAAAAAAKBJ3X777Xr++ef13//+V3369JEk9e/fX1OmTNHTTz+tvXv3atiwYVqxYoWeffZZ/fSnP9WIESNC1nHqqafqxRdf1LHHHqsjjjhCknTCCSeodevWWrdunS6++OIWrytRNbqBdcMNN+jvf/+7kpOTA7GJEyfq2GOP1X333acXXnih5sVcLl166aWNfUkAAAAAAIBm1b17d1166aVh3yZ75plnVFBQoDlz5ui1115Tu3btdOutt+qOO+4IW4e/gXXKKacEYi6XS0OGDNHChQu5/1UDWMYY0xwr9n+H87PPPpNU/RXC+fPny+12a//+/crIyDjkdZeUlCgzM1Nut7tR67GV776LdwbVav2SQkR2yVWKLV8AAIDDQKJ9zS2R8k2kXIF4KC8v14YNG9S1a1elpqbGOx3YVH37SWN7Oc1yE3djjHbu3Km2bduGxA8cOKCMjAxlZmYqOztb11xzjUpLS5sjBQAAAAAAABwmmuVOYXPnztXWrVt11113BWLt27fXzTffrBNOOEE+n0/vvfeennzySX355ZdasmRJnTctq6ioUEVFReDfJSUlkiSPxyOPxyNJcjgccjgc8vl88vl8gWX9ca/Xq+DJZtHiTqdTlmUF1hsclySv1xtT3OVyyRgTErcsS06nMyxHy7LklOQzRr7gHA/m6fP55Atat8Oy5LAseX0+mRjiTsuqrskXvJbquCR5gyfheTz11xScuySnwxGWe7R4k9fU0tspQjzh9z1qoiZqoiZqoiZqSoiajE+S5ZBlOWR8Xin46siqrsn4QmuSVZ27jDemuOWorik0bslyOGWM72ASksdTf03Byx9ceZTcW6amurZTTZrhtYbk2AI1Be+Wdtn36oon6niipobV5PF4ao5FEb7EZVmWreINYbfcE7kmqXr/CO7VBO97tfe/hmryBtbatWt1zTXXaMiQIZoyZUogPmvWrJDlJk2apB49euj222/X/PnzNWnSpKjrnDVrlu68886w+MqVK9W6dWtJUm5urrp166YNGzbohx9+CCzTqVMnderUSevWrZPb7Q7ECwoKlJeXp9WrV6usrCwQ79Wrl7KysrRy5cqQQdyvXz8lJyersLAwJIcBAwaosrJSq1atCsScTqcGDhwot9sd8guLaWlp6t+/v4qKirR+/fpAPDMzU72TkrTN7daWoBxz09PVLSdHG/bs0Q9BM9U6ZWaqU1aW1hUVyR2Ue0FOjvLS07V6xw6VVVXV1JSXp6y0NK3cujWk+dSvfXslu1wq3Ly5pqDi4vprClo+LSlJ/Tt0UNH+/Vq/e3dNTWlp6p2X1/w1xbKd9u/XgPx8VXo8WrV9e01NDocG5ufLXVamtbt2hddUWhq5pr17I9e0e3fkmnbtqq7p4L5a575XVKSVmzfXv52k5q9p8ODEHU+9e2vbtm3asmVLTU2JfoygJmqiJmqiph99TZX7JFdmgZyt8lS1e7WMp6ampOxeslKyVLVrpUxQAyepbT9ZzmRV7gytKfnIATLeSlUV1dRkWU4ltxsoU+lWVXFNTZYrTcm5/eUrK5LHXV1T4YH6a/K6N8hbVlOTM72TXG06ybN3nXwVNdupJWqqbztV7quOO1IylZTdW97SbfKW1tTkTMuVK6tlaio8UFOTXfY96fAbT9TU8Jr8Xwnzer0qLy8PxB0Oh1q1aiWPxxMy8cTpdCotLU1VVVWqrKwMxF0ul1JTU1VRURHS0EhOTlZycrLKy8tDckxJSVFSUpLKyspCmnipqalyuVw6cOBASDMlLS1NDodD+/fvD6mpdevW8vl8Ie+LZVlq3bo1NTVRTZJUVVWl1atrvpcdvO/5JyMdqia9B9aOHTt08sknq6qqSsuXL1eHDh3qXL6srEzp6emaNm1a2K8TBos0Ays/P1+7d+8OfG/SLp1pvwZ32zdssMcMrIKC+mv69tua3BXnGVhHHRVaU6Tc16+PXKskl8NRXVMMuTe6poKC6nhd+97338e2neqIN1lNPXok7niy8V+vqImaqImaqMleNS1aE5RkM81WqjMeNLPnjN5117RoTdDycZ6BdcYx9W+n97+yzwysn/Spe9+r2Q/iPwPrjGNqwok2noIdLscIaqqOl5eX63//+58KCgoCjYpgzFaiJqm6d7N+/Xp17tw50PAM3vdKSkqUk5NzyPfAarIZWG63W2eddZb27t2rpUuX1tu8kqq7iDk5OSouLq5zuZSUlIiDxOVyhX310D9ga/MPwFjj0b7S2JC4ZVkR49Fy9Dc8Ii4f4TWdEdZRV9wVLR78mkH5Rq2pIbk3d02xbI+g57oi5GJZVsR4k9dUK9eo+14s26meeJPWlKjjqYFxaqKmaHFqoiaJmqLl2NC4HWuyIp12rSiXyBHilmVFiTsUaeV1xV2uumsKfprliFyT5Yg992jxWGoKvdSKvD2i1ho19+atqa59r3aaDd5+TVhTpCGVKOOpsXFqsm9NLper+tggBf63NrvFG8JuuSd6TZF6NZFiDdUkDazy8nKNGTNG69at08KFC3XMMcfU/yRJ+/btU1FRkXJzc5siDQAAAAAAAByGGt3A8nq9mjhxopYtW6Y33nhDQ4YMCVumvLxcVVVVatOmTUj87rvvljFGo0ePbmwaAAAAAAAAOEw1uoF144036s0339SYMWNUXFysF154IeTxSy+9VDt27NDxxx+viy66SL169ZIkvf/++3rnnXc0evRonXfeeY1NAwAAAAAAAIepRjewvvjiC0nSW2+9pbfeeivs8UsvvVRZWVk699xztWDBAj377LPyer3q3r27Zs6cqV/96lcRv8sLAAAAAAAASE3QwFqyZEm9y2RlZen5559v7EsBAAAAAADgR4ipTwAAAAAAALA1GlgAAAAAAADNxLIs/f73v493GgmPBhYAAAAAAPhRsiwrpv9iuX0Smlej74EFAAAAAAB+xL77Lt4ZSN27H9LTat+v+7nnntOCBQvC4r179z7k1NA0aGABAAAAAIAfpUsvvTTk38uXL9eCBQvC4og/vkIIAAAAAAAQxf79+3XjjTcqPz9fKSkp6tmzpx588EEZY0KWq6io0C9/+Uvl5uaqTZs2Gjt2rLZs2RK2vk2bNunqq69Wz549lZaWppycHE2YMEEbN24MLLN+/XpZlqWHH3447Pkff/yxLMvSP/7xjyav1c5oYAEAAAAAAERgjNHYsWP18MMPa/To0XrooYfUs2dP3XTTTbrhhhtClv3Zz36mRx55RKNGjdJ9992npKQknXPOOWHr/PTTT/Xxxx9r0qRJeuyxx3TllVdq0aJFGj58uA4cOCBJKigo0Mknn6y5c+eGPX/u3Llq06aNzjvvvOYp2qb4CiEAAAAAAEAEb775pv71r3/pnnvu0e233y5JuuaaazRhwgQ9+uijuvbaa9WtWzd9+eWXeuGFF3T11VfrT3/6U2C5Sy65RKtWrQpZ5znnnKPx48eHxMaMGaMhQ4bolVde0WWXXSZJmjx5sn7+859r7dq16tWrlySpqqpK8+bN0wUXXKBWrVo1d/m2wgwsAAAAAACACN555x05nU7NmDEjJH7jjTfKGKN33303sJyksOWuv/76sHWmpaUF/n9VVZV2796t7t27KysrS59//nngsQsvvFCpqakhs7Def/99FRUV/Sjv0UUDCwAAAAAAIIJNmzapQ4cOatOmTUjc/6uEmzZtCvyvw+FQt27dQpbr2bNn2DrLysr0u9/9LnBPrbZt2yo3N1d79+6V2+0OLJeVlaUxY8bo73//eyA2d+5cdezYUaeffnqT1ZgoaGABAAAAAAC0kOuuu0733nuvLrzwQs2bN08ffPCBFixYoJycHPl8vpBlJ0+erPXr1+vjjz/Wvn379Oabb+qiiy6Sw/Hja+dwDywAAAAAAIAIunTpooULF2rfvn0hs7DWrl0beNz/vz6fT99//33IrKv//ve/YeucP3++pkyZoj/+8Y+BWHl5ufbu3Ru27OjRo5Wbm6u5c+dq8ODBOnDgQOAeWT82P76WHQAAAAAAQAzOPvtseb1ePfHEEyHxhx9+WJZl6ayzzpKkwP8+9thjIcs98sgjYet0Op0yxoTEHn/8cXm93rBlXS6XLrroIs2bN09z5szRscceq379+jWmpITFDCwAAAAAAIAIxowZoxEjRuj222/Xxo0b1b9/f33wwQd64403dP311wfueXXcccfpoosu0pNPPim3262hQ4dq0aJF+u6778LWee655+r5559XZmamjjnmGC1btkwLFy5UTk5OxBwmT56sxx57TIsXL9b999/frPXaGQ0sAAAAAACACBwOh95880397ne/00svvaTZs2frqKOO0gMPPKAbb7wxZNm//e1vga/7vf766zr99NP1z3/+U/n5+SHLPfroo3I6nZo7d67Ky8t18skna+HChTrzzDMj5nDiiSeqT58++uabb3TJJZc0W612Z5na89YSQElJiTIzM+V2u5WRkRHvdJpGhK5sXHTvXv8ydslVSqx8EylXKbZ8AQBIcB+sjncGNUb1rfvxRMpVSqx8EylXIB7Ky8u1YcMGde3aVampqfFO50fp+OOPV3Z2thYtWhTvVKKqbz9pbC+He2ABAAAAAADYVGFhob744gtNnjw53qnEFV8hBAAAAAAAsJnVq1frs88+0x//+Ee1b99eEydOjHdKccUMLAAAAAAAAJuZP3++pk2bpqqqKv3jH//40X99kwYWAAAAAACAzfz+97+Xz+fTN998o2HDhsU7nbjjK4QAAAAAkEC46TyAHyNmYAEAAAAAAMDWaGABAAAAAIB6GWPinQJsrLn3DxpYAAAAAAAgKqfTKUmqqqqKcyawM//+4d9fmhoNLAAAAAAAEFVSUpJSUlLkdruZhYWIjDFyu91KSUlRUlJSs7wGN3EHAAAAAAB1atu2rbZu3aotW7YoMzNTSUlJsiwr3mkhzowxqqqqktvtVmlpqTp27Nhsr0UDCwAAAAAA1CkjI0OSVFRUpK1bt8Y5G9hNSkqKOnbsGNhPmgMNLAAAAAAAUK+MjAxlZGSoqqpKXq833unAJpxOZ7N9bTAYDSwAAAAAABCzpKSkFmlYAMG4iTsAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGzNFe8EACSw776LdwbVunePdwYAAKCWNlttcp0gSX25VgCARMcMLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaN3EHAABAk/lgdbwzqDGqb7wzAAAATYUZWAAAAAAAALA1GlgAAAAAAACwNb5CCAAAAABoFnytGEBTYQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyt0Q2sTz/9VNdee6369Omj1q1bq3Pnzrrwwgu1bt26sGW/+eYbjR49Wunp6crOztZll12mH374obEpAAAAAAAA4DDmauwK7r//fn300UeaMGGC+vXrpx07duiJJ57QCSecoOXLl6tv376SpC1btui0005TZmamZs6cqdLSUj344IP66quvtGLFCiUnJze6GAAAAAAAABx+Gt3AuuGGG/T3v/89pAE1ceJEHXvssbrvvvv0wgsvSJJmzpyp/fv367PPPlPnzp0lSYMGDdJPfvITzZkzR1dccUVjUwEAAAAAAMBhqNFfIRw6dGjY7Kmjjz5affr00TfffBOIvfLKKzr33HMDzStJGjlypHr06KF58+Y1Ng0AAAAAAAAcpprlJu7GGO3cuVNt27aVJG3dulW7du3SgAEDwpYdNGiQVq5c2RxpAAAAAAAA4DDQ6K8QRjJ37lxt3bpVd911lyRp+/btkqT27duHLdu+fXsVFxeroqJCKSkpEddXUVGhioqKwL9LSkokSR6PRx6PR5LkcDjkcDjk8/nk8/kCy/rjXq9Xxph6406nU5ZlBdYbHJckr9cbU9zlcskYExK3LEtOpzMsR8uy5JTkM0a+4BwP5unz+eQLWrfDsuSwLHl9PpkY4k7Lqq7JF7yW6rgkeYNeUx5P/TUF5y7J6XCE5R4t3uQ1xbKdfL7ItUpyORzVNcWQe6NrqrWvRtz3pNi2Ux3xJqtJqn88HXysSfa9xtQUtB9EG2cJf4ygJmqiJmpKkJqMcR78P6Fxy1FdU2jckuVwyhifZHz1xy2HLMsRPe7zSkFnIp+v/ppCXzZy7tHiTV2Tx1P3djK+6LXKqq7J+EK3U3PV5PHUv++ZkPoPrseymiR+MPmY4tXvb93jqeYlmmbfa8x2Ch5q0caZ1PLjKVrcmLqPEdXLR641JNwCxwiO5dRETfGtqXZdDdXkDay1a9fqmmuu0ZAhQzRlyhRJUllZmSRFbFClpqYGlonWwJo1a5buvPPOsPjKlSvVunVrSVJubq66deumDRs2hPyyYadOndSpUyetW7dObrc7EC8oKFBeXp5Wr14dyE+SevXqpaysLK1cuTJkY/fr10/JyckqLCwMyWHAgAGqrKzUqlWrAjGn06mBAwfK7XZr7dq1gXhaWpr69++voqIirV+/PhDPzMxU76QkbXO7tSUox9z0dHXLydGGPXv0Q2lpTU2ZmeqUlaV1RUVyB+VekJOjvPR0rd6xQ2VVVTU15eUpKy1NK7duDWk+9WvfXskulwo3b64pqLi4/pqClk9LSlL/Dh1UtH+/1u/eXVNTWpp65+U1f02xbKf9+zUgP1+VHo9WHWymStXNj4H5+XKXl2vtrl3NX1NxcXVNde17UmzbSWr+mqT6x9P+/bFtp+auKWh7Z2Zmqnfv3tq2bZu2bNlSU5NlVW+n3bsjb6dduyLve9u2Ra5p8+ZDrykjo+HHiEg1Jfpxj5rqr6moqKamptj3/OOprCzyeCotjXyM2LtXW4IuONhO1FRXTWo1QMZbqaqimposy6nkdgNlKt2qKq6pyXKlKTm3v3xlRfK4a2pypGQqKbu3vKXb5C2tqcmZlitXVjd53RvkLaupyZneSa42neTZu06+ipqaitrVX1Pl3pqaktr2k+VMVuXO0JqSj2yZmgoL695OlfskV2aBnK3yVLV7tYynpqak7F6yUrJUtWuljGn+mgoP1L/vlXn3qNJXc85NdWYq1Zml/Z4ieUxN7mnOHKU401Xq2SGvqTnntnblKclKU0nVVpmgPxO2SWovh1xyV4Ue9zKT8uWTR/uqao57lhzKTM6vdzxV7ot9O8Wy7zVmOxUeqKkp2jFCaS0/nqLV5O5c9zEiXuMpUk2xHPd+2Fe9nRwpWarc0fjx5KuIXJP3QOSaPPtqasptw/mJmg6vmvyTkQ6VZYJbY420Y8cOnXzyyaqqqtLy5cvVoUMHSVJhYaEGDhyo5557TpdddlnIc26++WY98MADKi8vb9AMrPz8fO3evVsZGRmSDoOO54YN9piBVVBQf03ffluTu+I8A+uoo0JripT7+vX2mIFVUFAdr2vf+/57+8zA6tGj/vF08MAX9xlYXbvWxKP9BWH9+pYfT9HiBQW2/atISO6HyV96Erqm77+vybGlxlMM44ztRE115b7oG/vMwPpJ3/prWrQm+GXjOwPrjN51b6dFa6LX2tIzsM44pv597+P31oW+ZhxnYJ00qlud46lmP4j/DKwzjqkJRxtn/1prnxlYo46t+xjxwVf2mYF1Ru/6j3vV46xlx1O0+BnHcH6ipsOrppKSEuXk5Mjtdgd6OQ3RZDOw3G63zjrrLO3du1dLly4NNK+kmq8Obg/6K7Df9u3blZ2dHbV5JVXP3Ir0uMvlkssVWoL/TavNv2Fjjdde76HELcuKGI+Wo/8Dc8TlI7ymM8I66oq7osWDXzMo36g1NST35q4plu0R9FxXhFwsy4oYb/KaauUadd+LZTvVE2/SmuoaT7Uea9S+V0+8zppiGWcH/3+Ljqdo8YP5NvgY0cB4Qhz3qKnumiIsH7djRAPegx/ddooxx4bGE7WmwC5kRa4pctwhWeE5NjjuCM3dX3ZdNUVYTcQco8WbsiaXq+7tFPy02rXWxGPPPVo8lppCL7Ui72NWxDe36eI1Dav64/WNp9ov0dh9r/549O0RaahFO0a05HiKFveP+WjHiIbsk81dUyzHvdBx1jLjKVo8lnHG+YmaosXtWFO0/GPVJA2s8vJyjRkzRuvWrdPChQt1zDHHhDzesWNH5ebmhk8xl7RixQodd9xxTZEGAAAAAAAADkON/hVCr9eriRMnatmyZXr55Zc1ZMiQiMuNGzdOb7/9tjYH3aNj0aJFWrdunSZMmNDYNAAAAAAAAHCYavQMrBtvvFFvvvmmxowZo+LiYr3wwgshj1966aWSpNtuu00vv/yyRowYoV/84hcqLS3VAw88oGOPPVbTpk1rbBoAAAAAAAA4TDW6gfXFF19Ikt566y299dZbYY/7G1j5+fn68MMPdcMNN+jXv/61kpOTdc455+iPf/xjnfe/AgAAAAAAwI9boxtYS5YsiXnZPn366P3332/sSwIAAAAAAOBHpNH3wAIAAAAAAACaEw0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANiaK94JAACAw8R338U7gxrdu9f9eCLlimbVZquN9oW+de8LiZQrAABNjRlYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNVe8EwAAAAAAAA3zwep4Z1BjVN94Z4AfA2ZgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1rgHFgAAgM1xnxMAAPBjxwwsAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2BoNLAAAAAAAANgaDSwAAAAAAADYGg0sAAAAAAAA2Jor3gkAAAAAAIDD2wer451BjVF9450BDgUzsAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABga/wKIRps2ffxzqDGkO7xzgAAAAAAADQ3GlgAAAAAftTabP0u3inU6MtfaAEgEr5CCAAAAAAAAFujgQUAAAAAAABbo4EFAAAAAAAAW+MeWDZhlxujc1N0AAAAAMCP2Qer451BjVF9452BfTADCwAAAAAAALZGAwsAAAAAAAC2xlcIcdjj65kAAAAAACQ2ZmABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWXPFOAAAQwXffxTuDGt27xzsDAAAAAD9yzMACAAAAAACArTEDCwAA/Ogs+z7eGdQYwiRHAACAejEDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAttYkDazS0lLdcccdGj16tLKzs2VZlubMmRO23NSpU2VZVth/vXr1aoo0AAAAAAAAcBhyNcVKioqKdNddd6lz587q37+/lixZEnXZlJQUPfPMMyGxzMzMpkgDAAAAAAAAh6EmaWC1b99e27dvV7t27VRYWKiBAwdGf0GXS5deemlTvCwAAAAAAAB+BJrkK4QpKSlq165dzMt7vV6VlJQ0xUsDAAAAAADgMNfiN3E/cOCAMjIylJmZqezsbF1zzTUqLS1t6TQAAAAAAACQIJrkK4Sxat++vW6++WadcMIJ8vl8eu+99/Tkk0/qyy+/1JIlS+RyRU6noqJCFRUVgX/7Z295PB55PB5JksPhkMPhkM/nk8/nCyzrj3u9Xhlj6o07nU5ZlhVYb3Bcqp49Fkvc5XLJGBMStyxLTqczLEfLsiTpYB4mZD2W5ZAxPoWqvvl9U8Sr1bymx+Opt6ba66nOMVruzVtTLNup+rnhtR567odWU+19NeK+J8njC12P8+D+4TUmprjLUZ1jcNyS5HQ45DNGvhjijoP/1TueDj7msCw5LEteny/knXEe/KGGZq8paD+INs4cPl/NMSJo3dFyb9aaPJ6GHSNUx3ZqiZpiPB429LgXcTsl+LG8yWsKWr7FxlMM4yxqTca0/HiKVpPXW+d2ssM51x+vvY9J4fte9eosWQ5n9bpD1h8lbjlqaooU93lD84karx5Pxle9D/h3hWjjxhjnwf8TGrcc1TWFxpu3Jp+v/mOEqfW6B5NXqJa5jvBEGGfBufuvaZpq32tMTR6Pp97jXjzGU1011XUsD36NlriGraum4P0g2jiTWn48RYsbU/c5t3r54HTid4yI5TqiepiFHvfqy725avJ46r6OkA79WN7UNUn1XxsFym2m81NDagreXSNd7xmfPc65UvV+kHDXsFHOubWPEw3Vog2sWbNmhfx70qRJ6tGjh26//XbNnz9fkyZNivq8O++8Myy+cuVKtW7dWpKUm5urbt26acOGDfrhhx8Cy3Tq1EmdOnXSunXr5Ha7A/GCggLl5eVp9erVKisrC8R79eqlrKwsrVy5MmRj9+vXT8nJySosLAzJYcCAAaqsrNSqVasCMafTqYEDB8rtdmvt2rWBeFpamvr376+ioiKtX78+EK++iX2SKnxulXtrckx2pKuVK0dl3j2q9NXMUkt1ZirVmaX9niJ5TE3uac4cpTjTVerZIa+pCsRbu/KUZKWppGqrTNDH3DZJ7eWQS+6qzYFYYWFxvTUFL++0ktQmqYMqfftV5t0diLusNKUn5TV7TbFsJ3fVfmUm5csnj/ZVbQ/ELTmUmZwvjynXfs+uZq+psLBYUj37nqSVW7fKG3SA6Ne+vZJdLhVurnnfJWlAfr4qPR6t2l5Tk9Ph0MD8fLnLy7V2V01NaUlJ6t+hg4r279f63TU1ZaalqXdenra53doSND5y09PVTap/PO3fX11TTo7y0tO1escOlVXVbKdeeXnKSktr/pqCtndmZqZ69+6tbdu2acuWLTU1WZa65eRow549+iFo1menzEx1ysrSuqIiuYO2R7PW5HbXf4wIWk+d26klamqm417E7dQSx/ItWxq275WVRd73Sksjj6e9eyNvp927w7fTgAF111RUVFNTS42naMeIoP0g6nZyuVp+PEWrqayszn3PDudcScpMyldZWVm946lyn2S50pSc21++siJ53DU1OVIylZTdW97SbfKW1ownZ1quXFnd5HVvkLesZjs50zvJ1aaTPHvXyVdR8x64MgvkbJWnqt2rZTw1tSZl95KVkqWqXStljFeFBw5upyjXRm32Zkc852Yk56vKVxbxnFvhLY14zi337o24nQ54dkfcTqVVu0K2U1G7Y+s9Rriram5rUdd2aonriOD3MtJxz121v0n3vcbUVFhYXO+xPB7jKVpN9Z2f3FX7Y95OzV2T/5pRin7OVdpAmUq3qopraorXMcLdue7PT75NH8a0nVriGLHOWVXvdUTlvvDjnl9S236ynMmq3Bl63Es+coCMt1JVRTXbybKcSm7XuO1UeKDuayPp0I/lTV2TVP/1XuW+6nhznZ8aUpP/XBbtGraqzB7nXKl6P2jufkRLXZc39lZSljGm9p8uGsV/E/fZs2dr6tSp9S5fVlam9PR0TZs2LezXCf0izcDKz8/X7t27lZGRISnx/2q/YuEGW/w1eNDIgnprWvb+txFyjM8MrIFnHBUSjZT7ioXrI9Z66LkfWk2DRhZIqmff+/57+8zA6tGj/vF08MAX9xlYXbvWxKP9BWH9evvMwCooqP8Y8d13kWuNxwysoPdXSry/9ITl/t13LT+eom2no4+uu6bvvw/JMa4zsIL2g6jbacMG+8zA6tatzn3v4/e+VbzPuf74kDO71zueFq05uG4b/DX4jGOqw9GOBSsWbohYa0uec/1OGtW93mNE9XVCzXoi5d5S1xH+awUp8vHNf01jhxlYg0YW1Hss//i9dTHn2Nw1nTSqW53np+D9IN4zsIL3g2jj7F9r7TMDa9SxdX9+qv3ZIZ7X5YNGdq33OmLRGtlmBtYZx9R9bbRwjX1mYJ3Zr/7rvepzmZps32tMTf5zmRT5GnbRGnucc6Xq/eBwmYFVUlKinJwcud3uQC+nIVp0BlYkaWlpysnJUXFxcdRlUlJSlJKSEhZ3uVxhXzv0v2m1+TdsrPFoX2dsSNyyrIjxaDlWf5XQihCPfKuypooHv2ZwvtFqirSe6Lk3b02xbI/Q5zYkx6atqXaukfa9Zd9L0W9NF/6a0eORc2xIfEiPGMZTrcecEZaVqj9cRoxbkWuKFLcsK2LcYVlyxDLODv5/h8MR8R2Olnuz1HQw34YeI/xNgIjLR3jNJqupGY97DY03ybE8yr4kHcK+15B4tO1UV00R3oNmH0+NGWcHn9ui4ynw0rVqOvi+2vmcG5xLfePJCnmbHaGBQ407Iu970ePVudROtXbuVmA7xO+c6+ff9nUdIyKvK/ZzblPWFGk/CM49ONem2PeixWPJPTjX6OOs5cdTtHh956farxHPY0SkPKMdI2RFirfsMcI/5KNdLzT0eNicx4hYriNCjreOKB+XI7zv0eKN2U7Bb2nUcXaIx/LwBxpfU33XdbXLberzU/gD0eO1d9faxwh/WvE+50qh+0GiX5dHyz9WLX4T99r27dunoqIi5ebmxjsVAAAAAAAA2FCLNbDKy8u1b9++sPjdd98tY4xGjx7dUqkAAAAAAAAggTTZVwifeOIJ7d27V9u2bZMkvfXWW4EbgF133XXas2ePjj/+eF100UXq1auXJOn999/XO++8o9GjR+u8885rqlQAAAAAAABwGGmyBtaDDz6oTZs2Bf796quv6tVXX5UkXXrppcrKytK5556rBQsW6Nlnn5XX61X37t01c+ZM/epXv4r4nUoAAAAAAACgyRpYGzdurHeZ559/vqleDgAAAAAAAD8STHsCAAAAAACArdHAAgAAAAAAgK3RwAIAAAAAAICt0cACAAAAAACArTXZTdwBAMCP27Lv451BjSHd450BAAAAmhIzsAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBr3MQdAADA5tps/S7eKdToyx3yAQBAy2MGFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABszRXvBAAAQGTLvo93BjWGdI93BgAAAPgxYwYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbM0V7wQAJK5l38c7g2pDusc7AwAAAABAc2IGFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABszRXvBAAAaEnLvo93BjWGdI93BgAAAEBiYAYWAAAAAAAAbI0GFgAAAAAAAGyNBhYAAAAAAABsjQYWAAAAAAAAbI2buAMAAABAAmmz9bt4p1CjL79IAqBlMAMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALZGAwsAAAAAAAC2RgMLAAAAAAAAtkYDCwAAAAAAALbWJA2s0tJS3XHHHRo9erSys7NlWZbmzJkTcdlvvvlGo0ePVnp6urKzs3XZZZfphx9+aIo0AAAAAAAAcBhyNcVKioqKdNddd6lz587q37+/lixZEnG5LVu26LTTTlNmZqZmzpyp0tJSPfjgg/rqq6+0YsUKJScnN0U6AAAAAAAAOIw0SQOrffv22r59u9q1a6fCwkINHDgw4nIzZ87U/v379dlnn6lz586SpEGDBuknP/mJ5syZoyuuuKIp0gEAAAAAAMBhpEm+QpiSkqJ27drVu9wrr7yic889N9C8kqSRI0eqR48emjdvXlOkAgAAAAAAgMNMi93EfevWrdq1a5cGDBgQ9tigQYO0cuXKlkoFAAAAAAAACaRJvkIYi+3bt0uq/rphbe3bt1dxcbEqKiqUkpIS9nhFRYUqKioC/y4pKZEkeTweeTweSZLD4ZDD4ZDP55PP5wss6497vV4ZY+qNO51OWZYVWG9wXJK8Xm9McZfLJWNMSNyyLDmdzrAcLcuSpIN5mJD1WJZDxvgUypJlWU0Sr1bzmh6Pp96aaq+nOsdouTdvTbFsp+rnhtd66LkfWk2199VI+15NvqHriZR7c9ckqd7xVJNr4/e9xtQUvB9EG2cOn6/mGBG0DodlyWFZ8vp8IWuPFndaB/c9X2hNzoPj2GtM/XGPp2HHCElOh0M+Y+QLPo5JLVNTjMfDhh73Im6nFjiWR97f43OMkFRPTb6Q5VtiPMUyzqJtJ2NMs52fGlqT1+utc9+zwznXH689bqTw8eRfXzzPubXPZ9GOBTX7c/zOuX6+g8f+uo4RtcdZpNxb6hgRaZwF5+6/ponnOdcf93g89R7L4zGe6qqprvNT8Gu05HiKlHvwfhBtnEl1fXZo2WOE/9gf7bo81u3XEseIWK4jqodZ9THC+Dy1VuM8mLo3prjlqD6Wh8YtWQ5ndY61z/O14h5P3ddGkkPG5w19DyxH9XsQFm/emqT6r/dqPjo4arZT8HsQNfemryl4d410DWt8sW+n5q7J42n+fkRLXZfXPk40VIs1sMrKyiQpYoMqNTU1sEykx2fNmqU777wzLL5y5Uq1bt1akpSbm6tu3bppw4YNIb9q2KlTJ3Xq1Enr1q2T2+0OxAsKCpSXl6fVq1cHcpOkXr16KSsrSytXrgzZ2P369VNycrIKCwtDchgwYIAqKyu1atWqQMzpdGrgwIFyu91au3ZtIJ6Wlqb+/furqKhI69evD8QzMzMlJanC51a5tybHZEe6WrlyVObdo0pfac375cxUqjNL+z1F8pia3NOcOUpxpqvUs0NeUxWIt3blKclKU0nVVpmgj7ltktrLIZfcVZsDscLC4nprCl7eaSWpTVIHVfr2q8y7OxB3WWlKT8pr9ppi2U7uqv3KTMqXTx7tq9oeiFtyKDM5Xx5Trv2eXc1eU2FhsaS69z1JMW0nSc1ek6R6x5O7an9M26m5awre3pmZmerdu7e2bdumLVu2BOK5lqVuOTnasGePfiit2U6dMjPVKStL64qK5A7aHgU5OcpLT9fqHTtUVlVTU6+8PGWlpWnl1q3yBh3I+7Vvr2SXS4WbQ2sakJ+vSo9Hq7bX1OR0u+s/RgStJzMtTb3z8rTN7daWoONYbnp6y9RU33Fv/345HQ4NzM+Xu6xMa3fVbKe0pCT179BBRaWlWr+7Zt8L1LR3b+Sadu+OXNOuXZFr2ratuqaD54S6juWSafHxFO0YIanO85O7qigQb6nxFK2m4P0g2jm3wudqtvNTQ2tavbos6jm3d+/etjjn+msqKyur9zrCXbU/7udcf03+81m0ayMpO+7nXL+ioqx6r/fcVSUxbaeWqCn4vYx0Deuu2h/3c66/psLC4ujn3IPHiHiMp2g11Xdd7r+maenxFKkm/xiTon/WkI5o8fEUrSa3O6/Oz092OeemOrNi+kxYuU9Kyu4lKyVLVbtWygQ1QZLa9pPlTFblztDjXvKRA2S8laoqqtlOluVUcruBMpVuVRXX7HuWK03Juf3lKyuSx11zfnKkZCopu7e8pdvkLa0eT4UH6v6c2+2Df2nnESkqT3EG4tnuSrUp82hb21RVuWq+cJVXXK60Sp/+d2SajGUF4u2LyuTyGm0+slVITfk7D8jjtLS9bVpN7sao884ylSU7tCs7teZ98fikfhdGPef6jxGV+6rjzrRcubK6yeveIG9ZTU3O9E5ytekkz9518lXUbCdXZoGcrfJUtXu1jKdmn2zMdio8cPA1o3x2ryqLfTs1d02FB5q/H1HXsbwpeyz+yUiHyjLBrbEm4L+J++zZszV16tSw+HPPPafLLrss5Dk333yzHnjgAZWXl8c8Ays/P1+7d+9WRkaGpMSfgbVi4QZb/DV40MiCemta9v63EXKMz1+DB55xVEg0Uu4rFq6PWOuh535oNQ0aWSCp7n1v+Qff22YG1tDRPeodT9XvbXit0d6D5qpp0MiuQbEof0FYv94+M7AKCuo/Rnz3Xci7EtcZWF27hsZrj7ODJ0CX4+BfuINyjJZ7s9VUUBDIMdqxfNn738kuM7CGjj66zvPTJwu+D1k+njOwgsdZtHPuioUbbDMDa/BPutX5V8aP3/s2ynpafsbIkDO713sd4T/e2mEGlv98Fu16YcXCDRFrjccMrJNGda/3eq/mXFa9nki5t9Qxwv/eSpGvF/zXNHaYgTVoZEG9f7X/+L11MefY3DWdNKpbndflwftBvGdgBe8H0cbZp4s22mYG1pAzj67z81Ptzw7xvC4fNLJrvZ8JF61RxFkw1atp2RlYZxxT9+fcDY+8IJ+lEJapfocbEpckE2PcYarf8drxo385ud6ZPYvWBN6YuM/AOuOYmnCk6/JFa+wzA+uMYw6fGVglJSXKycmR2+0O9HIaosVmYPm/Org9aBaC3/bt25WdnR2xeSVVz9qK9JjL5ZLLFVqC/02rzb9hY43XXu+hxC3LihiPlmP1VwmtCPHItyprqnjwawbnG62mSOuJnnvz1hTL9gh9bkNybNqaaucabd+LZTvVF2+qmuobT7Vzbcy+V1+8rtxjGmcH/7/D4Yh48z9nhDrriruixa3INYXED+bb0GOEv1kTcfkIr9lkNdU3zoKeZ1lWxPcgau5NXVOtXKMdx+IxnqKNg7rOT5GPt/E5RsSyr/q/Et8c56f64rVz97+vdj7nBudS33VE8Pridc6Ndj6r/W8rMKbjd87182/7uq73Iq8rPseISPtBcO6h+0F8zrn+eHCu0cdZy4+naPH6jmPh1zTxO0ZEyrMh57OWPkb4x3y064WGHg/jdc4NPDfoqZYjysdlK/a4ZVlR4o7QF4sQD35Lo14fRpmO0tC41YC4FSUeNUf/OKv1UNT3wBHlc1LUeMO3U+3dtfYxwp9WLNsppngjagrOtTn7EQ2NH0qPJVr+sWqxBlbHjh2Vm5sbYZq5tGLFCh133HEtlQqAH6Fl39e/TEsZ0j3eGQAAAABAYmmxXyGUpHHjxuntt9/W5qB7uyxatEjr1q3ThAkTWjIVAAAAAAAAJIgmm4H1xBNPaO/evdq2bZsk6a233grcAOy6665TZmambrvtNr388ssaMWKEfvGLX6i0tFQPPPCAjj32WE2bNq2pUgEAAAAAAMBhpMkaWA8++KA2bdoU+Perr76qV199VZJ06aWXKjMzU/n5+frwww91ww036Ne//rWSk5N1zjnn6I9//GPU+18BAOyNr2cCAAAAaG5N1sDauHFjTMv16dNH77//flO9LAAAAAAAAA5zLXoPLAAAAAAAAKChaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1mhgAQAAAAAAwNZoYAEAAAAAAMDWaGABAAAAAADA1lzxTgAAEG7Z9/HOoMaQ7vHOAAAAAMCPHTOwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrNLAAAAAAAABgazSwAAAAAAAAYGs0sAAAAAAAAGBrrngnAAAAAACAHbTZ+l28U6jRt3u8MwBshRlYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsDUaWAAAAAAAALA1GlgAAAAAAACwNRpYAAAAAAAAsLUWbWAtWbJElmVF/G/58uUtmQoAAAAAAAAShCseLzpjxgwNHDgwJNa9e/d4pAIAAAAAAACbi0sD69RTT9X48ePj8dIAAAAAAABIMHG7B9a+ffvk8Xji9fIAAAAAAABIEHFpYE2bNk0ZGRlKTU3ViBEjVFhYGI80AAAAAAAAkABa9CuEycnJGjdunM4++2y1bdtWa9as0YMPPqhTTz1VH3/8sY4//viIz6uoqFBFRUXg3yUlJZIkj8cTmMXlcDjkcDjk8/nk8/kCy/rjXq9Xxph6406nU5Zlhc0OczqdkiSv1xtT3OVyyRgTErcsS06nMyxHy7Ik6WAeJmQ9luWQMT6Fqr7xfVPEq9W8psfjqbem2uupzjFa7s1bUyzbqfq54bUeeu6HVlPtfTXSvleTb+h6IuXe3DVJqnc81eTa+H2vMTUF7wfRxpkxvhYfT9HiHo+n3mNEw8ZZ89ZU3zjzP68lx1O0uD/Xuo7lkff3+BwjJNVzfvKFLN8S4ymWcRbtnGuMafHxFC13r9cb9ZwbbT+I1zGi9rFACr+OaNw4a9qagseZFH69ULM/x++c6+fz+eq93qs9ziLl3lLHiEjjLDh3/zVNPM+5/rjH44l6zvXnbodzbnDudV2XB79GPM+5UujxNto4k+r67NCyxwj/sT/a9UKs268ljhGxfCasb5xFyr25avJ4PHV+zpUkn6XQdZjqbBoSlyQTY9xhqrOrHZfCPzuEjbPARwdHzXYKfo/9cZ9XIe9N1Hj1sdz4an2zy3IeTN4bNR68u0a6Ljc+S5bDGZ6josSbsSaPp/n7EXUdy5uyx9LYb+G1aANr6NChGjp0aODfY8eO1fjx49WvXz/deuuteu+99yI+b9asWbrzzjvD4itXrlTr1q0lSbm5uerWrZs2bNigH374IbBMp06d1KlTJ61bt05utzsQLygoUF5enlavXq2ysrJAvFevXsrKytLKlStDNna/fv2UnJwcNltswIABqqys1KpVqwIxp9OpgQMHyu12a+3atYF4Wlqa+vfvr6KiIq1fvz4Qz8zMlJSkCp9b5d6aHJMd6WrlylGZd48qfaWBeKozU6nOLO33FMljanJPc+YoxZmuUs8OeU1VIN7alackK00lVVtlVLPjtUlqL4dccldtDsQKC4vrrSl4eaeVpDZJHVTp268y7+5A3GWlKT0pr9lrimU7uav2KzMpXz55tK9qeyBuyaHM5Hx</t>
         </is>
       </c>
     </row>
@@ -585,29 +585,29 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45656.95833333334</v>
+        <v>45657.875</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>9.743513192330049</v>
+        <v>9.905910129317759</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>45656.95833333334</v>
+        <v>45657.875</v>
       </c>
       <c r="H4" t="n">
-        <v>4.692596968675582</v>
+        <v>4.970275733960977</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.14331891032121</v>
+        <v>-0.1060689800844212</v>
       </c>
       <c r="J4" t="n">
-        <v>9.743513192330049</v>
+        <v>9.905910129317759</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACGOElEQVR4nOzdeXxTdfb/8fdN0o2WtlIoWwu0ZRUERBZBVnUQEHAUEB2VRfy6jaI/HZ1xRVDAbRTFcRtHcBRHEccRVBRQGBERZGRVsCgFgbKVJaWlW5r7+6M0bWjSBWhyA6/n49EH9OTm3nNyt+T0c28M0zRNAQAAAAAAABZlC3YCAAAAAAAAQGVoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAGAhLVq0kGEYXj8RERFq1qyZRo8ereXLlwckj3HjxskwDM2ePTsgy6stpa/n9u3bg53KGa90ewUAAKgNNLAAALCgiy66SGPHjtXYsWM1ePBgud1uzZ07V/369dNzzz0X7PQsIZSabIFspM2ePVuGYWjcuHG1viwAAIBAcQQ7AQAAUNFNN93k1YDIz8/XLbfcon/+85+6//77NXToULVu3Tp4CYaIL7/8UkVFRWratGmwUwEAAMApYAQWAAAhIDIyUn/7298UHR2t4uJi/fvf/w52SiEhLS1Nbdu2VVhYWLBTAQAAwCmggQUAQIiIiYlRmzZtJKnCpWhffPGFhg4dqsTERIWHh6tJkyYaPXq01qxZ43d+hw4d0t13363mzZt77rN1xx136NChQyeV32OPPSbDMPTYY49px44dGjNmjBo3bqzIyEi1bt1ajz32mPLy8io8r6ioSO+8846uu+46tW3bVrGxsYqKilKbNm00ceJEZWZmek2/fft2GYaht956S5I0fvx4r3uGPfbYY55pq7p0b968eRo0aJAaNGig8PBwNW3aVNdff71++umnCtOWLrdFixYyTVOvv/66LrjgAkVHRysuLk4DBw7UypUrvZ5Tejnfjh07JEkpKSleuS5btswz7ZIlSzRs2DA1bNhQYWFhOuecc9SqVStdf/31+vrrr6uzCtSiRQuNHz9ekvTWW295Lat///5e0x47dkxPPvmkunTporp166pOnTpq3769Hn74YR0+fLhay/Pn73//u+e1iY+P15AhQ/Tdd9/5nd7lcumNN95Q//79Va9ePUVERCglJUW33Xabdu7cWePl/+9//9Po0aOVlJSk8PBwxcbGKjU1VSNGjNDHH3/s9znXXXedmjVrpoiICNWrV0+XXXaZPvvss9OW97JlyzzroqioSE899ZTat2+vqKgoJSQk6KqrrtLmzZtrXC8AAGcDLiEEACCEZGdnS5IiIiI8sUceeURPPPGEDMNQr1691KxZM23evFlz587Vhx9+qNdff1033nij13z27dunPn36aOvWrTrnnHM0dOhQud1uzZkzR59//rnat29/0jlmZGToggsukMPhUN++fZWXl6elS5dq8uTJWrJkiZYsWaLIyEivXG644QbFxcWpXbt26tixo3Jzc7Vu3TrNnDlT7733nr799lu1bNlSUkkjb+zYsfrmm2/066+/6qKLLvI8JkmdO3euMkeXy6XrrrtOc+fOVUREhC644AI1bdpU6enpmjNnjv7973/r3//+twYNGuTz+ePHj9e7776rPn36aOjQoVq3bp0WL16sr7/+Wv/973/Vo0cPSVLLli01duxYzZs3T7m5uRoxYoRiYmI882nUqJGkkmZTaeOpe/fuGjBggPLy8rRr1y699957ql+/vvr27VtlXSNHjtR3332nFStWKC0tTb179/Y81rZtW8//Dx06pEsuuUTr1q1TbGysLr74YoWFhem///2vpk6dqnfffVdfffWVWrRoUeUyT3TPPfdoxowZuuiii3TFFVdo48aNWrhwoRYvXqy5c+fqyiuv9Jr+6NGjGj58uJYtW6aYmBhdcMEFatCggTZu3KhXX31VH3zwgRYvXqzzzz+/Wsv/8ssvNXjwYBUVFalTp07q2bOniouLtXv3bn366acqLi7WFVdc4fWcF154Qffcc4/cbrc6d+6sHj16aO/evVq2bJkWLVqkyZMn69FHHz1teRcVFWnIkCH69ttv1bdvX7Vr106rV6/WRx99pKVLl2rt2rUn9doDAHBGMwEAgGU0b97clGTOmjWrwmPr1683bTabKcl88803TdM0zYULF5qSzMjISHPRokVe07/xxhumJDMsLMzctGmT12MjR440JZl9+vQxjxw54okfPHjQ7NGjhynJbx7+TJo0yfO8K664wjx27JjnsZ07d5qtW7c2JZl/+ctfvJ6XnZ1tfvzxx2ZBQYFXvLCw0HzggQdMSeaQIUMqLG/s2LFV5lj6emZkZHjFH3zwQVOS2aNHD3Pbtm1ej33wwQem3W43zznnHPPw4cOeeEZGhqe+5s2bmz///LPnMZfLZd54442mJHPgwIHVzqNUSkqKKclcvnx5hcf27dtn/vDDD35rPNGsWbNMSebYsWP9TjN69GhP/VlZWZ740aNHzcGDB5uSzF69elV7maZpel6bqKgo88svv/R67OmnnzYlmXFxcea+ffu8HvvDH/5gSjKHDh1a4bHnn3/elGS2atXKdLlc1cpjwIABpiTznXfeqfDYkSNHzJUrV3rFPv/8c9MwDLN+/frmf//7X6/HNmzYYCYlJZmSzGXLlp1y3kuXLvW8Tueff765Z88ez2N5eXnmZZddZkoyb7755mrVCgDA2YQGFgAAFuKrgXXkyBHz008/NdPS0kxJZpMmTcycnBzTNE3zkksuMSWZ99xzj8/5DR061JRk/t///Z8n9ttvv5k2m800DMP88ccfKzxn7dq1p9TAioqK8vpgXmrBggWmJDM2NtbMy8ur9nybNGli2mw2Mzs72yt+sg2sgwcPmlFRUWZkZKS5a9cun8+7/fbbTUnmzJkzPbHyDaz58+dXeM6ePXtMSWZERIRZWFhYZR7l1alTx4yLi/NbR01U1cDasWOHZ/2vX7++wuO7du0yIyMjTUnmihUrqr3c0tfm7rvv9vl4165dTUnm1KlTPbGffvrJNAzDbNKkSYX1W2rIkCGmJHPBggXVyuPcc881JZmHDh2q1vSlDdt58+b5fHzu3LmmJHPEiBGnnHdpA8swDHPdunUVnvPdd9+ZkszU1NRq5Q4AwNmEe2ABAGBB5e/rFB8fr8svv1y//vqr0tLS9Nlnnyk6Oloul0srVqyQJK9vLCxvwoQJkqSlS5d6Yl9//bXcbre6dOmic889t8JzOnfurI4dO5507gMHDvRcGlfe0KFDlZCQoOzsbP3www8VHl+/fr2ee+453Xnnnbrxxhs1btw4jRs3Ti6XS263W7/88stJ51Te0qVLlZeXp4suusjvtxOW3i/q22+/rfCYw+HweWlho0aNdM4556igoEAHDx6sUU7du3eX0+nUmDFj9L///U9ut7tGz6+J0vV//vnn+1zPTZs21WWXXSbJe7uprrFjx/qMjxkzRpK87vv12WefyTRNDR48WHXr1vX5vMrWhS/du3eXJF133XX65ptv5HK5/E6blZWl1atXKyoqSsOGDav28k8172bNmqlTp04V4u3atZMk7d6922/OAACcrbgHFgAAFlT+vk7h4eFKTEzUhRdeqEGDBsnhKDl9Hzx4UPn5+ZJKbg7uS1pamiTvD8S7du2q9Dmlj23YsOGkcq9svi1atNDBgwc9OUhSbm6ubrjhBn300UeVzrf0/l+natu2bZJK7pVkGEal0x44cKBCrHHjxn6/1TA2NlaHDx/2rJfqevnllzV06FC9/fbbevvtt1W3bl1169ZNF198sW644QY1a9asRvOrTOm2UNl68rXdVJe/+ZbGy6/70nXxj3/8Q//4xz8qna+vdeHL9OnTtWHDBi1cuFALFy5UVFSUunTpov79++u6667zNImkkvu1maapvLw8r/vKVbX8U83b3/qMjY2VJBUUFFQ6TwAAzkY0sAAAsKCbbrrJ76iqM4Fpmp7/P/DAA/roo4/Utm1bPfnkk+rWrZvq16+v8PBwSVKvXr20cuVKr+ecitLRTS1bttRFF11U6bTlb3xeymY7/QPY27Vrp59//lmLFi3SV199pW+//VbLly/XV199pSlTpugf//iHrr/++tO+3GAovx5L10Xnzp19jkgqr/TG+FVp1KiR1qxZo//+979asmSJVqxYoVWrVmnFihWaNm2apk+frj//+c9ey4+JidGIESOqXcOp5l0b2xAAAGc6GlgAAISohIQERUREqKCgQNu2bfN5OVjpSJHyl8qV/n/79u1+513ZY1XJyMiocr5JSUme2Ny5cyVJ77//vs8atm7detK5+JKcnCxJatOmjWbPnn1a530qHA6HhgwZoiFDhkgqGXH23HPPafLkybrlllt05ZVXKjo6+pSXU7r+S7cNX3xtN9WVkZHh85sgfa370nVx0UUX6aWXXqrxsvwxDEP9+/f3XMaXn5+v2bNn649//KMefPBBjRw5UmlpaZ7lG4ahN998s9qNpdrKGwAA+MeffwAACFEOh0O9e/eWJL+NmDfffFOSNGDAAE+sb9++MgxDP/zwg7Zs2VLhOevXrz/pywcladGiRdq/f3+F+GeffaaDBw+qbt26uuCCCzzxQ4cOSZKaN29e4TlffPGFsrKyfC6ndIRWZfc48uWSSy5ReHi4li1b5jPP2nAyucbGxuqxxx5TfHy8jh07pvT09NOyrL59+8pms2ndunVav359hcf37Nmjzz//XJL3dlNdb7/9dqXx0qaSJA0ePFiSNH/+/BpfdlkTkZGRuvXWW9WxY0e53W7P9t2kSRN17NhRR48e9dRcHYHKGwAAlKGBBQBACLv33nslSa+88oq+/PJLr8dmz56t+fPnKywsTHfddZcn3qxZM1155ZVyu9267bbbvO4tdfjwYd1+++2ndLleXl6ebrvtNuXl5XlimZmZnlxvvfVWRUZGeh4rvSfRzJkzvebz888/69Zbb/W7nNKRPD/++GON8mvYsKHuvPNO5ebmatiwYdq4cWOFaQoKCjR//nyfDb6TUVmux44d03PPPefzXknLly/XkSNHZLfbvUYuVWdZP/30k8/HmzVrplGjRsk0Td1yyy1eN5zPzc3VzTffrPz8fPXq1Uu9evWq1jLLe+WVV7xu1C5Jzz//vFavXq26det6vlhAks4//3yNGDFCO3fu1FVXXeVz5F9ubq7mzJmjffv2VWv5zz77rH777bcK8S1btnhG85Vvlj7xxBOSSr44YcGCBRWeZ5qmVq1apUWLFtVq3gAAoHJcQggAQAgbPHiwHn74YT3xxBP63e9+p4suukjNmjXTli1b9MMPP8hut+vVV19V+/btvZ73t7/9TevXr9eyZcuUkpKi/v37yzRNLV26VAkJCRo+fLjmz59/UjmNGTNGn3zyiVJTU9WnTx/l5+frq6++Um5urnr27KnJkyd7TT9p0iSNHDlSjzzyiObOnav27dtr//79Wr58ufr06aMmTZr4/Ca33//+95o8ebJefPFFbdq0ScnJybLZbBo+fLiGDx9eaY5PPvmk9uzZo3fffddzH6PU1FQ5HA7t2rVL69atU25urhYuXOjzPlg1NWLECC1dulTXX3+9Bg4cqHPOOUeSdN9996lhw4a69957dd999+m8885Tq1atFBYWpu3bt+u7776TJD300ENq0KBBtZZ14YUXqkmTJlq7dq26dOmi8847T2FhYWrTpo3uu+8+SSXrf8uWLVq1apXS0tI0YMAAORwO/fe//9WBAweUkpKiOXPmnFStt9xyiy6++GL16dNHTZs21aZNm7Rx40bZ7Xa9+eabFb6hctasWTpy5IgWLlyoNm3aqFOnTkpJSZFpmtq+fbvWr1+vwsJCbd68WQ0bNqxy+U888YTuu+8+tW3bVu3atVNUVJQyMzM930g4ZswYdenSxTP9sGHD9MILL+jee+/V8OHD1bJlS7Vp00ZxcXE6cOCA1q9fr/379+vPf/6zBg4cWGt5AwCAKpgAAMAymjdvbkoyZ82aVaPnLVy40BwyZIiZkJBgOhwOs1GjRuaoUaPMVatW+X1OVlaWeeedd5pJSUlmeHi4mZSUZN56663mgQMHzLFjx9Y4j0mTJpmSzEmTJpnbtm0zr732WrNhw4ZmeHi42bJlS/PRRx81c3NzfT7366+/Ni+55BKzfv36Zp06dcwOHTqYU6dONQsKCsx+/fqZksylS5dWeN5HH31kXnTRRWbdunVNwzA8yy9V+npmZGT4XO5nn31mXnXVVWbTpk3NsLAwMz4+3mzXrp15zTXXmO+++65XvhkZGaYks3nz5n5fA3/LKy4uNqdPn262b9/ejIyMNCV5aioqKjJfffVV89prrzXbtm1rxsXFmVFRUWZaWpo5YsQI88svv/S7PH82btxoDh8+3GzQoIFps9lMSWa/fv28psnNzTWnT59udu7c2axTp44ZGRlptmvXznzwwQfNQ4cO1XiZpTWZpmm+8sorZufOnc2oqCgzNjbWHDRokLlixQq/zy0uLjbfffddc8iQIWbDhg3NsLAwMyEhwezQoYM5fvx486OPPjILCwurlcc777xjjh8/3uzQoYNZr149MyIiwmzevLk5ePBg86OPPjLdbrfP523cuNG8+eabzVatWpmRkZFmnTp1zNTUVPOyyy4zX3zxRXP37t2nnPfSpUt9rgt/ryMAAChjmOZp+kofAABwVnvsscc0efJkTZo0SY899liw0wEAAMAZhHtgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0rgHFgAAAAAAACyNEVgAAAAAAACwNBpYAAAAAAAAsDRHsBM4GW63W5mZmapbt64Mwwh2OgAAAAAAAKiEaZo6evSomjRpIput5uOpQrKBlZmZqeTk5GCnAQAAAAAAgBrYuXOnkpKSavy8kGxg1a1bV1JJ0bGxsUHOBgAAAAAAAJXJzs5WcnKyp6dTUyHZwCq9bDA2NpYGFgAAAAAAQIg42VtBcRN3AAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFhaSH4LIQAAAAAACDzTNFVcXCyXyxXsVGARDodDdrv9pL9dsNrLqdW5AwAAAACAkGeapo4cOaIDBw6ouLg42OnAYux2uxITExUXF1drjSwaWAAAAAAAoFJ79+7VkSNHFBsbq9jYWDkcjlofcQPrM01TLpdL2dnZ2rNnj/Ly8tS4ceNaWRYNLAAAAAAA4FdxcbGcTqcaNGig+vXrBzsdWFDdunUVERGhrKwsJSYmym63n/ZlcBN3AAAAAADgV1FRkUzTVHR0dLBTgYVFR0fLNE0VFRXVyvxpYAEAAAAAgCpxySAqU9vbBw0sAAAAAAAAWBoNLAAAAAAAAPg0btw4tWjRIthp0MACAAAAAABnr9mzZ8swDL8/3333XbBTrNJPP/2kxx57TNu3bw92KrWGbyEEAAAAAABnvSlTpiglJaVCvGXLlkHIpmZ++uknTZ48Wf3797fEaKnaQAMLAAAAAACctEWbgp2BNLDDqc9j8ODB6tq166nPCLWCSwgBAAAAAAAqMWnSJNlsNn355Zde8Ztvvlnh4eFav369JGnZsmUyDEPvv/++HnzwQTVq1EjR0dEaPny4du7cWWG+q1at0qBBgxQXF6c6deqoX79+WrFiRYXpdu/erQkTJqhJkyaKiIhQSkqKbrvtNhUWFmr27NkaNWqUJGnAgAGeSx+XLVvmef7ChQvVp08fRUdHq27durr88sv1448/VljOf/7zH3Xo0EGRkZHq0KGDPvroo1N52U4rRmABAAAAAICzntPpVFZWllfMMAwlJCTo4Ycf1oIFCzRhwgRt3LhRdevW1RdffKG///3vevzxx9WpUyev502dOlWGYejPf/6z9u/frxkzZujSSy/VunXrFBUVJUn66quvNHjwYF1wwQWeBtmsWbN08cUXa/ny5erevbskKTMzU927d9eRI0d08803q23bttq9e7fmzZunY8eOqW/fvpo4caJefPFFPfjgg2rXrp0kef59++23NXbsWF122WV66qmndOzYMb3yyivq3bu31q5d67nkcNGiRRoxYoTOPfdcTZ8+XQcPHtT48eOVlJRUmy97tRmmaZrBTqKmsrOzFRcXJ6fTqdjY2GCnAwAAAADAGSs/P18ZGRlKSUlRZGRkhcdD/RLC2bNna/z48T4fi4iIUH5+viRp06ZNuuCCCzRmzBg988wz6tChgxo3bqyVK1fK4SgZH7Rs2TINGDBATZs21ebNm1W3bl1J0gcffKCrr75aL7zwgiZOnCjTNNWmTRulpqZq4cKFMgxDkpSXl6f27durZcuWWrRokSRp7Nixeuedd7Rq1aoKlziapinDMDRv3jyNGjVKS5cuVf/+/T2P5+TkKDk5WaNGjdLrr7/uie/bt09t2rTR1Vdf7Ymff/752rdvnzZv3qy4uDhJ0uLFizVw4EA1b968yhvEV7WdnGovhxFYAAAAAADgrPe3v/1NrVu39orZ7XbP/zt06KDJkyfrgQce0IYNG5SVlaVFixZ5mlfljRkzxtO8kqSRI0eqcePG+uyzzzRx4kStW7dOW7du1cMPP6yDBw96PfeSSy7R22+/LbfbLanksr5hw4b5vD9XaePLn8WLF+vIkSO69tprvUaX2e129ejRQ0uXLpUk7dmzR+vWrdNf/vIXT/NKkn73u9/p3HPPVW5ubqXLCQQaWAAAAAAA4KzXvXv3Km/ift999+m9997T6tWrNW3aNJ177rk+p2vVqpXX74ZhqGXLlp5RTFu3bpVUMrrKH6fTqcLCQmVnZ6tDh5MbYla6nIsvvtjn46UjoXbs2OEzb0lq06aNfvjhh5Na/ulEAwsAAAAIBb/8EuwMyoTAV8oDQG3Ytm2bpym0cePGk55P6eiqZ555Rp07d/Y5TUxMjA4dOnTSyyi/nLfffluNGjWq8Liv0WNWFTqZAgAAAAAABInb7da4ceMUGxuru+++W9OmTdPIkSN11VVXVZi2tMlVyjRN/fLLL+rYsaMkKS0tTVLJCKhLL73U7zIbNGig2NhYbdpU+Y3G/F1KWLqcxMTESpfTvHlzn3lL0s8//1zpsgPFFuwEAAAAAAAArO65557Tt99+q9dff12PP/64evXqpdtuu63CNxdK0j//+U8dPXrU8/u8efO0Z88eDR48WJJ0wQUXKC0tTc8++6xycnIqPP/AgQOSJJvNpt///vdasGCB1qxZU2G60u/li46OliQdOXLE6/HLLrtMsbGxmjZtmoqKivwup3HjxurcubPeeustOZ1Oz+OLFy/WTz/9VOnrEiiMwAIAAAAAAGe9hQsXasuWLRXivXr1UkFBgR555BGNGzdOw4YNk1Ty7YWdO3fW7bffrrlz53o9p169eurdu7fGjx+vffv2acaMGWrZsqX+7//+T1JJY+qNN97Q4MGD1b59e40fP15NmzbV7t27tXTpUsXGxmrBggWSpGnTpmnRokXq16+fbr75ZrVr10579uzRBx98oG+++Ubx8fHq3Lmz7Ha7nnrqKTmdTkVEROjiiy9WYmKiXnnlFd1www3q0qWLrrnmGjVo0EC//fabPv30U1100UV66aWXJEnTp0/X5Zdfrt69e+vGG2/UoUOHNHPmTLVv395nky3QaGABAAAAAICz3qOPPuoz/sYbb+i1115T/fr1NWPGDE+8VatWmj59uu666y7NnTtXV199teexBx98UBs2bND06dN19OhRXXLJJXr55ZdVp04dzzT9+/fXypUr9fjjj+ull15STk6OGjVqpB49euiWW27xTNe0aVOtWrVKjzzyiObMmaPs7Gw1bdpUgwcP9syvUaNGevXVVzV9+nRNmDBBxcXFWrp0qRITE/WHP/xBTZo00ZNPPqlnnnlGBQUFatq0qfr06aPx48d7ljNo0CB98MEHevjhh/XAAw8oLS1Ns2bN0scff6xly5adplf55Blm6XizEJKdna24uDg5nU7PHfMBAACAMxo3cQcQJPn5+crIyFBKSooiIyODnY6lLVu2TAMGDNAHH3ygkSNHBjudgKpqOznVXg73wAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKVxE3cAAAAAAIDToH///grBW42HBEZgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAACAs9bs2bNlGIYiIyO1e/fuCo/3799fHTp0CEJmKM8R7AQAAAAAAEAI+/zzYGcgDRp0yrMoKCjQk08+qZkzZ56GhHC6MQILAAAAAACc9Tp37qy///3vyszMDHYq8IEGFgAAAAAAOOs9+OCDKi4u1pNPPlnpdC6XS48//rjS0tIUERGhFi1a6MEHH1RBQYFnmnvuuUcJCQkyTdMTu/POO2UYhl588UVPbN++fTIMQ6+88srpL+gMQwMLAAAAAACc9VJSUjRmzJgqR2HddNNNevTRR9WlSxc9//zz6tevn6ZPn65rrrnGM02fPn106NAh/fjjj57Y8uXLZbPZtHz5cq+YJPXt27cWKjqz0MACAAAAAACQ9NBDD8nlcumpp57y+fj69ev11ltv6aabbtIHH3yg22+/XW+99Zb+9Kc/6T//+Y+WLl0qSerdu7eksgaV0+nUxo0bNWLEiAoNrHr16uncc8+t5cpCHw0sAAAAAAAASampqbrhhhv0+uuva8+ePRUe/+yzzySVXCJY3r333itJ+vTTTyVJDRo0UNu2bfX1119LklasWCG73a777rtP+/bt09atWyWVNLB69+4twzBqraYzBQ0sAAAAAACA4x5++GG5XC6f98LasWOHbDabWrZs6RVv1KiR4uPjtWPHDk+sT58+ntFWy5cvV9euXdW1a1fVq1dPy5cvV3Z2ttavX68+ffrUbkFnCBpYAAAAAAAAx6Wmpur666/3OwpLUrVGTPXu3Vu7d+/Wtm3btHz5cvXp00eGYah3795avny5vv32W7ndbhpY1UQDCwAAAAAAoJzSUVgn3gurefPmcrvdnksAS+3bt09HjhxR8+bNPbHSxtTixYv1/fffe37v27evli9fruXLlys6OloXXHBBLVdzZqCBBQAAAAAAUE5aWpquv/56vfbaa9q7d68nPmTIEEnSjBkzvKZ/7rnnJEmXX365J5aSkqKmTZvq+eefV1FRkS666CJJJY2tX3/9VfPmzdOFF14oh8NRy9WcGU5LAysnJ0eTJk3SoEGDVK9ePRmGodmzZ3tN43a7NXv2bA0fPlzJycmKjo5Whw4d9MQTTyg/P/90pAEAAAAAAHBaPPTQQyoqKtLPP//siXXq1Eljx47V66+/rtGjR+vll1/WuHHj9PTTT+v3v/+9BgwY4DWPPn366Oeff1aHDh10zjnnSJK6dOmi6Ohopaenc/lgDZyWBlZWVpamTJmizZs3q1OnTj6nOXbsmMaPH68DBw7o1ltv1YwZM9S9e3dNmjRJgwcPlmmapyMVAAAAAACAU9ayZUtdf/31FeJvvPGGJk+erO+//1533323vvrqKz3wwAN67733Kkxb2qDq3bu3J+ZwONSzZ0+vx1E1wzwNnaOCggIdPnxYjRo10po1a9StWzfNmjVL48aN80xTWFioNWvWqFevXl7PnTJliiZNmqTFixfr0ksvrdbysrOzFRcXJ6fTqdjY2FNNHwAAALC+X34JdgZlTvj2LQBntvz8fGVkZCglJUWRkZHBTgcWVdV2cqq9nNMyAisiIkKNGjWqdJrw8PAKzStJuvLKKyVJmzdvPh2pAAAAAAAA4AwT9Ju4l94MrX79+kHOBAAAAAAAAFYU9FvdP/3004qNjdXgwYP9TlNQUKCCggLP79nZ2ZIkl8sll8slSbLZbLLZbHK73XK73Z5pS+PFxcVe99nyF7fb7TIMwzPf8nFJKi4urlbc4XDINE2vuGEYstvtFXL0F6cmaqImaqImaqImaqImavLk7nbLZhiyGYaK3W6Vvw+I3TBKaio3j9K4JBWfcNcQf3GHzVZSU7m4Iclus8ltmnKXxl0u1hM1UdNZVJPL5fLMz9ddiAzDsFS8JqyWeyjXJJVsH+V7NeW3vRO3v5oKagNr2rRpWrJkiV5++WXFx8f7nW769OmaPHlyhfjatWsVHR0tSWrQoIHS0tKUkZGhAwcOeKZJSkpSUlKS0tPT5XQ6PfHU1FQlJiZq06ZNysvL88Tbtm2r+Ph4rV271msn7tixo8LDw7VmzRqvHLp27arCwkJt2LDBE7Pb7erWrZucTqe2bNniiUdFRalTp07KysrStm3bPPG4uDi1a9dOmZmZ2rVrlydOTdRETdRETdRETdRETdTkqSk3V6kJCUqMidGmvXuVV1RUVlNiouKjorR2924Vl/uQ27FxY4U7HFqzc6d3TcnJKnS5tGHPnrKabDZ1S06WMz9fW/bvL6spLEydmjRRVm6uth08WBI8dKjqmr7/XgdycspqiotTUny80vfvl7Pc+vDUlJnpu6adO0+9pvr12faoiZpOsabSexoVFxcrPz/fE7fZbKpTp45cLpfXwBO73a6oqCgVFRWpsLDQE3c4HIqMjFRBQYFXQyM8PFzh4eHKz8/3yjEiIkJhYWHKy8vzauJFRkbK4XDo2LFjXs2UqKgo2Ww25ebmetUUHR0tt9vt9boYhqHo6GhqOk01SVJRUZE2bdrkiZff9koHI52s03IT9/L83cT9RO+//76uvfZa3XjjjXrjjTcqnaevEVjJyck6ePCg58ZfVulMlzqTuu3URE3URE3URE3URE3UZIGatm2zzgis1NSqa0pPV/ls/OUekJrS0tj2qImaTqGm/Px8/fbbb0pNTfU0KspjtBI1SSW9m23btqlZs2aehmf5bS87O1sJCQknfRP3oDSwFi9erKFDh2rgwIH66KOP5HDUbCAY30IIAACAs06ofQthqOULwC++hRDVERLfQlgTq1at0pVXXqmuXbtq7ty5NW5eAQAAAAAA4OwS0AbW5s2bdfnll6tFixb65JNPFBUVFcjFAwAAAAAAIASdtuFPL730ko4cOaLMzExJ0oIFCzw3n7vzzjtls9l02WWX6fDhw7rvvvv06aefej0/LS1NPXv2PF3pAAAAAAAA4Axx2u6B1aJFC+3YscPnYxkZGZKklJQUv88fO3asZs+eXa1lcQ8sAAAAnHVC7Z5SoZYvAL+4Bxaqo7bvgXXaRmBt3769ymlO8/3iAQAAAAAAcBYI+E3cAQAAAAAAzhaGYeixxx4LdhohjwYWAAAAAAA4KxmGUa2fZcuWBTvVs95pu4QQAAAAAACchaxwz7uTvNfd22+/7fX7P//5Ty1evLhCvF27diedGk4PGlgAAAAAAOCsdP3113v9/t1332nx4sUV4gg+LiEEAAAAAADwIzc3V/fee6+Sk5MVERGhNm3a6Nlnn63wRXUFBQX6f//v/6lBgwaqW7euhg8frl27dlWY344dO3T77berTZs2ioqKUkJCgkaNGuX15Xjbtm2TYRh6/vnnKzz/22+/lWEY+te//nXaa7UyGlgAAAAAAAA+mKap4cOH6/nnn9egQYP03HPPqU2bNrrvvvt0zz33eE170003acaMGRo4cKCefPJJhYWF6fLLL68wz++//17ffvutrrnmGr344ou69dZb9eWXX6p///46duyYJCk1NVUXXXSR5syZU+H5c+bMUd26dXXFFVfUTtEWxSWEAAAAAAAAPsyfP19fffWVnnjiCT300EOSpD/+8Y8aNWqUXnjhBd1xxx1KS0vT+vXr9c477+j222/X3/72N8901113nTZs2OA1z8svv1wjR470ig0bNkw9e/bUhx9+qBtuuEGSNGbMGN1yyy3asmWL2rZtK0kqKirS3LlzddVVV6lOnTq1Xb6lMAILAAAAAADAh88++0x2u10TJ070it97770yTVMLFy70TCepwnR33313hXlGRUV5/l9UVKSDBw+qZcuWio+P1w8//OB57Oqrr1ZkZKTXKKwvvvhCWVlZZ+U9umhgAQAAAAAA+LBjxw41adJEdevW9YqXfivhjh07PP/abDalpaV5TdemTZsK88zLy9Ojjz7quadW/fr11aBBAx05ckROp9MzXXx8vIYNG6Z3333XE5szZ46aNm2qiy+++LTVGCpoYAEAAAAAAATInXfeqalTp+rqq6/W3LlztWjRIi1evFgJCQlyu91e044ZM0bbtm3Tt99+q6NHj2r+/Pm69tprZbOdfe0c7oEFAAAAAADgQ/PmzbVkyRIdPXrUaxTWli1bPI+X/ut2u/Xrr796jbr6+eefK8xz3rx5Gjt2rP761796Yvn5+Tpy5EiFaQcNGqQGDRpozpw56tGjh44dO+a5R9bZ5uxr2QEAAAAAAFTDkCFDVFxcrJdeeskr/vzzz8swDA0ePFiSPP+++OKLXtPNmDGjwjztdrtM0/SKzZw5U8XFxRWmdTgcuvbaazV37lzNnj1b5513njp27HgqJYUsRmABAAAAAAD4MGzYMA0YMEAPPfSQtm/frk6dOmnRokX6+OOPdffdd3vuedW5c2dde+21evnll+V0OtWrVy99+eWX+uWXXyrMc+jQoXr77bcVFxenc889VytXrtSSJUuUkJDgM4cxY8boxRdf1NKlS/XUU0/Var1WRgMLAAAAAADAB5vNpvnz5+vRRx/V+++/r1mzZqlFixZ65plndO+993pN++abb3ou9/vPf/6jiy++WJ9++qmSk5O9pnvhhRdkt9s1Z84c5efn66KLLtKSJUt02WWX+czhggsuUPv27bV582Zdd911tVar1RnmiePWQkB2drbi4uLkdDoVGxsb7HQAAACA2ufjr/hB07Jl1dOEWr4A/MrPz1dGRoZSUlIUGRkZ7HTOSueff77q1aunL7/8Mtip+FXVdnKqvRzugQUAAAAAAGBRa9as0bp16zRmzJhgpxJUXEIIAAAAAABgMZs2bdL//vc//fWvf1Xjxo01evToYKcUVIzAAgAAAAAAsJh58+Zp/PjxKioq0r/+9a+z/vJNGlgAAAAAAAAW89hjj8ntdmvz5s3q169fsNMJOhpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAKBKpmkGOwVYWG1vHzSwAAAAAACAX3a7XZJUVFQU5ExgZaXbR+n2crrRwAIAAAAAAH6FhYUpIiJCTqeTUVjwyTRNOZ1ORUREKCwsrFaW4aiVuQIAAAAAgDNG/fr1tXv3bu3atUtxcXEKCwuTYRjBTgtBZpqmioqK5HQ6lZOTo6ZNm9basmhgAQAAAACASsXGxkqSsrKytHv37iBnA6uJiIhQ06ZNPdtJbaCBBQAAAAAAqhQbG6vY2FgVFRWpuLg42OnAIux2e61dNlgeDSwAAAAAAFBtYWFhAWlYAOVxE3cAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFjaaWlg5eTkaNKkSRo0aJDq1asnwzA0e/Zsn9Nu3rxZgwYNUkxMjOrVq6cbbrhBBw4cOB1pAAAAAAAA4AzkOB0zycrK0pQpU9SsWTN16tRJy5Yt8zndrl271LdvX8XFxWnatGnKycnRs88+q40bN2r16tUKDw8/HekAAAAAAADgDHJaGliNGzfWnj171KhRI61Zs0bdunXzOd20adOUm5ur//3vf2rWrJkkqXv37vrd736n2bNn6+abbz4d6QAAAAAAAOAMclouIYyIiFCjRo2qnO7DDz/U0KFDPc0rSbr00kvVunVrzZ0793SkAgAAAAAAgDNMwG7ivnv3bu3fv19du3at8Fj37t21du3aQKUCAAAAAACAEHJaLiGsjj179kgqudzwRI0bN9ahQ4dUUFCgiIiICo8XFBSooKDA83t2drYkyeVyyeVySZJsNptsNpvcbrfcbrdn2tJ4cXGxTNOsMm6322UYhme+5eOSVFxcXK24w+GQaZpeccMwZLfbK+ToL05N1ERN1ERN1ERN1ERN1OTJ3e2WzTBkMwwVu90qq0iyG0ZJTeXmURqXpGLTrFbcYbOV1FQubkiy22xym6bcpXGXq3o1lZu3v9wDVhPbHjVREzVRU1BrOrGumgpYAysvL0+SfDaoIiMjPdP4enz69OmaPHlyhfjatWsVHR0tSWrQoIHS0tKUkZHh9a2GSUlJSkpKUnp6upxOpyeempqqxMREbdq0yZObJLVt21bx8fFau3at18ru2LGjwsPDtWbNGq8cunbtqsLCQm3YsMETs9vt6tatm5xOp7Zs2eKJR0VFqVOnTsrKytK2bds88bi4OLVr106ZmZnatWuXJ05N1ERN1ERN1ERN1BRyNdWrp0KXSxuO//FSKml+dEtOljMvT1v27y+rKSxMnZo0UVZOjrYdPFhWU1SU2iUmKvPIEe0ql2ODmBilJSQo4+BBHcjJKaspLk5J8fFK379fznK5p5533pm1nnJzlZqQoMSYGG3au1d5RUVlNSUmKj4qSmt371ZxuQ8aHRs3VrjDoTU7d3rXlJzsfz3l5/teT7m5Zevp0KGqazp82Pd6ysryXk+BqClU9yerbHvURE3URE2noabSwUgnyzDNE/5EcYpKb+I+a9YsjRs3rkL8n//8p2644Qav59x///165plnlJ+fX+0RWMnJyTp48KBiY2Ml0fGkJmqiJmqiJmqiJmqyRE0ZGSXxkx3ZU0ncdjzPao/sadnyzFpP27ZZZwRWamrVNaWnW2cEVlpaaO5PVtn2qImaqImaTkNN2dnZSkhIkNPp9PRyaiJgI7BKLx3cU+4vIqX27NmjevXq+WxeSSWjtnw95nA45HB4l1D6op2odMVWN37ifE8mbhiGz7i/HGsapyZq8henJmqSqMlfjjWNUxM1SdTkL0ef8eNNBMfxf70fMnzGSxsY1Y7bbD5v5Go/sc7jv58x66nc4xVqLc3RX9zH6+gvXq31VK7mSmvysUx/udd6TaG4P1USpyZqkqjJX441jVNTYGryl391Bewm7k2bNlWDBg0qDHmTpNWrV6tz586BSgUAAAAAAAAhJGANLEkaMWKEPvnkE+0sd736l19+qfT0dI0aNSqQqQAAAAAAACBEnLZLCF966SUdOXJEmZmZkqQFCxZ4bgB25513Ki4uTg8++KA++OADDRgwQHfddZdycnL0zDPP6LzzztP48eNPVyoAAAAAAAA4g5y2m7i3aNFCO3bs8PlYRkaGWrRoIUn68ccfdc899+ibb75ReHi4Lr/8cv31r39Vw4YNq72s7OxsxcXFnfSNvwAAAFBLfvkl2BmUadky2BmcXqH22oZavgCAWnWqvZzTNgJr+/bt1Zquffv2+uKLL07XYgEAAAAAAHCGC+g9sAAAAAAAAICaooEFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLcwQ7AQAAACBofvkl2BmUadky2BkAAGBZjMACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAIClBbyBtXXrVl1zzTVKSkpSnTp11LZtW02ZMkXHjh0LdCoAAAAAAAAIAY5ALmznzp3q3r274uLidMcdd6hevXpauXKlJk2apP/973/6+OOPA5kOAAAAAAAAQkBAG1hvv/22jhw5om+++Ubt27eXJN18881yu9365z//qcOHD+ucc84JZEoAAAAAAACwuIBeQpidnS1JatiwoVe8cePGstlsCg8PD2Q6AAAAAAAACAEBbWD1799fkjRhwgStW7dOO3fu1Pvvv69XXnlFEydOVHR0dCDTAQAAAAAAQAgI6CWEgwYN0uOPP65p06Zp/vz5nvhDDz2kJ554wu/zCgoKVFBQ4Pm9dCSXy+WSy+WSJNlsNtlsNrndbrndbs+0pfHi4mKZplll3G63yzAMz3zLxyWpuLi4WnGHwyHTNL3ihmHIbrdXyNFfnJqoiZqoiZqoiZqoKeRqOv7c4nLzkCSHzVZSU7m4Iclus8ltmnJXI247nqfb7VZZRZLNMGQzDBW73Sq/VJvbXXVN5V4bu2H4zN1f/LTXVO419rk+3G6/tdoNo6Qmd/lXphZrcrmqt+2Vm7ff9RSomkJxfzoTjxHURE3UdNbWdGJdNRXQBpYktWjRQn379tWIESOUkJCgTz/9VNOmTVOjRo10xx13+HzO9OnTNXny5ArxtWvXekZtNWjQQGlpacrIyNCBAwc80yQlJSkpKUnp6elyOp2eeGpqqhITE7Vp0ybl5eV54m3btlV8fLzWrl3rtbI7duyo8PBwrVmzxiuHrl27qrCwUBs2bPDE7Ha7unXrJqfTqS1btnjiUVFR6tSpk7KysrRt2zZPPC4uTu3atVNmZqZ27drliVMTNVETNVETNVETNUmScnMVFRamTk2aKCsnR9sOHiyrKSpK7RITlXnkiHaVy7FBTIzSEhKUcfCgDuTklNUUF6ek+Hil798vZ7ncUxMSlBgTo02ZmcorKiqrKTFR8VFRWrtzp4rdbun4ey+/NdWrp0KXSxv27CmryWZTt+RkOfPztWX//rL1VFpTbq7vmpxO3zUdPuy7pqws75ri46teT8f/MCpJHRs3VrjDoTU7d3rXlJwcmJrKvZY+t73c3LL1tHev7/W0e3fJeqrtmg4dqnp/qu56CkRNZ/oxgpqoiZqoKQRqyi53zj0Zhmme8CeKWvTee+/pxhtvVHp6upKSkjzx8ePHa+7cufrtt9+UkJBQ4Xm+RmAlJyfr4MGDio2NlUTHk5qoiZqoiZqoiZrO4Jq2bav90UrVHQWTmlp5TRkZJXErjMBq2bLq9VTuTXzQR2Adf20lP9vYtm3WGYGVmlr1/pSebp0RWGlpZ/YxgpqoiZqoKQRqys7OVkJCgpxOp6eXUxMBbWD17dtXxcXFWrFihVf8o48+0lVXXaXFixfr0ksvrXI+2dnZiouLO+miAQAAQsovvwQ7gzItW1b+eCjlKoVWvqGUqxR6+QIAatWp9nICehP3ffv2VegMSlLR8aHCp3o9JAAAAAAAAM48AW1gtW7dWmvXrlV6erpX/F//+pdsNps6duwYyHQAAAAAAAAQAgJ6E/f77rtPCxcuVJ8+fXTHHXcoISFBn3zyiRYuXKibbrpJTZo0CWQ6AAAAAAAACAEBbWD17dtX3377rR577DG9/PLLOnjwoFJSUjR16lTdf//9gUwFAAAAAAAAISKgDSxJ6t69uz777LNALxYAAAAAAAAhKqD3wAIAAAAAAABqigYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAszRHsBHDcL78EO4MyLVsGOwMAAAAgcHgvDtS+UNrP/vnPwORRHWPGBDsDy2AEFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACzNEewEAAAAAJx5Vv4a7AzK9GwZ7AwAAKeKBhYAAAAQAmgIAQDOZlxCCAAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLC0oD64cfftDw4cNVr1491alTRx06dNCLL74YjFQAAAAAAABgcY5AL3DRokUaNmyYzj//fD3yyCOKiYnRr7/+ql27dgU6FQAAAADQyl+DnUGZni2DnQEAWFNAG1jZ2dkaM2aMLr/8cs2bN082G1cwAgAAAAAAoHIB7SC9++672rdvn6ZOnSqbzabc3Fy53e5ApgAAAAAAAIAQE9AG1pIlSxQbG6vdu3erTZs2iomJUWxsrG677Tbl5+cHMhUAAAAAAACEiIBeQrh161a5XC5dccUVmjBhgqZPn65ly5Zp5syZOnLkiP71r3/5fF5BQYEKCgo8v2dnZ0uSXC6XXC6XJMlms8lms8ntdnuN6iqNFxcXyzTNKuN2u12GYXjmWz4uScXFxdWKOxwOmabpFTcMQ3a7vUKOhmHILsltmnKXz/F4nm63W+XHqdkMQzbDULHbLbMacbthlNR0wmg3u2GU5G6a3vHjv59yTT7iIb+eqImaqImaqImaglGT2y1Dkt1mq/B+wV+81t5HHK/Nb02l7yNOeH/hsNlKaqpG7qetJre76vVUbn37fW/kJ37aayq33fjaxkzTLalkfZT8vzz/8RJmteKGYTu+vMrjLperyv2pJjkGoqbKjhHll1H5a1D7NZU/fpzVxz1qOvNqOv5Y0D7nlo+Xex181iSVfEY//lNV3Hb8x1+8WN5HFH9x+/FleK0ll+uM2fZO3P5qKqANrJycHB07dky33nqr51sHr7rqKhUWFuq1117TlClT1KpVqwrPmz59uiZPnlwhvnbtWkVHR0uSGjRooLS0NGVkZOjAgQOeaZKSkpSUlKT09HQ5nU5PPDU1VYmJidq0aZPy8vI88bZt2yo+Pl5r1671WtkdO3ZUeHi41qxZ45VD165dVVhYqA0bNnhidrtd3bp1k9Pp1JYtWzzxqKgoderUSVlZWdq2bZsnHhcXp3ZhYcp0OrWrXI4NYmKUlpCgjMOHdSAnp6ymuDglxccrPStLznK5pyYkKDEmRpv27lVeUVFZTYmJio+K0trdu1VcbsPr2Lixwh0Ordm507um1NTTU1O7dsrMzPS6QX/IrydqoiZqoiZqoqZg1JSbq6iwMHVq0kRZubnadvBgWU1RUWqXmBi49xGHDlVeU716KnS5tGHPnrKabDZ1S06WMz9fW/bvL1tPtV1TfHzV6+n4H0alSt4bJScHpqZyr6Wvbc9ZlKsoe4Ii7DHKce1VsVm2nqIdiQozopRdtFtmuY9PdcMayyaHnEXeNcWFJcstl44WldVkyKa48GS5zHzluspqshthqhvWRIXuXOUVl9S0Zs2hKvenvOLDKnSXradIe5wi7fHKdWXJZZatj0DUVNUxwlmUK0lyGFGKCUtUgdup/OKy9RRui1EdR0JAalqz5pAnflYf94JVU25u2XFv587qfX6q7BiRl+f7GJGT4/sYceRI2TEiOvrMWk+5JftZ0D7nll9Px89lfmuKjFSn/HxlORzaFh5eVlNxsdoVFCgzLEy7wsI88QYul9IKC5URHq4DjrI2S1JRkZKKipQeESHn8WaTJKUWFirR5dKmyEjllbs3eNv8fMW73VobFaXi4w03rVkTuvuTvLe97HLn3JNhmKZ54p8uak2HDh30448/6r///a/69u3riX/99dfq16+f3nrrLY0ZM6bC83yNwEpOTtbBgwcVGxsr6QzoTGdkWGcE1vEmYqh0cb1yP0M609RETdRETdRETV41bdtmnRFYqamV15SRURK3wgisli2rXk/l3sQHfQTW8ddW8r2NrV6yTVYZgdX90tQq96dvP0+vdo61XdOFA9MqPUaUvLbVeQ1qfwRW90vLtoOz+rgXrJq2bTu1kT3lazrVY0Rq6pm1no4fby0xAqvc8dZnTe++a50RWH/4Q+juT/Le9rKzs5WQkCCn0+np5dREQEdgNWnSRD/++KMaNmzoFU9MTJQkHT582OfzIiIiFBERUSHucDjkcHiXUPqinah0xVY3fuJ8TyZuGIbPuL8cS3dMn9P7WKbdxzwqizv8xU9c5vHfT0tNNYyHxHqiJmryk2NN49RETRI1+cuxpvEzvqZyOfl9vxCo9xEn5Foh99L3ET5yMQzDZ7zWajr+e2XraWWGrzlVXKb/uHGa4jb1bF1xOyifu2HYfP7fa+5+4jWpyTB851g+Xn69+9tvappjbddU2THixGX4fw1qvyZfeZ6Vx71q5FgrNZV7XrU/P1USP6XjXjX2s5BaTyc8FvDPueXjJ+Tvt6bjP6ca9702/Me9MimXV8jtTyfk6C//6groTdwvuOACSdLu3bu94pmZmZJKhqgBAAAAAAAA5QW0gXX11VdLkv7xj394xd944w05HA71798/kOkAAAAAAAAgBAT0EsLzzz9fN954o9588025XC7169dPy5Yt0wcffKAHHnhATZo0CWQ6AAAAAAAACAEBbWBJ0quvvqpmzZpp1qxZ+uijj9S8eXM9//zzuvvuuwOdCgAAAAAAAEJAwBtYYWFhmjRpkiZNmhToRQMAAAAAACAEBfQeWAAAAAAAAEBN0cACAAAAAACApQX8EkIAAAAAwMlbtCnYGZQZ2CHYGQA4WzACCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAluYIdgIAAAAAgDPTok3BzqDMwA7BzgDAqWAEFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACzNEewEAAAAcOZY+WuwMyjTs2WwMwAQajiGAdbFCCwAAAAAAABYGg0sAAAAAAAAWBqXEAIAAAAAEGIWbQp2BmUGdgh2BjgbMAILAAAAAAAAlsYILNTcL78EO4MyLbmzIQAAAGBVdXdb6LNDhzPrswOvLc42jMACAAAAAACApTECCwAAAAAA1KqVvwY7gzI9GTAWkhiBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLcwQ7AQAAAAAAAKv4NSvYGZRJC3YCFsIILAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWFrQG1hTp06VYRjq0KFDsFMBAAAAAACABTmCufBdu3Zp2rRpio6ODmYaAAAAlrby12BnUKZny2BnAAAAzkZBbWD96U9/0oUXXqji4mJlZWUFMxUAAAAAAABYVNAuIfz66681b948zZgxI1gpAAAAAAAAIAQEpYFVXFysO++8UzfddJPOO++8YKQAAAAAAACAEBGUSwhfffVV7dixQ0uWLKnW9AUFBSooKPD8np2dLUlyuVxyuVySJJvNJpvNJrfbLbfb7Zm2NF5cXCzTNKuM2+12GYbhmW/5uFTSfKtO3OFwyDRNr7hhGLLb7RVyNAxDdklu05S7fI7H83S73XKXm7fNMGQzDBW73TKrEbcbRklN7vJzKYlLUrFpeseP/+63pvK5S7LbbBVy9xc/7TUFej35iIf8tkdN1ERN1ERNlq/JNN3H87cdX573ubvyuPf5Xyo5h55svLQ2f7mXvR41ybF2anK73VWuJ+/nGD5z9xc/3TWV3258bWMludZ8/dVGTS6Xq8r96XRve6daU2XHiPLLCOT+5Cv38tuBv/1MKjlGyCwfN2TY7CXzPmG79hk3bGU1+Yq7i71fAz9x06z8uFfd9ReIY0R1juVV7We+cq+tmlwuV6Xnp7J8K9Ya6GOEpCrPuRX3s+AdI8pvr77eR7gNyWaWzME0vOfiM26WfNZ1l1+MJMMs+dV9wjxqEne5XGfMe6MTjxM1FfAG1sGDB/Xoo4/qkUceUYMGDar1nOnTp2vy5MkV4mvXrvXcAL5BgwZKS0tTRkaGDhw44JkmKSlJSUlJSk9Pl9Pp9MRTU1OVmJioTZs2KS8vzxNv27at4uPjtXbtWq+V3bFjR4WHh2vNmjVeOXTt2lWFhYXasGGDJ2a329WtWzc5nU5t2bLFE4+KilKnTp2UlZWlbdu2eeJxcXFqFxamTKdTu8rl2CAmRmkJCco4fFgHcnLKaoqLU1J8vNKzsuQsl3tqQoISY2K0ae9e5RUVldWUmKj4qCit3b3bq/nUsXFjhTscWrNzp3dNqamV11Ru+qiwMHVq0kRZubnadvBgWU1RUWqXmFj7NQV6PbVrp8zMTO3atausplDf9qiJmqiJmqjJ8jU5i3JlN8JUN6yJCt25yisuO+c6jCjFhCWqwO1UfnFZjuG2GNVxJCiv+LAK3WXn3Eh7nCLt8cp1ZcllluUeZU9QhD1GOa69KjbLzrnRjkSFGVHKLtotU26tWXOo0pqkenLLpaNFezwRQzbFhSfLZeYr17W/rNZarikrK77K9eQsyvbE64Y1lk0OOYu83xvFhSUHpKbyr6Wvbc9ZlFvt9VTbNa1Zc6jK/el0b3unUlNVxwhnUW6111Nt11S6j0n+jxGK6iaz0KmiQ2U1GY4ohTfoJHdellzOsuOeLSJOYfXaqTgnU8U5ZevJHtVAjvg0FTszVJxXdtyzxyTJUTdJriPpcheUvQaOuFTZ6ySq6OAmma6yWp3NKj/uBWt/8rWeqnMsdxblBnx/8lfTmjWHKj0/SQrK/uSrJql1lefc0v0skPuTv5pK9zN/7yOKEiLVJCtfOVEOHYoLL8uxoFgNDxfIGRMmZ0yYJx6T51KCs1CH48KVE1XWZonLKVJ8TpEOxEcoP8LuiddzFqpunkt7EyJV5Ci7MC7xUL6iCt3alRgl8/iAk4Nr1pwx741KByOdLMMs3xoLgNtuu01LlizRjz/+qPDwkg2hf//+ysrK0qZNm3w+x9cIrOTkZB08eFCxsbGSrP+XU6mKjmdGhnVGYLVqVXlNW7eW5a4gj8Bq0cI79zOkM01N1ERN1ERN1FS+ptVLth3PP/gjsLpfmlpp7quXZBz/X/BHYF04sGWV66n0tS2dj6/cAzVipPS1lXxvYyW5WmMEVvdLU6vcn779PL3aOdZ2TRcOTKv0GFF+Owj2CKzy24G//eyrLdYZgTXwvMqPeyu/2CpvwRuB1f3SlCqP5VXtZ75yr62aul+aWun5adXibZYZgdVrUOsqz7kV97PgjcAqv5/5eh+RMfNdy4zASrnzD2fMe6Ps7GwlJCTI6XR6ejk1EdARWFu3btXrr7+uGTNmKDMz0xPPz89XUVGRtm/frtjYWNWrV8/reREREYqIiKgwP4fDIYfDu4TSF+1EpSu2uvET53syccMwfMb95VjarPE5vY9l2n3Mo7K4w1/8xGUe/91vTTXJvbZrCsZ6qmE8JLY9aqImPznWNE5N1CRRk78caxovX5Nh2LziXu+Oq4z7PoeebPzEXE/83fCc92uSY+3UVLouK1tPvudVcZn+4qezJl/bQfncvbeDmq2/011T+Vz97Tene9vz8Ui141UdI05cRqD2Jx+P+MzT3zFChq+4TfIx/xrHbb73mxPjpbu8v+NbTdZfbR8jqnMsr85+FqhjRCD3s9NRU1Xn1or7WfCOEb7OXV6vt1k2B8PHkB9/cZvk6+pKz/xOJl4+r1B/b+Qv/+oK6E3cd+/eLbfbrYkTJyolJcXzs2rVKqWnpyslJUVTpkwJZEoAAAAAAACwuICOwOrQoYM++uijCvGHH35YR48e1QsvvKC0tLRApgQAAAAAAACLC2gDq379+vr9739fIT5jxgxJ8vkYAAAAAAAAzm4BvYQQAAAAAAAAqKmAjsDyZ9myZcFOAQAAAAAAABbFCCwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFiaI9gJAAAABNqiTcHOoMzADsHOAAAAwPoYgQUAAAAAAABLYwSWRaz8NdgZlOnZMtgZAAAAAAAAlGEEFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNm7gDAGBVv/wS7AzKtKzGN3yEUL51d1so1w58ewqAmuEYBuBsxAgsAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFiaI9gJIPSs/DXYGZTp2TLYGQAAAAAAgNrGCCwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFiaI9gJAACAM8PKX4OdQZmeLYOdAQAAAE4nRmABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0gLawPr+++91xx13qH379oqOjlazZs109dVXKz09PZBpAAAAAAAAIIQ4Armwp556SitWrNCoUaPUsWNH7d27Vy+99JK6dOmi7777Th06dAhkOgAAAAAAAAgBAW1g3XPPPXr33XcVHh7uiY0ePVrnnXeennzySb3zzjuBTAcAAAAAAAAhIKANrF69elWItWrVSu3bt9fmzZsDmQoAAAAAAABCRNBv4m6apvbt26f69esHOxUAAAAAAABYUEBHYPkyZ84c7d69W1OmTPE7TUFBgQoKCjy/Z2dnS5JcLpdcLpckyWazyWazye12y+12e6YtjRcXF8s0zSrjdrtdhmF45ls+LknFxcXVijscDpmm6RU3DEN2u71CjoZhSNLxPEyv+RiGTabpljdDhmGclngJ72WWvh7+ajpxPiU5+su9dmsK9HryFQ/1bY+aqImaLFxTuentxvHjntv7eGg/fg4pNs1qxR22kmNz+bghyW6zyW2acvuLl3st/dVkmmatnp/8xX2db4qLiytdT1Y550pGhW1Mqrjtlc4vmOfc0njpfuVvvynbnmuSY+3U5Ha7qzxGeD/n1Le9U6nJ5WM/K597Sa6B3598xV0uV5XHvWDsT5XVVNmxvPwyArk/+cq9/Hbgbz+TKvvsENhjROmx3985t7rrLxDHiOq8j6hqP/OVe23V5HK5Kn0fUZZvxVoDfYyQVOV7o4r7WfCOEeW3V1/v99yGZDNL5mAa3nPxGTdLRge5yy9GkmGW/Oo+YR41ibtcrtB7D+vnnHvicaKmgtrA2rJli/74xz+qZ8+eGjt2rN/ppk+frsmTJ1eIr127VtHR0ZKkBg0aKC0tTRkZGTpw4IBnmqSkJCUlJSk9PV1Op9MTT01NVWJiojZt2qS8vDxPvG3btoqPj9fatWu9VnbHjh0VHh6uNWvWeOXQtWtXFRYWasOGDZ6Y3W5Xt27d5HQ6tWXLFk88KipKnTp1UlZWlrZt2+aJx8XFSQpTgdup/OKyHMNtMarjSFBe8WEVunM88Uh7nCLt8cp1ZcllluUeZU9QhD1GOa69KjaLPPFoR6LCjChlF+2WqbINr25YY9nkkLNop1dNxcWpldZUfnq7Eaa6YU1U6M5VXvFBT9xhRCkmLLHWawr0emrXrp0yMzO1a9cuTzzUtz1qsmhNGzeW1RQVpXaJico8ckS7yuXYICZGaQkJyjh4UAdyyvanpLg4JcXHK33/fjnL5Z6akKDEmBhtysxUXlHZ/tQ2MVHxUVFau3OnisudnDo2bqxwh0NrDh06PTWdieuptmvKyiqrqXQ97d7tez3t9D6Wd01OVqHLpQ179pTVZLOpW3KynPn52rJ/f1lNYWHq1KSJsnJzte1g2bHcs+05ndpV7jXzV1OB21Gr56e4sGS55dLRorKaDNkUF54sl5mvXFdZTZs25VW6nqxyzo0LS1ZeXl6V256zKDfo59zSmtasKTkm+NufpHrVXk+1XVNWVnyVxwhnUXa11lMgair/Wvo6RjiLcoOyP/mqac2aQ1Ue94KxP/mrqapjubMot9rrqbZrKt3HJP/nJ+mcgO9P/mpyOhMrPecGa3/yVVN13kc4i3IDvj/5q2nNmkOVvo+QZIlzrt0Ik9S6yvdGpftZMM+5pTWV7mf+3u8VJUSqSVa+cqIcOhRXdg/vyIJiNTxcIGdMmJwxYZ54TJ5LCc5CHY4LV05UWZslLqdI8TlFOhAfofwIuydez1mounku7U2IVJGj7MK4xEP5iip0a1dilMzjf4w8uGZN6L2H9XPOLR2MdLIMs3xrLID27t2riy66SEVFRfruu+/UpEkTv9P6GoGVnJysgwcPKjY2VlLo/9V+9ZIMy/w1uOdlrSqtaeUXW33kGJy/Bne7pIVX1Nf6+PInScbxg4XpXZNhK6nJO27IsNlLlnnCX2V9xg1bWU2+4u5iz2twybnW2/YYBWPRmn75pSwu36NjbMfzdLvdKr+l2gxDNsNQsdvttff5i1c5sicl5fTUdCaup9qu6ddfy3IM9gisctuBv5pWL8mwzAisHr9Lq3Q9ffv5Vj/zCfxfg3te1rLKbW/1km1+a606fnpr6n5pqiT/+83qJRk+aw3GCKwLB7as8hhR+tqWzsdX7oEaMVL62kq+jxEluVpjBFb3S1OrPO59+3l6tXOs7ZouHJhW6bG8/HYQ7BFY5bcDf/vZ919ut8wIrJ6Xtar0nHviZ4dgjsDqfmlKle8jqtrPfOVeWzV1vzS10vcRqxZvs8Q5V5J6DWpd5XujivtZ8EZgld/PfL3fy5j5rmVGYKXc+YfQew/r55ybnZ2thIQEOZ1OTy+nJoIyAsvpdGrw4ME6cuSIli9fXmnzSpIiIiIUERFRIe5wOORweJdQ+qKdqHTFVjd+4nxPJm4Yhs+4vxxLLiU0fMR936rsdMVPXGbpJY3+avI1H/+5125N1VkfXk81fNfkO2474cknGbeVbWPl07XStlfTeCjsT2dkTccbUD6n97FMu495VBZ3+IuznoJXk4/p/a4nH9uGv7hhGD7jfrcxw5CtGq9B6fmjts5PlcVPPN+Uvq5WP+eW5lLVtld+fsE655bGT8z1xN8NzzZUkxxrp6bSdV/ZMcL3vE5+2zv5uM3ndlA+d+/tIHD7k694+Vz972eB35/8xas6lp+4jGAeI3zl6e8YEcj9yV+8ss8Olc0nGMeI6ryPqM5+FqhjRCD3s9NRU1XvgSpuO8E7Rvg6d3m93mbZHAwfQ378xW2Sr6srPfM7mXj5vELmPayfHP3lX10Bb2Dl5+dr2LBhSk9P15IlS3TuuecGOgUAAAAAAACEkIA2sIqLizV69GitXLlSH3/8sXr27BnIxQMAAAAAACAEBbSBde+992r+/PkaNmyYDh06pHfeecfr8euvvz6Q6QAAAAAAACAEBLSBtW7dOknSggULtGDBggqP08ACAAAAAADAiQLawFq2bFkgFwcAAAAAAIAzQFC+hRAAAFRt5a/BzqBMz5bBzgAAAABnM3/fNwkAAAAAAABYAg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaDSwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFiaI9gJACizaFOwMygzsEOwMwAAAAAAoAQjsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGncAwsAcFbhXnMAAABA6GEEFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACzNEewEAISuRZuCnUGZgR2CnQEAAAAAoLbQwMIZr+7uX4KdQpkOLYOdwWkVUq/tLxbKteWZtR2s/MI6r23Py6p+bUNquwUAAAAgiUsIAQAAAAAAYHE0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpfAshAFjQyl+DnUGZnnxRHgAAAIAgo4EF4KxAQwgAAAAAQheXEAIAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSAt7AKigo0J///Gc1adJEUVFR6tGjhxYvXhzoNAAAAAAAABAiAt7AGjdunJ577jldd911euGFF2S32zVkyBB98803gU4FAAAAAAAAIcARyIWtXr1a7733np555hn96U9/kiSNGTNGHTp00P33369vv/02kOkAAAAAAAAgBAR0BNa8efNkt9t18803e2KRkZGaMGGCVq5cqZ07dwYyHQAAAAAAAISAgDaw1q5dq9atWys2NtYr3r17d0nSunXrApkOAAAAAAAAQkBALyHcs2ePGjduXCFeGsvMzPT5vIKCAhUUFHh+dzqdkqRDhw7J5XJJkmw2m2w2m9xut9xut2fa0nhxcbFM06wybrfbZRiGZ77l45JUXFxcrbjD4ZBpml5xwzBkt9sr5GgYhnJzj6okDdNrPoZheOV3PCrD0GmJl/COl76+/mrKycn2kaO/3Gu3pkOHDnlFfa2Pknx913pyuZ98TYcOHap028vNMWS6XSfMxn489eJqxQ1byXryjhsybHaZplsy3VXHDZuys6ven8q2hdOz7Z3KeirdFvztZzk52UHZn3zFDx06VOUxomb7We3WVNV+VpproPcnX/HSXCs</t>
+          <t>iVBORw0KGgoAAAANSUhEUgAABLAAAAJYCAYAAABy5h8aAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjkuNCwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy8ekN5oAAAACXBIWXMAAA9hAAAPYQGoP6dpAACJXklEQVR4nOzdeXxU9fX/8fedmWwQkkggbAlLAgKCgMgiKptaZBGsoKJVWcSvolX0p1WLG0IFtFrFpW61BResImrFBWURFBFBlEUUGpRAgbCFQEJCtpm5vz9CJhkyk0wgmbkDr+fj4aPlzJ17z5m7zsnn3jFM0zQFAAAAAAAAWJQt1AkAAAAAAAAAVaGBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAgIW0bt1ahmF4/RcVFaWWLVtq9OjRWrFiRVDyGDdunAzD0Jw5c4KyvLpS9nlu37491Kmc8sq2VwAAgLpAAwsAAAu64IILNHbsWI0dO1ZDhgyR2+3WvHnz1L9/fz399NOhTs8SwqnJFsxG2pw5c2QYhsaNG1fnywIAAAgWR6gTAAAAld10001eDYjCwkLdcssteuONN3Tffffpsssu05lnnhm6BMPE0qVLVVJSohYtWoQ6FQAAAJwERmABABAGoqOj9fe//13169eXy+XSBx98EOqUwkJaWpo6dOigiIiIUKcCAACAk0ADCwCAMBEbG6v27dtLUqVb0b744gtddtllSkpKUmRkpJo3b67Ro0dr7dq1fueXnZ2tu+66S61atfI8Z+v2229Xdnb2CeX36KOPyjAMPfroo9qxY4fGjBmjZs2aKTo6WmeeeaYeffRRFRQUVHpfSUmJ3nrrLV133XXq0KGD4uLiFBMTo/bt22vSpEnKzMz0mn779u0yDEOvv/66JGn8+PFezwx79NFHPdNWd+ve/PnzNXjwYDVu3FiRkZFq0aKFrr/+ev3yyy+Vpi1bbuvWrWWapl599VWde+65ql+/vuLj4zVo0CCtWrXK6z1lt/Pt2LFDktSmTRuvXJcvX+6ZdsmSJRo+fLiaNGmiiIgInXHGGWrXrp2uv/56ff3114GsArVu3Vrjx4+XJL3++uteyxowYIDXtEePHtXjjz+u7t27q0GDBqpXr546deqkhx56SIcOHQpoef784x//8Hw2CQkJGjp0qL777ju/0zudTr322msaMGCAGjZsqKioKLVp00a33nqrdu7cWePl//DDDxo9erSSk5MVGRmpuLg4paamatSoUfroo4/8vue6665Ty5YtFRUVpYYNG+rSSy/VZ599Vmt5L1++3LMuSkpK9MQTT6hTp06KiYlRYmKiRo4cqc2bN9e4XgAATgfcQggAQBjJzc2VJEVFRXliDz/8sB577DEZhqHzzz9fLVu21ObNmzVv3jy9//77evXVV3XjjTd6zWffvn3q27evtm7dqjPOOEOXXXaZ3G635s6dq88//1ydOnU64RwzMjJ07rnnyuFwqF+/fiooKNCyZcs0depULVmyREuWLFF0dLRXLjfccIPi4+PVsWNHdenSRfn5+Vq/fr2ef/55vfPOO/r222/Vtm1bSaWNvLFjx+qbb77Rb7/9pgsuuMDzmiR169at2hydTqeuu+46zZs3T1FRUTr33HPVokULpaena+7cufrggw/0wQcfaPDgwT7fP378eL399tvq27evLrvsMq1fv16LFy/W119/ra+++kq9e/eWJLVt21Zjx47V/PnzlZ+fr1GjRik2NtYzn6ZNm0oqbTaVNZ569eqlgQMHqqCgQLt27dI777yjRo0aqV+/ftXWdeWVV+q7777TypUrlZaWpgsvvNDzWocOHTz/Pzs7WxdffLHWr1+vuLg4XXTRRYqIiNBXX32l6dOn6+2339aXX36p1q1bV7vM4919992aNWuWLrjgAl1++eX66aeftHDhQi1evFjz5s3TFVdc4TX9kSNHNGLECC1fvlyxsbE699xz1bhxY/300096+eWX9d5772nx4sU655xzAlr+0qVLNWTIEJWUlKhr167q06ePXC6Xdu/erU8//VQul0uXX36513ueffZZ3X333XK73erWrZt69+6tvXv3avny5Vq0aJGmTp2qRx55pNbyLikp0dChQ/Xtt9+qX79+6tixo9asWaMPP/xQy5Yt07p1607oswcA4JRmAgAAy2jVqpUpyZw9e3al1zZs2GDabDZTkvmvf/3LNE3TXLhwoSnJjI6ONhctWuQ1/WuvvWZKMiMiIsxNmzZ5vXbllVeaksy+ffuahw8f9sQPHjxo9u7d25TkNw9/pkyZ4nnf5Zdfbh49etTz2s6dO80zzzzTlGT++c9/9npfbm6u+dFHH5lFRUVe8eLiYnPy5MmmJHPo0KGVljd27Nhqcyz7PDMyMrziDzzwgCnJ7N27t7lt2zav19577z3TbrebZ5xxhnno0CFPPCMjw1Nfq1atzP/+97+e15xOp3njjTeaksxBgwYFnEeZNm3amJLMFStWVHpt37595o8//ui3xuPNnj3blGSOHTvW7zSjR4/21J+VleWJHzlyxBwyZIgpyTz//PMDXqZpmp7PJiYmxly6dKnXa3/9619NSWZ8fLy5b98+r9f+8Ic/mJLMyy67rNJrzzzzjCnJbNeunel0OgPKY+DAgaYk86233qr02uHDh81Vq1Z5xT7//HPTMAyzUaNG5ldffeX12saNG83k5GRTkrl8+fKTznvZsmWez+mcc84x9+zZ43mtoKDAvPTSS01J5s033xxQrQAAnE5oYAEAYCG+GliHDx82P/30UzMtLc2UZDZv3tzMy8szTdM0L774YlOSeffdd/uc32WXXWZKMv/v//7PE/vf//5n2mw20zAM8+eff670nnXr1p1UAysmJsbri3mZjz/+2JRkxsXFmQUFBQHPt3nz5qbNZjNzc3O94ifawDp48KAZExNjRkdHm7t27fL5vttuu82UZD7//POeWMUG1oIFCyq9Z8+ePaYkMyoqyiwuLq42j4rq1atnxsfH+62jJqprYO3YscOz/jds2FDp9V27dpnR0dGmJHPlypUBL7fss7nrrrt8vt6jRw9Tkjl9+nRP7JdffjENwzCbN29eaf2WGTp0qCnJ/PjjjwPK46yzzjIlmdnZ2QFNX9awnT9/vs/X582bZ0oyR40addJ5lzWwDMMw169fX+k93333nSnJTE1NDSh3AABOJzwDCwAAC6r4XKeEhAQNGzZMv/32m9LS0vTZZ5+pfv36cjqdWrlypSR5/WJhRRMmTJAkLVu2zBP7+uuv5Xa71b17d5111lmV3tOtWzd16dLlhHMfNGiQ59a4ii677DIlJiYqNzdXP/74Y6XXN2zYoKefflp33HGHbrzxRo0bN07jxo2T0+mU2+3Wr7/+esI5VbRs2TIVFBToggsu8PvrhGXPi/r2228rveZwOHzeWti0aVOdccYZKioq0sGDB2uUU69evZSTk6MxY8bohx9+kNvtrtH7a6Js/Z9zzjk+13OLFi106aWXSvLebgI1duxYn/ExY8ZIktdzvz777DOZpqkhQ4aoQYMGPt9X1brwpVevXpKk6667Tt98842cTqffabOysrRmzRrFxMRo+PDhAS//ZPNu2bKlunbtWinesWNHSdLu3bv95gwAwOmKZ2ABAGBBFZ/rFBkZqaSkJJ133nkaPHiwHI7S0/fBgwdVWFgoqfTh4L6kpaVJ8v5CvGvXrirfU/baxo0bTyj3qubbunVrHTx40JODJOXn5+uGG27Qhx9+WOV8y57/dbK2bdsmqfRZSYZhVDntgQMHKsWaNWvm91cN4+LidOjQIc96CdSLL76oyy67TG+++abefPNNNWjQQD179tRFF12kG264QS1btqzR/KpSti1UtZ58bTeB8jffsnjFdV+2Lv75z3/qn//8Z5Xz9bUufJk5c6Y2btyohQsXauHChYqJiVH37t01YMAAXXfddZ4mkVT6vDbTNFVQUOD1XLnqln+yeftbn3FxcZKkoqKiKucJAMDpiAYWAAAWdNNNN/kdVXUqME3T8/8nT56sDz/8UB06dNDjjz+unj17qlGjRoqMjJQknX/++Vq1apXXe05G2eimtm3b6oILLqhy2ooPPi9js9X+APaOHTvqv//9rxYtWqQvv/xS3377rVasWKEvv/xS06ZN0z//+U9df/31tb7cUKi4HsvWRbdu3XyOSKqo7MH41WnatKnWrl2rr776SkuWLNHKlSu1evVqrVy5UjNmzNDMmTN1//33ey0/NjZWo0aNCriGk827LrYhAABOdTSwAAAIU4mJiYqKilJRUZG2bdvm83awspEiFW+VK/v/27dv9zvvql6rTkZGRrXzTU5O9sTmzZsnSXr33Xd91rB169YTzsWXlJQUSVL79u01Z86cWp33yXA4HBo6dKiGDh0qqXTE2dNPP62pU6fqlltu0RVXXKH69euf9HLK1n/ZtuGLr+0mUBkZGT5/CdLXui9bFxdccIFeeOGFGi/LH8MwNGDAAM9tfIWFhZozZ47++Mc/6oEHHtCVV16ptLQ0z/INw9C//vWvgBtLdZU3AADwjz//AAAQphwOhy688EJJ8tuI+de//iVJGjhwoCfWr18/GYahH3/8UVu2bKn0ng0bNpzw7YOStGjRIu3fv79S/LPPPtPBgwfVoEEDnXvuuZ54dna2JKlVq1aV3vPFF18oKyvL53LKRmhV9YwjXy6++GJFRkZq+fLlPvOsCyeSa1xcnB599FElJCTo6NGjSk9Pr5Vl9evXTzabTevXr9eGDRsqvb5nzx59/vnnkry3m0C9+eabVcbLmkqSNGTIEEnSggULanzbZU1ER0dr4sSJ6tKli9xut2f7bt68ubp06aIjR454ag5EsPIGAADlaGABABDG7rnnHknSSy+9pKVLl3q9NmfOHC1YsEARERG68847PfGWLVvqiiuukNvt1q233ur1bKlDhw7ptttuO6nb9QoKCnTrrbeqoKDAE8vMzPTkOnHiREVHR3teK3sm0fPPP+81n//+97+aOHGi3+WUjeT5+eefa5RfkyZNdMcddyg/P1/Dhw/XTz/9VGmaoqIiLViwwGeD70RUlevRo0f19NNP+3xW0ooVK3T48GHZ7XavkUuBLOuXX37x+XrLli111VVXyTRN3XLLLV4PnM/Pz9fNN9+swsJCnX/++Tr//PMDWmZFL730kteD2iXpmWee0Zo1a9SgQQPPDwtI0jnnnKNRo0Zp586dGjlypM+Rf/n5+Zo7d6727dsX0PKfeuop/e9//6sU37Jli2c0X8Vm6WOPPSap9IcTPv7440rvM01Tq1ev1qJFi+o0bwAAUDVuIQQAIIwNGTJEDz30kB577DH97ne/0wUXXKCWLVtqy5Yt+vHHH2W32/Xyyy+rU6dOXu/7+9//rg0bNmj58uVq06aNBgwYINM0tWzZMiUmJmrEiBFasGDBCeU0ZswYffLJJ0pNTVXfvn1VWFioL7/8Uvn5+erTp4+mTp3qNf2UKVN05ZVX6uGHH9a8efPUqVMn7d+/XytWrFDfvn3VvHlzn7/k9vvf/15Tp07Vc889p02bNiklJUU2m00jRozQiBEjqszx8ccf1549e/T22297nmOUmpoqh8OhXbt2af369crPz9fChQt9PgerpkaNGqVly5bp+uuv16BBg3TGGWdIku699141adJE99xzj+69916dffbZateunSIiIrR9+3Z99913kqQHH3xQjRs3DmhZ5513npo3b65169ape/fuOvvssxUREaH27dvr3nvvlVS6/rds2aLVq1crLS1NAwcOlMPh0FdffaUDBw6oTZs2mjt37gnVesstt+iiiy5S37591aJFC23atEk//fST7Ha7/vWvf1X6hcrZs2fr8OHDWrhwodq3b6+uXbuqTZs2Mk1T27dv14YNG1RcXKzNmzerSZMm1S7/scce07333qsOHTqoY8eOiomJUWZmpucXCceMGaPu3bt7ph8+fLieffZZ3XPPPRoxYoTatm2r9u3bKz4+XgcOHNCGDRu0f/9+3X///Ro0aFCd5Q0AAKphAgAAy2jVqpUpyZw9e3aN3rdw4UJz6NChZmJioulwOMymTZuaV111lbl69Wq/78nKyjLvuOMOMzk52YyMjDSTk5PNiRMnmgcOHDDHjh1b4zymTJliSjKnTJlibtu2zbz22mvNJk2amJGRkWbbtm3NRx55xMzPz/f53q+//tq8+OKLzUaNGpn16tUzO3fubE6fPt0sKioy+/fvb0oyly1bVul9H374oXnBBReYDRo0MA3D8Cy/TNnnmZGR4XO5n332mTly5EizRYsWZkREhJmQkGB27NjRvOaaa8y3337bK9+MjAxTktmqVSu/n4G/5blcLnPmzJlmp06dzOjoaFOSp6aSkhLz5ZdfNq+99lqzQ4cOZnx8vBkTE2OmpaWZo0aNMpcuXep3ef789NNP5ogRI8zGjRubNpvNlGT279/fa5r8/Hxz5syZZrdu3cx69eqZ0dHRZseOHc0HHnjAzM7OrvEyy2oyTdN86aWXzG7dupkxMTFmXFycOXjwYHPlypV+3+tyucy3337bHDp0qNmkSRMzIiLCTExMNDt37myOHz/e/PDDD83i4uKA8njrrbfM8ePHm507dzYbNmxoRkVFma1atTKHDBlifvjhh6bb7fb5vp9++sm8+eabzXbt2pnR0dFmvXr1zNTUVPPSSy81n3vuOXP37t0nnfeyZct8rgt/nyMAAChnmGYt/aQPAAA4rT366KOaOnWqpkyZokcffTTU6QAAAOAUwjOwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTwDCwAAAAAAAJbGCCwAAAAAAABYGg0sAAAAAAAAWJoj1AmcCLfbrczMTDVo0ECGYYQ6HQAAAAAAAFTBNE0dOXJEzZs3l81W8/FUYdnAyszMVEpKSqjTAAAAAAAAQA3s3LlTycnJNX5fWDawGjRoIKm06Li4uBBnAwAAAAAAgKrk5uYqJSXF09OpqbBsYJXdNhgXF0cDCwAAAAAAIEyc6KOgeIg7AAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACwtLH+FEAAAAAAABJ9pmnK5XHI6naFOBRbhcDhkt9tP+NcFA15Onc4dAAAAAACEPdM0dfjwYR04cEAulyvU6cBi7Ha7kpKSFB8fX2eNLBpYAAAAAACgSnv37tXhw4cVFxenuLg4ORyOOh9xA+szTVNOp1O5ubnas2ePCgoK1KxZszpZFg0sAAAAAADgl8vlUk5Ojho3bqxGjRqFOh1YUIMGDRQVFaWsrCwlJSXJbrfX+jJ4iDsAAAAAAPCrpKREpmmqfv36oU4FFla/fn2ZpqmSkpI6mT8NLAAAAAAAUC1uGURV6nr7oIEFAAAAAAAAS6OBBQAAAAAAAJ/GjRun1q1bhzoNGlgAAAAAAOD0NWfOHBmG4fe/7777LtQpVuuXX37Ro48+qu3bt4c6lTrDrxACAAAAAIDT3rRp09SmTZtK8bZt24Ygm5r55ZdfNHXqVA0YMMASo6XqQq00sPLy8vTkk09q9erVWrNmjQ4dOqTZs2dr3LhxnmncbrfeeOMNffDBB1q3bp2ys7PVpk0bXXPNNfrTn/6k6Ojo2kgFAAAAAAAE0aJNoc5AGtT55OcxZMgQ9ejR4+RnhDpRK7cQZmVladq0adq8ebO6du3qc5qjR49q/PjxOnDggCZOnKhZs2apV69emjJlioYMGSLTNGsjFQAAAAAAgFo1ZcoU2Ww2LV261Ct+8803KzIyUhs2bJAkLV++XIZh6N1339UDDzygpk2bqn79+hoxYoR27txZab6rV6/W4MGDFR8fr3r16ql///5auXJlpel2796tCRMmqHnz5oqKilKbNm106623qri4WHPmzNFVV10lSRo4cKDn1sfly5d73r9w4UL17dtX9evXV4MGDTRs2DD9/PPPlZbzn//8R507d1Z0dLQ6d+6sDz/88GQ+tlpVKyOwmjVrpj179qhp06Zau3atevbsWWmayMhIrVy5Uueff74n9n//939q3bq1pkyZoqVLl+qSSy6pjXQAAAAAAABqJCcnR1lZWV4xwzCUmJiohx56SB9//LEmTJign376SQ0aNNAXX3yhf/zjH/rLX/5SaTDP9OnTZRiG7r//fu3fv1+zZs3SJZdcovXr1ysmJkaS9OWXX2rIkCE699xzPQ2y2bNn66KLLtKKFSvUq1cvSVJmZqZ69eqlw4cP6+abb1aHDh20e/duzZ8/X0ePHlW/fv00adIkPffcc3rggQfUsWNHSfL875tvvqmxY8fq0ksv1RNPPKGjR4/qpZde0oUXXqh169Z5bjlctGiRRo0apbPOOkszZ87UwYMHNX78eCUnJ9flxx6wWmlgRUVFqWnTplVOExkZ6dW8KnPFFVdoypQp2rx5Mw0sAAAAAAAQEr56ElFRUSosLFRERITeeOMNnXvuubr77rv15JNPasKECerRo4f+/Oc/V3pfdna2Nm/erAYNGkiSunfvrquvvlr/+Mc/NGnSJJmmqYkTJ2rgwIFauHChDMOQJN1yyy3q1KmTHnroIS1atEiSNHnyZO3du1erV6/2usVx2rRpMk1TCQkJ6tu3r5577jn97ne/04ABAzzT5OXladKkSbrpppv06quveuJjx45V+/btNWPGDE/8/vvvV5MmTfTNN98oPj5ektS/f38NGjRIrVq1OslP9+SF/CHue/fulSQ1atQoxJkAAAAAAIDT1d///nedeeaZXjG73e75/507d9bUqVM1efJkbdy4UVlZWVq0aJEcjsqtlTFjxniaV5J05ZVXqlmzZvrss880adIkrV+/Xlu3btVDDz2kgwcPer334osv1ptvvim32y2p9La+4cOH+3w+V1njy5/Fixfr8OHDuvbaa71Gl9ntdvXu3VvLli2TJO3Zs0fr16/Xn//8Z0/zSpJ+97vf6ayzzlJ+fn6VywmGkDew/vrXvyouLk5DhgzxO01RUZGKioo8/87NzZUkOZ1OOZ1OSZLNZpPNZpPb7fas5Ipxl8vl9Zwtf3G73S7DMDzzrRiXJJfLFVDc4XDINE2vuGEYstvtlXL0F6cmaqImaqImaqImaqImaqImaqImagp1TU6n0zM/38+vNiSFNn6ij9U2DMNTU8+ePT1NoorxijXfe++9euedd7RmzRpNnz5dHTt2lGmanunLpm3btq1XvCy2fft2maaprVu3SiodCeXP4cOHVVxcrNzcXHXq1KnKZ4cfn2vZ/6anp0uSLrroIp/vi4uLkyRt377dK++Kn0H79u31448/Vor7y6Nir6bitnf89ldTIW1gzZgxQ0uWLNGLL76ohIQEv9PNnDlTU6dOrRRft26d6tevL0lq3Lix0tLSlJGRoQMHDnimSU5OVnJystLT05WTk+OJp6amKikpSZs2bVJBQYEn3qFDByUkJGjdunVeO3GXLl0UGRmptWvXeuXQo0cPFRcXa+PGjZ6Y3W5Xz549lZOToy1btnjiMTEx6tq1q7KysrRt2zZPPD4+Xh07dlRmZqZ27drliVu2ph9+KK8pIkJdmzdXVl6etlXoGsfHxKhjUpIyDx/Wrgo5No6NVVpiojIOHtSBvLzymuLjlZyQoPT9+5VTIffUxEQlxcZqU2amCkpKymtKSlJCTIzWHTrEeqImaqImaqImaqKm06Om/Pzqr4127pSrwpfcLs2aKdLh0NrjHhzcIyVFxU6nNu7ZU16TzaaeKSnKKSjQlv37y2vydb1Xvz7riZqo6TSrKTo6WlJpU6uwsNATt9lskurJ5XJ5NShsNpsiIiIrxe12uxyOCDmdTq9cHA6H7HaHSkpKvJp1ZfHi4mKvpklERIRsNrsnnp/v9HzGNput0oih+vXry+12e30uhmF44pJUUFCg/Px82Ww21atXT06n02swjd1u165duzzNp/Xr1ys/P18Oh0PR0dEqKiryfDZFRUUqKSlRZGSkCgsL5XK55HK55Ha75XQ6Pct87LHH1KVLF0mlj16y2+0qLCz0NL+OHj3qWX5VNZXlWbb8svVU9u/XXntNrVq1ktPpVEmF80dkZKQkedZRUVFRpZrKGpj5+fmKjIz0qqlMVFSUJKmkpESbNpX/LGXFba9sMNKJMsxa/vm/soe4z549W+PGjfM73bvvvqtrr71WN954o1577bUq5+lrBFZKSooOHjzo6RZapTNd5lTqtleq6djOKpX2u+02m9ymKXeFZfqL247l6Xa7VV6RZDMM2QxDLrfbq6/uL24/9qsKzmMPmzvpmk7F9URN1ERN1ERN1ERNp1ZN27ZVf21UYR5lcUlyHXfJ7y/usNlKa6ruui41lfVETdR0GtVUWFio//3vf0pNTfU0Kipa/HPoR2D9rpOPlwNgGIZmz56tG2+8UWvWrPE5AquM2+1Wv379tG3bNo0fP14zZ87U/PnzNXLkSM/0y5cv10UXXaQ///nPmjFjhtfIrOTkZHXp0kULFy7U2rVr1atXL7388su6+eabvfKpuFy3262GDRtq4MCBVf4i4Pvvv6+rrrpKX375pQYOHOiZx3vvvafRo0fr888/16WXXupz5JRhGMrMzFSLFi10//33a+bMmV65dO7cWfn5+crIyPD72UilvZtt27apZcuWnoZnxW0vNzdXiYmJysnJ8fRyaiIkI7AWL16sMWPGaNiwYXr55ZernT4qKsrnTuJwOCrda1q2wx6vbAcMNO7rHtaaxg3D8Bn3l2NN4yGryVeOxy6mAo7bbKo8l9KLI1/8xVlP1ERN1FRVnJqoiZqoqap42NVU4XW/10b+4j6ux/zFDcPwGfe6rqtQM+uJmvzlWNM4NVm3JofDIePY/m/4OZ6UNpNCF/ebVgAq1laxvuNrfeaZZ/Ttt99qwYIFGjZsmL766ivddttt6t+/vxo1auT1/jfffFMPPPCAGjRoIMMwNH/+fO3Zs0f333+/DMPQueeeq7S0NP3tb3/Tddddp9jYWK/lHjhwQI0bN5bdbtfvf/97vfXWW/rhhx8qPQerbKRW2fvLRuSV5TF48GDFxcVp5syZuuiiixQREeH1/rLlNG/eXN26ddMbb7yhyZMne56DtWTJEv3yyy9q1apVlZ9NxbivXo2vWE0FvYG1evVqXXHFFerRo4fmzZt30gUAAAAAAACcrIULF3rd8lnm/PPPV1FRkR5++GGNGzdOw4cPlyTNmTNH3bp102233aZ58+Z5vadhw4a68MILNX78eO3bt0+zZs1S27Zt9X//93+SSpuSr732moYMGaJOnTpp/PjxatGihXbv3q1ly5YpLi5OH3/8saTSxy8tWrRI/fv3180336yOHTtqz549eu+99/TNN98oISFB3bp1k91u1xNPPKGcnBxFRUXpoosuUlJSkl566SXdcMMN6t69u6655ho1btxY//vf//Tpp5/qggsu0AsvvCCp9PFNw4YN04UXXqgbb7xR2dnZev7559WpUyflVXgEUKgEtXu0efNmDRs2TK1bt9Ynn3yimJiYYC4eAAAAAADAp0ceecRn/LXXXtMrr7yiRo0aadasWZ54u3btNHPmTN15552aN2+err76as9rDzzwgDZu3KiZM2fqyJEjuvjii/Xiiy+qXr16nmkGDBigVatW6S9/+YteeOEF5eXlqWnTpurdu7duueUWz3QtWrTQ6tWr9fDDD2vu3LnKzc1VixYtNGTIEM/8mjZtqpdfflkzZ87UhAkT5HK5tGzZMiUlJekPf/iDmjdvrscff1xPPvmkioqK1KJFC/Xt21fjx4/3LGfw4MF677339NBDD2ny5MlKS0vT7Nmz9dFHH2n58uW19CmfuFp7BtYLL7ygw4cPKzMzUy+99JJGjhypc845R5J0xx13yGazqVOnTtq9e7dmzJihFi1aeL0/LS1Nffr0CWhZubm5io+PP+H7JnGSfv011BmUa9s21BkAAAAEB9dgAEKksLBQGRkZatOmjefZRvBt+fLlGjhwoN577z1deeWVoU4nqKrbTk62l1NrI7Ceeuop7dixw/PvDz74QB988IEk6frrr5ck7Tz26yd//vOfK71/7NixATewAAAAAAAAcPqotQbW9u3bq52mln/wEAAAAAAAAKcB3z9TAgAAAAAAAFgEPwEIAAAAAABQCwYMGMDdZ3WEEVgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAOC0NWfOHBmGoejoaO3evbvS6wMGDFDnzp1DkBkqcoQ6AQAAAAAAEMY+/zzUGUiDB5/0LIqKivT444/r+eefr4WEUNsYgQUAAAAAAE573bp10z/+8Q9lZmaGOhX4QAMLAAAAAACc9h544AG5XC49/vjjVU7ndDr1l7/8RWlpaYqKilLr1q31wAMPqKioyDPN3XffrcTERJmm6YndcccdMgxDzz33nCe2b98+GYahl156qfYLOsXQwAIAAAAAAKe9Nm3aaMyYMdWOwrrpppv0yCOPqHv37nrmmWfUv39/zZw5U9dcc41nmr59+yo7O1s///yzJ7ZixQrZbDatWLHCKyZJ/fr1q4OKTi00sAAAAAAAACQ9+OCDcjqdeuKJJ3y+vmHDBr3++uu66aab9N577+m2227T66+/rj/96U/6z3/+o2XLlkmSLrzwQknlDaqcnBz99NNPGjVqVKUGVsOGDXXWWWfVcWXhjwYWAAAAAACApNTUVN1www169dVXtWfPnkqvf/bZZ5JKbxGs6J577pEkffrpp5Kkxo0bq0OHDvr6668lSStXrpTdbte9996rffv2aevWrZJKG1gXXnihDMOos5pOFTSwAAAAAAAAjnnooYfkdDp9Pgtrx44dstlsatu2rVe8adOmSkhI0I4dOzyxvn37ekZbrVixQj169FCPHj3UsGFDrVixQrm5udqwYYP69u1btwWdImhgAQAAAAAAHJOamqrrr7/e7ygsSQGNmLrwwgu1e/dubdu2TStWrFDfvn1lGIYuvPBCrVixQt9++63cbjcNrADRwAIAAAAAAKigbBTW8c/CatWqldxut+cWwDL79u3T4cOH1apVK0+srDG1ePFiff/9955/9+vXTytWrNCKFStUv359nXvuuXVczamBBhYAAAAAAEAFaWlpuv766/XKK69o7969nvjQoUMlSbNmzfKa/umnn5YkDRs2zBNr06aNWrRooWeeeUYlJSW64IILJJU2tn777TfNnz9f5513nhwORx1Xc2qggQUAAAAAAHCcBx98UCUlJfrvf//riXXt2lVjx47Vq6++qtGjR+vFF1/UuHHj9Ne//lW///3vNXDgQK959O3bV//973/VuXNnnXHGGZKk7t27q379+kpPT+f2wRqggQUAAAAAAHCctm3b6vrrr68Uf+211zR16lR9//33uuuuu/Tll19q8uTJeueddypNW9aguvDCCz0xh8OhPn36eL2O6hmmaZqhTqKmcnNzFR8fr5ycHMXFxYU6ndPPr7+GOoNyx/3yAwAAwCmLazAAIVJYWKiMjAy1adNG0dHRoU4HFlXddnKyvRxGYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNIcoU4Ax/CzyAAAAAAAAD4xAgsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAACgjhiGoUcffTTUaYQ9GlgAAAAAAOC0ZBhGQP8tX7481Kme9hyhTgAAAAAAAISxX38NdQZS27Yn9LY333zT699vvPGGFi9eXCnesWPHE04NtYMGFgAAAAAAOC1df/31Xv/+7rvvtHjx4kpxhB63EAIAAAAAAPiRn5+ve+65RykpKYqKilL79u311FNPyTRNr+mKior0//7f/1Pjxo3VoEEDjRgxQrt27ao0vx07dui2225T+/btFRMTo8TERF111VXavn27Z5pt27bJMAw988wzld7/7bffyjAM/fvf/671Wq2MBhYAAAAAAIAPpmlqxIgReuaZZzR48GA9/fTTat++ve69917dfffdXtPedNNNmjVrlgYNGqTHH39cERERGjZsWKV5fv/99/r22291zTXX6LnnntPEiRO1dOlSDRgwQEePHpUkpaam6oILLtDcuXMrvX/u3Llq0KCBLr/88rop2qK4hRAAAAAAAMCHBQsW6Msvv9Rjjz2mBx98UJL0xz/+UVdddZWeffZZ3X777UpLS9OGDRv01ltv6bbbbtPf//53z3TXXXedNm7c6DXPYcOG6corr/SKDR8+XH369NH777+vG264QZI0ZswY3XLLLdqyZYs6dOggSSopKdG8efM0cuRI1atXr67LtxRGYAEAAAAAAPjw2WefyW63a9KkSV7xe+65R6ZpauHChZ7pJFWa7q677qo0z5iYGM//Lykp0cGDB9W2bVslJCToxx9/9Lx29dVXKzo62msU1hdffKGsrKzT8hldNLAAAAAAAAB82LFjh5o3b64GDRp4xct+lXDHjh2e/7XZbEpLS/Oarn379pXmWVBQoEceecTzTK1GjRqpcePGOnz4sHJycjzTJSQkaPjw4Xr77bc9sblz56pFixa66KKLaq3GcEEDCwAAAAAAIEjuuOMOTZ8+XVdffbXmzZunRYsWafHixUpMTJTb7faadsyYMdq2bZu+/fZbHTlyRAsWLNC1114rm+30a+fwDCwAAAAAAAAfWrVqpSVLlujIkSNeo7C2bNnieb3sf91ut3777TevUVf//e9/K81z/vz5Gjt2rP72t795YoWFhTp8+HClaQcPHqzGjRtr7ty56t27t44ePep5Rtbp5vRr2QEAAAAAAARg6NChcrlceuGFF7zizzzzjAzD0JAhQyTJ87/PPfec13SzZs2qNE+73S7TNL1izz//vFwuV6VpHQ6Hrr32Ws2bN09z5szR2WefrS5dupxMSWGLEVgAAAAAAAA+DB8+XAMHDtSDDz6o7du3q2vXrlq0aJE++ugj3XXXXZ5nXnXr1k3XXnutXnzxReXk5Oj888/X0qVL9euvv1aa52WXXaY333xT8fHxOuuss7Rq1SotWbJEiYmJPnMYM2aMnnvuOS1btkxPPPFEndZrZTSwAAAAAAAAfLDZbFqwYIEeeeQRvfvuu5o9e7Zat26tJ598Uvfcc4/XtP/61788t/v95z//0UUXXaRPP/1UKSkpXtM9++yzstvtmjt3rgoLC3XBBRdoyZIluvTSS33mcO6556pTp07avHmzrrvuujqr1eoM8/hxa2EgNzdX8fHxysnJUVxcXKjTqR0+urIh07Zt1a+HU64AAACnCq7BAIRIYWGhMjIy1KZNG0VHR4c6ndPSOeeco4YNG2rp0qWhTsWv6raTk+3l8AwsAAAAAAAAi1q7dq3Wr1+vMWPGhDqVkOIWQgAAAAAAAIvZtGmTfvjhB/3tb39Ts2bNNHr06FCnFFKMwAIAAAAAALCY+fPna/z48SopKdG///3v0/72TRpYAAAAAAAAFvPoo4/K7XZr8+bN6t+/f6jTCTkaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAACgWqZphjoFWFhdbx80sAAAAAAAgF92u12SVFJSEuJMYGVl20fZ9lLbaGABAAAAAAC/IiIiFBUVpZycHEZhwSfTNJWTk6OoqChFRETUyTIcdTJXAAAAAABwymjUqJF2796tXbt2KT4+XhERETIMI9RpIcRM01RJSYlycnKUl5enFi1a1NmyaGABAAAAAIAqxcXFSZKysrK0e/fuEGcDq4mKilKLFi0820ldoIEFAAAAAACqFRcXp7i4OJWUlMjlcoU6HViE3W6vs9sGK6KBBQAAAAAAAhYRERGUhgVQUa08xD0vL09TpkzR4MGD1bBhQxmGoTlz5vicdvPmzRo8eLBiY2PVsGFD3XDDDTpw4EBtpAEAAAAAAIBTUK2MwMrKytK0adPUsmVLde3aVcuXL/c53a5du9SvXz/Fx8drxowZysvL01NPPaWffvpJa9asUWRkZG2kAwAAAAAAgFNIrTSwmjVrpj179qhp06Zau3atevbs6XO6GTNmKD8/Xz/88INatmwpSerVq5d+97vfac6cObr55ptrIx0AAAAAAACcQmrlFsKoqCg1bdq02unef/99XXbZZZ7mlSRdcsklOvPMMzVv3rzaSAUAAAAAAACnmFppYAVi9+7d2r9/v3r06FHptV69emndunXBSgUAAAAAAABhJGi/Qrhnzx5JpbcbHq9Zs2bKzs5WUVGRoqKiKr1eVFSkoqIiz79zc3MlSU6nU06nU5Jks9lks9nkdrvldrs905bFXS6XTNOsNm6322UYhme+FeOSKv1UqL+4w+GQaZpeccMwZLfbK+VoGIbsktymKXfFHI/l6Xa75a4wb5thyGYYcrndMgOI2w2jtCZ3xbmUxiXJZZre8WP/9ltTxdwl2W22Srn7i9d6TcFeTz7iYb/tURM1URM1URM1UVN41OR21971np+4w2Yrram66zqnk/VETdRETdRETTWq6fi6aipoDayCggJJ8tmgio6O9kzj6/WZM2dq6tSpleLr1q1T/fr1JUmNGzdWWlqaMjIyvH7VMDk5WcnJyUpPT1dOTo4nnpqaqqSkJG3atMmTmyR16NBBCQkJWrdundfK7tKliyIjI7V27VqvHHr06KHi4mJt3LjRE7Pb7erZs6dycnK0ZcsWTzwmJkZdu3ZVVlaWtm3b5onHx8erY0SEMnNytKtCjo1jY5WWmKiMQ4d0IC+vvKb4eCUnJCg9K0s5FXJPTUxUUmysNu3dq4KSkvKakpKUEBOjdbt3ezWfujRrpkiHQ2t37vSuKTW16poqTB8TEaGuzZsrKz9f2w4eLK8pJkYdk5LqvqZgr6eOHZWZmaldu3aV1xTu2x41URM1URM1UdPpXNOxP4xKVVwbpaSo2OnUxmN/kJVKGzo9U1KUU1CgLfv3l9dUdm2Ul+f72ujwYd/XRgcP6kCFC36fNeXn1971XlU1FRb6rqni9V52NtseNVETNVETNdWoptwK59wTYZjmcX92OUllD3GfPXu2xo0bVyn+xhtv6IYbbvB6z3333acnn3xShYWFAY/ASklJ0cGDBxUXFyfpFOh4ZmRYZwRWu3ZV17R1a3nuCvEIrNatvXM/RTrT1ERN1ERN1ERN1BSkmipcxNfZaKUq4l7XRqmpVee+bZt1RmClprLtURM1URM1UVONasrNzVViYqJycnI8vZyaCNoIrLJbB/dU+CtPmT179qhhw4Y+m1dS6agtX685HA45HN4llH1oxytbsYHGj5/vicQNw/AZ95dj2QWJz+l9LNPuYx5VxR3+4scv89i//dZUk9zruqZQrKcaxsNi26MmavKTY03j1ERNEjX5y7GmcWoKUk0+5lPp2qiKuGEYPuMndG3k47Pxyr1Crid9vVdFPKCaKuTKtkdN/nKsaZyaqEmiJn851jRuxZr85R+ooD3EvUWLFmrcuHGlIW+StGbNGnXr1i1YqQAAAAAAACCMBK2BJUmjRo3SJ598op0V7sFfunSp0tPTddVVVwUzFQAAAAAAAISJWruF8IUXXtDhw4eVmZkpSfr44489DwC74447FB8frwceeEDvvfeeBg4cqDvvvFN5eXl68skndfbZZ2v8+PG1lQoAAAAAAABOIbX2EPfWrVtrx44dPl/LyMhQ62MP2/755591991365tvvlFkZKSGDRumv/3tb2rSpEnAy8rNzVV8fPwJP/jLkn79NdQZlGvbturXwylXAACAqoTTdU045QoAwHFOtpdTayOwtm/fHtB0nTp10hdffFFbiwUAAAAAAMApLqjPwAIAAAAAAABqigYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAszRHqBAAAAHAK+fXXUGdQrm3bUGcAAABqCSOwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpQW9gbd26Vddcc42Sk5NVr149dejQQdOmTdPRo0eDnQoAAAAAAADCgCOYC9u5c6d69eql+Ph43X777WrYsKFWrVqlKVOm6IcfftBHH30UzHQAAAAAAAAQBoLawHrzzTd1+PBhffPNN+rUqZMk6eabb5bb7dYbb7yhQ4cO6YwzzghmSgAAAAAAALC4oN5CmJubK0lq0qSJV7xZs2ay2WyKjIwMZjoAAAAAAAAIA0FtYA0YMECSNGHCBK1fv147d+7Uu+++q5deekmTJk1S/fr1g5kOAAAAAAAAwkBQbyEcPHiw/vKXv2jGjBlasGCBJ/7ggw/qscce8/u+oqIiFRUVef5dNpLL6XTK6XRKkmw2m2w2m9xut9xut2fasrjL5ZJpmtXG7Xa7DMPwzLdiXJJcLldAcYfDIdM0veKGYchut1fK0TAM2SW5TVPuijkey9PtdstdYd42w5DNMORyu2UGELcbRmlN7opzKY1Lkss0vePH/u23poq5S7LbbJVy9xev9ZqCvZ58xMN+26MmaqImaqImaqrNmsquI467vnDYbKU1BXC9UGvXEW539TVV+Gz8Xhv5idd6TRU+Y5/rw+2uveu9k63J6bTetncq7k/URE3URE2nUE3H11VTQW1gSVLr1q3Vr18/jRo1SomJifr00081Y8YMNW3aVLfffrvP98ycOVNTp06tFF+3bp1n1Fbjxo2VlpamjIwMHThwwDNNcnKykpOTlZ6erpycHE88NTVVSUlJ2rRpkwoKCjzxDh06KCEhQevWrfNa2V26dFFkZKTWrl3rlUOPHj1UXFysjRs3emJ2u109e/ZUTk6OtmzZ4onHxMSoa9euysrK0rZt2zzx+Ph4dYyIUGZOjnZVyLFxbKzSEhOVceiQDuTlldcUH6/khASlZ2Upp0LuqYmJSoqN1aa9e1VQUlJeU1KSEmJitG73bq/mU5dmzRTpcGjtzp3eNaWmVl1TheljIiLUtXlzZeXna9vBg+U1xcSoY1JS3dcU7PXUsaMyMzO1a9eu8prCfdujJmqiJmqiJuvXlJ9ffs7Ny/N9zj182Pc59+BB3+fc/ft9n3MzM32fc3fuLL2OOHbt5bemhg1V7HRq45495TXZbOqZkqKcwkJt2b+/fD3V9XVEQkL16+nYH0alKq6NUlKCU1OFz9LntpefX3vXeydbU3Z2+O5POgWPEdRETdRETWFQU26Fc+6JMEzzuD+71KF33nlHN954o9LT05WcnOyJjx8/XvPmzdP//vc/JSYmVnqfrxFYKSkpOnjwoOLi4iSdAh3PjAzrjMBq167qmrZuLc9dIR6B1bq1d+6nSGeamqiJmqiJmqjJq6Zt20J/zi37XFJTq64pI6M0boURWG3bVr+eKlzEh3wE1rHPVvKzjW3bZp0RWKmp4bs/6RQ8RlATNVETNYVBTbm5uUpMTFROTo6nl1MTQW1g9evXTy6XSytXrvSKf/jhhxo5cqQWL16sSy65pNr55ObmKj4+/oSLtqRffw11BuXatq369XDKFQCAU0E4nXvDKVcpvPINp1wBADjOyfZygvoQ93379lXqDEpSybHhzyd7PyQAAAAAAABOPUFtYJ155plat26d0tPTveL//ve/ZbPZ1KVLl2CmAwAAAAAAgDAQ1Ie433vvvVq4cKH69u2r22+/XYmJifrkk0+0cOFC3XTTTWrevHkw0wEAAAAAAEAYCGoDq1+/fvr222/16KOP6sUXX9TBgwfVpk0bTZ8+Xffdd18wUwEAAAAAAECYCGoDS5J69eqlzz77LNiLBQAAAAAAQJgK6jOwAAAAAAAAgJqigQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABLc4Q6AaDO/fprqDMo17ZtqDMAAAAIDq7BAAC1iBFYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNBpYAAAAAAAAsDRHqBMAAAAAUL1Vv4U6g3J92oY6AwDA6YYGFgAAAIBaR8MNAFCbuIUQAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWRgMLAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACW5gh1AgAAAAAQSos2hTqDcoM6hzoDALAmRmABAAAAAADA0kIyAuvHH3/Uo48+qm+++UaFhYVKTU3VzTffrEmTJoUiHQAAAJymVv0W6gzK9Wkb6gwAALCuoDewFi1apOHDh+ucc87Rww8/rNjYWP3222/atWtXsFMBAAAAAABAGAhqAys3N1djxozRsGHDNH/+fNls3MEIAAAAAACAqgW1g/T2229r3759mj59umw2m/Lz8+V2u4OZAgAAAAAAAMJMUBtYS5YsUVxcnHbv3q327dsrNjZWcXFxuvXWW1VYWBjMVAAAAAAAABAmgnoL4datW+V0OnX55ZdrwoQJmjlzppYvX67nn39ehw8f1r///W+f7ysqKlJRUZHn37m5uZIkp9Mpp9MpSbLZbLLZbHK73V6jusriLpdLpmlWG7fb7TIMwzPfinFJcrlcAcUdDodM0/SKG4Yhu91eKUfDMGSX5DZNuSvmeCxPt9utiuPUbIYhm2HI5XbLDCBuN4zSmo4b7WY3jNLcTdM7fuzffmuqmLsku81WKXd/8VqvKZD15Hb7rdVhs5XWFEDutVKT02m9bc9HPOz3J2qiJmqiplOtJrc79Ofcss/lWG1+ayq7jgj1OVeSze2udj2ZZsU5Gcf+1zt3f3HDsB2bb23E3V7bja9trDTX0vXhnbeqjNdFTU6ns9r9qSY5BqOmqo4R5YswZNjspcusuFzD5llPPuNul/dy/cZLtz3T7X2MkGE/lrpLFQ8fp/Vxj5qoiZpOuZqOr6umgtrAysvL09GjRzVx4kQ999xzkqSRI0equLhYr7zyiqZNm6Z27dpVet/MmTM1derUSvF169apfv36kqTGjRsrLS1NGRkZOnDggGea5ORkJScnKz09XTk5OZ54amqqkpKStGnTJhUUFHjiHTp0UEJCgtatW+e1srt06aLIyEitXbvWK4cePXqouLhYGzdu9MTsdrt69uypnJwcbdmyxROPiYlR165dlZWVpW3btnni8fHx6hgRocycHO2qkGPj2FilJSYq49AhHcjLK68pPl7JCQlKz8pSToXcUxMTlRQbq01796qgpKS8pqQkJcTEaN3u3V7Npy7NminS4dDanTu9a0pNrbqmCtPHRESoa/PmysrP17aDB8triolRx6Skuq8pkPWUn68eKSkqdjq1cc+e8ppsNvVMSVFOYaG27N8fnJqys6237XXsqMzMTK8fUgj7/YmaqKmqmnbtqnzcq+oYUVDg+xiRl+f7GHH4sO9jxMGDlY8RPXqwnqgpsJry80N/zi27jsjOrrqmhg2tcc6VlJqQUO16yinJ9cQbRDSTTQ7llHgfI+IjUuSWU0dKymsyZFN8ZIqcZqHyneU12Y0INYhormJ3vgpc5TU5jBjFRiSpyJ2jQld5TZG2WNVzJKrAdcjrs/S17eWU5CvGnqgoe6zynHvlMsvXU31HkiKMGOWW7JZZob1XVzWtXZtd7f5U4DqkYnf5eoq2xyvanqB8Z5acZvn6CEZN1R0jio+Uxm1R8Ypo2FGuvEy58sprssc0liMhTa6cDLkKyo8R9thkORoky3k4Xe6i8vXqiE+VvV6SSg5ukuksrzWiYQcZUQkq2b9Opll+jIho1EWGPVLF+9Zq7dHymk7r4x41URM1nXI1lQ1GOlGGWbE1Vsc6d+6sn3/+WV999ZX69evniX/99dfq37+/Xn/9dY0ZM6bS+3yNwEpJSdHBgwcVFxcn6RToeGZkWGcE1rEmot+atm4tz10h/mtw69beuftaH9u2WWcEVmqq9bY9/oJATadbTb/+Wvm4F6pjRLt2rCdqCqymbdtCf84t+1xSU6uuKSOjNB7qc64kW9u21a6nNUu2VXhHaEdg9boktTx3H9tYaa7WGIHV65LUavenbz9PDzjHuq7pvEFpVR4jlv5SYZkhHoF18Vnl4dP6uEdN1ERNp1xNubm5SkxMVE5OjqeXUxNBHYHVvHlz/fzzz2rSpIlXPCkpSZJ06NAhn++LiopSVFRUpbjD4ZDD4V1C2Yd2vLIVG2j8+PmeSNwwDJ9xfzmWXXz5nN7HMu0+5lFV3OEvfvwyj/3bb001yb2uawpkfVR4b6VadaymmuR+MjVVyMtS214N42GxP1ETNfnJUX72eSlExwjWEzX5iXvVVCGnkJ1zy+LH5Vop97LriFCfc0snLI1XsZ4Mw9ecfB8jfMUNw6iluM3ndlAx94q5+s7bf7y2a6qYq7/9pqY51nVNVR0jjl+EYdhUKVhV3OZ7G/Mf9/M1zHAcv4tJOk2PewHkSE3U5C/HmsapKTg1+cs/UEF9iPu5554rSdq9e7dXPDMzU1LpEDUAAAAAAACgoqA2sK6++mpJ0j//+U+v+GuvvSaHw6EBAwYEMx0AAAAAAACEgaDeQnjOOefoxhtv1L/+9S85nU71799fy5cv13vvvafJkyerefPmwUwHAAAAAAAAYSCoDSxJevnll9WyZUvNnj1bH374oVq1aqVnnnlGd911V7BTAQAAAAAAQBgIegMrIiJCU6ZM0ZQpU4K9aAAAAAAAAIShoD4DCwAAAAAAAKgpGlgAAAAAAACwtKDfQggAAAAAOHGLNoU6g3KDOoc6AwCnC0ZgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0hyhTgAAAACnjlW/hTqDcn3ahjoDAABQWxiBBQAAAAAAAEujgQUAAAAAAABL4xZCAAAAAECdWLQp1BmUG9Q51BkAOBmMwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApTlCnQAAAAAAAFawaFOoMyg3qHOoMwCshRFYAAAAAAAAsDQaWAAAAAAAALA0GlgAAAAAAACwNJ6BBQA4Ob/+GuoMyrVtG+oMAABhqMFuC53LOnMuAwBfaGABAAAAABBmeOA8TjfcQggAAAAAAABLo4EFAAAAAAAAS6OBBQAAAAAAAEujgQUAAAAAAABL4yHuAAAAAACgTvHQeZwsRmABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSHKFOAAAAAAAAwCoWbQp1BuUGdQ51BtbBCCwAAAAAAABYGg0sAAAAAAAAWBoNLAAAAAAAAFgaz8ACAACwuFW/hTqDcn3ahjoDAABwOmIEFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACyNBhYAAAAAAAAsjQYWAAAAAAAALI0GFgAAAAAAACzNEeoEUGrVb6HOoFyftqHOAAAAAAAAoBwjsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpIW9gTZ8+XYZhqHPnzqFOBQAAAAAAABYU0gbWrl27NGPGDNWvXz+UaQAAAAAAAMDCHKFc+J/+9Cedd955crlcysrKCmUqAAAAAAAAsKiQjcD6+uuvNX/+fM2aNStUKQAAAAAAACAMhKSB5XK5dMcdd+imm27S2WefHYoUAAAAAAAAECZCcgvhyy+/rB07dmjJkiUBTV9UVKSioiLPv3NzcyVJTqdTTqdTkmSz2WSz2eR2u+V2uz3TlsVdLpdM06w2brfbZRiGZ74V41Jp8y2QuMPhkGmaXnHDMGS32yvlaBiGJB3Lw/Saj2HYZJpueTNkGEatxEt5L7Ps8/BbU8XcJdltNrlNU+4Kn6O/uE0qX08V5m0zDNkMQy632ysbf3G7YQS+ntxu2Y99xi7Tu1aHzVZaUwC510pNTqfltj1f8XDfn6gpyDUdW3bQ9ydf8WM1VFnTcTlKCt0x4tjnyLZHTdXVVHYOL70u8He9EJzrCGeF/cxX7uWfR01yrJua3G53tevJ+z2+r438xWu7porbja9trDTX2rneO9manE5ntftTsK9hq6upqmNExWUEc3/ylXvF7cDffiaVHiNkVowbMmz20nkft137jBu28pp8xd0u78/AT9w0qz7ulU5fMR37sTd6xw1b3dcUyLG8dDcrrcl0e9fkL/e6qsnprPr8JAW+nuq6Jqn6c66n3Fra9k6mpoqbq6/rCNMdmv3JV01O56lzbXT8caKmgt7AOnjwoB555BE9/PDDaty4cUDvmTlzpqZOnVopvm7dOs8D4Bs3bqy0tDRlZGTowIEDnmmSk5OVnJys9PR05eTkeOKpqalKSkrSpk2bVFBQ4Il36NBBCQkJWrdundfK7tKliyIjI7V27VqvHHr06KHi4mJt3LjRE7Pb7erZs6dycnK0ZcsWTzwmJkZdu3ZVVlaWtm3b5onHx8dLilCRO0eFrvIcI22xqudIVIHrkIrdeZ54tD1e0fYE5Tuz5DTLc4+xJyrKHqs85165zBJPvL4jSRFGjHJLdsus8PWpQUQz2eRQTslOr5pcrtSqa9pZPn1MRIS6Nm+urPx8bTt4sLymmBh1TEpSZk6OdlX43BvHxiotMVEZhw7pQF55Tcnx8UpOSFB6VpZyKqyP1MREJcXGatPevSooKa+pQ1KSEmJiAltP+fnqkZKiYqdTG/fsKa/JZlPPlBTlFBZqy/79wakpO9ty217Hjh2VmZmpXbt2ldcU5vsTNQW5pvz80OxP8nGMyM6uvibT1Nqd3se9kB0jJLY9agqoppySfNmNCDWIaK5id74KXOXbnsOIUWxEUtCuI9auza6yJqmh3HLqSEn5/mTIpvjIFDnNQuU7y/enuq4pKyuh2vWUU5Lrifu7NoqPSAlKTRU/S1/bXk5Jfq1d751sTWvXZle7PwX7Graqmqo7RuSU5Ae8nuq6prJ9TPJ/jFBMT5nFOSrJLq/JcMQosnFXuQuy5MwpP+7ZouIV0bCjXHmZcuWVryd7TGM5EtLkysmQq6D8uGePTZajQbKch9PlLir/DBzxqbLXS1LJwU0yneW15rSs+rhXvM/7GBHZpIdMV7FKssprMgy7IpvWfU2BHMvdB/JL15MtRjnFO09q24uLTFGJu8Dn/lTkyvN5jCh0HfZse2uP1q/y/CQFvp4iGnaQEZWgkv3rZFZo7EQ06iLDfvLrSar+nFt8JLD1FIya1h49tkw/1xElBaHZn3zVtPboqXNtVDYY6UQZZsXWWBDceuutWrJkiX7++WdFRkZKkgYMGKCsrCxt2rTJ53t8jcBKSUnRwYMHFRcXJ8n6fzmVqu54rlmSYZkRWH0ubVd1TVu3es0hpCOwWrf2ytHn+ti2zTojsFJTLbftheNIBGqyWE3HToCWGIGVmlp9Tb/+ap0RWO3ase1RU0A1rVmy7Vj+oR+B1euS8v3MV+5rlmQc+3+hH4F13qC21a6nss+2bD6+cg/WCKyyz1byvY2V5mqNEVi9Lkmtdn/69vP0gHOs65rOG5RW5TGi4nYQ6hFYFbcDf/vZl1usMwJr0NlVH/cW/WSdEVgXd6z+WF7dfnYs+YDiJ3uM6HVJapXnpyW/WGcE1qVdqj/nLv3luBxDOALr4rPKw76uI5b+Yp0RWBefdepcG+Xm5ioxMVE5OTmeXk5NBHUE1tatW/Xqq69q1qxZyszM9MQLCwtVUlKi7du3Ky4uTg0bNvR6X1RUlKKioirNz+FwyOHwLqHsQzte2YoNNH78fE8kbhiGz7i/HEtvJTR8xH0/qqy24scvs+yWRr81+ci97EtkwHGbzecD2Ow+5l1VPKD1UeG9Dh+5GIbhM14nNVXIy0rbXk3j4bA/UVMQa6qw7KDuT77ix+XqM3c/OUohOkaw7VGTn3jFmiqew/1fLwTnOuL4XI//t+HZ/muSY93UVLYuq1pPvufl+xhR1zX52g4q5u69HZzc9V5V8UByr5ir/2vb4F7DVhWv7hhx/DJCeV3uK09/xwgZvuI2ycf8axy3+d5vjo+X7fL+jm+Gzc9XTp+5121NgRzLA9nPgnWMCGg/C3A9lccDXx/+4v7WU3Xn1uM/zpPd9srjNa/p+M31+GNEWVrB3p/K4+W5VMw13K+N/OUfqKA+xH337t1yu92aNGmS2rRp4/lv9erVSk9PV5s2bTRt2rRgpgQAAAAAAACLC+oIrM6dO+vDDz+sFH/ooYd05MgRPfvss0pLSwtmSgAAAAAAALC4oDawGjVqpN///veV4rNmzZIkn68BAAAAAADg9BbUWwgBAAAAAACAmgrqCCx/li9fHuoUAAAAAAAAYFGMwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAIClWeIh7ggvq34LdQbl+rQNdQYAAAAAAKCuMQILAAAAAAAAlkYDCwAAAAAAAJZGAwsAAAAAAACWxjOwAADAaWfRplBnUG5Q51BnAAAAYH2MwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAICl0cACAAAAAACApdHAAgAAAAAAgKXRwAIAAAAAAIClOUKdAFDXVv0W6gzK9Wkb6gwAoA79+muoMyjXtuoDboPdFsq1MycHADXDMQySlLbojVCnUK7zmFBngNMAI7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGn8CiEAAKgV/OorAAAA6gojsAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaY5QJwCg3KJNoc6g3KDOoc4AAAAAAIBSjMACAAAAAACApdHAAgAAAAAAgKVxCyEAABbFbcUAAABAKUZgAQAAAAAAwNJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSgtrA+v7773X77berU6dOql+/vlq2bKmrr75a6enpwUwDAAAAAAAAYcQRzIU98cQTWrlypa666ip16dJFe/fu1QsvvKDu3bvru+++U+fO/EY3AAAAAAAAvAW1gXX33Xfr7bffVmRkpCc2evRonX322Xr88cf11ltvBTMdAAAAAAAAhIGgNrDOP//8SrF27dqpU6dO2rx5czBTAQAAAAAAQJgI+UPcTdPUvn371KhRo1CnAgAAAAAAAAsK6ggsX+bOnavdu3dr2rRpfqcpKipSUVGR59+5ubmSJKfTKafTKUmy2Wyy2Wxyu91yu92eacviLpdLpmlWG7fb7TIMwzPfinFJcrlcAcUdDodM0/SKG4Yhu91eKUfDMCTpWB6m13wMwybTdMubIcMwaiVeynuZZZ+Hv5qOn09pjv5yr9uaAllPpe/1XeuJ5X7iNTmdziq3PcmQ6XYeNxv7sdRdAcUNW+l68o4bMmz20ly88vQTN2ySwnd/8hUP92OEpWs6tmyHrXT/cFWYtyHJbrPJbZpyBxC3HcvT7Xar4pZqMwzZDEMut9tr76sUP1ZDlTUdl6Mk2Y8dh4+P13lNxz5Hv+vJXSEfo7SmUB0jnM7qtz3TNOv0/FSTY7nL5apyf7LKOVcyKh0LpMrHiLL5hfKcWxZ3VtjPpMrHiPLtObTnXElyu93VHvfM47Z5X7kH6zqi4jHL1zG77Jom2PuTr7jT6az2/BSK/amqmqo651ZcRjD3J1+5V9wO/O1nUlXfHYJ7jCg79vu7jjDdwb2G9dTkIx7ItVF1+9mx5AOKn+wxouJ3B1/7mSS5DXnPwyzNpiZxSTIDjNvM0uyOj0uq9hrW83FWs55KtxkzgPiJXxtV3Fx9XZeb7trd9k6mJqfz1PmucfxxoqZC2sDasmWL/vjHP6pPnz4aO3as3+lmzpypqVOnVoqvW7dO9evXlyQ1btxYaWlpysjI0IEDBzzTJCcnKzk5Wenp6crJyfHEU1NTlZSUpE2bNqmgoMAT79ChgxISErRu3Tqvld2lSxdFRkZq7dq1Xjn06NFDxcXF2rhxoydmt9vVs2dP5eTkaMuWLZ54TEyMunbtqqysLG3bts0Tj4+PlxShIneOCl3lOUbaYlXPkagC1yEVu/M88Wh7vKLtCcp3ZslpluceY09UlD1Wec69cpklnnh9R5IijBjlluyWWeHrU4OIZrLJoZySnV41uVypVdZUcXq7EaEGEc1V7M5XgeugJ+4wYhQbkVTnNQWynnJK8hUfkSK3nDpSsscTN2RTfGSKnGah8p37g1LT2rXZVW57DXZnKad4Z0DryV9NcZEpKnEX+KypyJXns6ZC1+FKNens3mG7P3Xs2FGZmZnatWuXJx7uxwhL15SfL7vNpp4pKcopLNSW/eXbXkxEhLo2b66s/HxtO1i+7cXHxKhjUpIyc3K0q0KOjWNjlZaYqIxDh3Qgr3x/So6PV3JCgtKzspRTIffUxEQlxcZq0969KigpkbKzq6/JNLV2p/f+1CMlRcVOpzbuKd+fglKTVOV6Kt5fXmtEww4yohJUsn+dzAoXZBGNusiwR6p4n/d6imzSQ6arWCVZ5dueYdgV2bSnzOIclWSXb3uGI0aRjbvKXZAlZ075tmeLildEw45y5WVq7drqt70it6NOz081OZZv2lRQ5f5klXNufESKCgoKqj1G5JTkh/ycW1bT2rWl+5m/Y4TU0BLnXEnKykqo9riXU5Ib0HoKRk0VP0tfx/KckvyQ7E++alq7Nrva81Mo9id/NVV3zs0pyQ94PdV1TWX7mOT/OkI6I+j7k7+acnKSqryOcO/4KqD1VFvXsPUciTrqPOizpnR7SbXXRjkl+UHfnyrWVHE9rV2bXeX1niQdSIhSYZTdE2+YU6wGBU7tTYxWiaP8hquk7ELFFLu1KylGplHefWqWVSCHy9TOJvW8akrZd1ROu6E9jWLKazJNtdxXoMJIm/Y3jPbEI5xutZOqvYYtPnLsM4hpLEdCmlw5GXIVlNdkj02Wo0GynIfT5S4qX0+O+FTZ6yWp5OAmmc7auTZae/TYMv1cl5cUVH9t5MorP+7VZU1rj5463zXKBiOdKMOs2BoLor179+qCCy5QSUmJvvvuOzVv3tzvtL5GYKWkpOjgwYOKi4uTZKGRCMfUtOO5ZkmGZf4a3OfSdlXWtOqLrT5yDM1fg3te3Nor6mt9rFmyzW+twf5rcK9LUqvc9r5b9FvI/9JT5vzBZ4bt/mTp0UqnYk3HToCWGIGVmlp9Tb/+ap0RWO3aVbmelvxsnRFYF3esfttbsyTDMiOwev8urcr96dvPt/qZT/BHjPS5tG21x4jSc1loz7ll8V6XlO9nUuVjxJolGT5rDcUIrPMGta32uFf22ZbNx1fuwbqOKPtsJd/H7LJrGiuMwOp1SWq156dvP08POMe6rum8QWlVnnMrbgehHoFVcTvwt599v3S7ZUZg9bm0XZXXEcd/dwjldXmvS9pUe21U3X7mK/e6qqnidwdf+1nGrLcsMwKr3f8bU+017NJfyl4I/Qisi88qD/u6Ll/6i3VGYF181qnzXSM3N1eJiYnKycnx9HJqIiQjsHJycjRkyBAdPnxYK1asqLJ5JUlRUVGKioqqFHc4HHI4vEso+9COV7ZiA40fP98TiRuG4TPuL8fSWwkrj8U0DN+PKqut+PHLLLul0V9NvubjP/e6rSmQ9eH93prkWPs1VczL37YX6HqqKl5bNYXz/lTTODWdRE0Vlm0YhhyGj23pWKMp4LjN5vMhjXYfdXrFj8vVZ+5+cpTkM17nNVWxnnwdDgybn1O3EXjcMAw/cZt8LdQwbHI4qt/2ys4fdXV+qip+/HGs7HO1+jm3LJfqjhEV5xeqc25Z/Phcj/+34dn+Q3vOlcpvsanquOd7XsE/55buZ5W3g4q5e28HwduffMUr5up/Pwv+/uQvXt059/hlhPIY4StPf8eIYO5P/uJVfXeoaj6hOEYEcm0UyH4WrGNEIPuZzc9wlJrGjRrEDT/x6q5Vj/84/V532Px8T/Ibr/m10fGb6/HHiLK0qro2qlH8JGqqmGu4f9fwl3+ggt7AKiws1PDhw5Wenq4lS5borLPOqv5NAADUklW/hTqDcn3ahjoDAAAAIDwEtYHlcrk0evRorVq1Sh999JH69OkTzMUDqGWLNoU6g3KDOoc6AwAAAABAXQlqA+uee+7RggULNHz4cGVnZ+utt97yev36668PZjoAAAAAAAAIA0FtYK1fv16S9PHHH+vjjz+u9DoNLAAAAAAAABwvqA2s5cuXB3NxAAAAAAAAOAX4+1kFAAAAAAAAwBJoYAEAAAAAAMDSaGABAAAAAADA0mhgAQAAAAAAwNJoYAEAAAAAAMDSgvorhACAU8+q30KdQbk+bUOdAQAAAIC6wAgsAAAAAAAAWBojsACcFhZtCnUG5QZ1DnUGAAAAABBeGIEFAAAAAAAAS2MEFgBYECPGAAAAAKAcI7AAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAAAAABgaTSwAAAAAAAAYGk0sAAAAAAAAGBpNLAAAAA</t>
         </is>
       </c>
     </row>

</xml_diff>